<commit_message>
CIERRE 19 AGO 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #08  AGOSTO 2022/CREDITOS  4 CARNES   ZAVALETA   AGOSTO     2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #08  AGOSTO 2022/CREDITOS  4 CARNES   ZAVALETA   AGOSTO     2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="12" activeTab="13"/>
+    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="13" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="REMISIONES OCTUBRE  2021     " sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="109">
   <si>
     <t>REMISION</t>
   </si>
@@ -544,6 +544,9 @@
   </si>
   <si>
     <t>NLP x prestamo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NORMA LEDO     Central </t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="246">
+  <cellXfs count="248">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1606,10 +1609,6 @@
     <xf numFmtId="165" fontId="10" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="16" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="16" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="10" fillId="17" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1631,13 +1630,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="17" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="16" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="16" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="3" fillId="13" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1740,11 +1749,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
       <color rgb="FF00FF00"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FF66FFFF"/>
       <color rgb="FF990033"/>
-      <color rgb="FF0000FF"/>
       <color rgb="FFFF99CC"/>
       <color rgb="FFCC0099"/>
       <color rgb="FFCC99FF"/>
@@ -3615,24 +3624,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="220" t="s">
+      <c r="B1" s="222" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="221"/>
-      <c r="D1" s="221"/>
-      <c r="E1" s="221"/>
-      <c r="F1" s="222"/>
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="224"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
       <c r="G2" s="5"/>
       <c r="H2" s="2"/>
     </row>
@@ -4778,12 +4787,12 @@
     <row r="55" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B55" s="37"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="216">
+      <c r="D55" s="218">
         <f>D51-F51</f>
         <v>0</v>
       </c>
-      <c r="E55" s="217"/>
-      <c r="F55" s="218"/>
+      <c r="E55" s="219"/>
+      <c r="F55" s="220"/>
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -4797,11 +4806,11 @@
     <row r="57" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B57" s="37"/>
       <c r="C57" s="2"/>
-      <c r="D57" s="219" t="s">
+      <c r="D57" s="221" t="s">
         <v>8</v>
       </c>
-      <c r="E57" s="219"/>
-      <c r="F57" s="219"/>
+      <c r="E57" s="221"/>
+      <c r="F57" s="221"/>
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -4912,8 +4921,8 @@
   </sheetPr>
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4921,7 +4930,7 @@
     <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="52" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="53" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="206" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" style="204" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" style="54" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="55" customWidth="1"/>
     <col min="7" max="7" width="18" style="56" customWidth="1"/>
@@ -4930,25 +4939,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="223" t="s">
+      <c r="B1" s="225" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="225"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -5312,7 +5321,7 @@
         <v>387</v>
       </c>
       <c r="C17" s="25"/>
-      <c r="D17" s="199" t="s">
+      <c r="D17" s="197" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="20">
@@ -5366,10 +5375,10 @@
       <c r="E19" s="20">
         <v>8500</v>
       </c>
-      <c r="F19" s="197">
+      <c r="F19" s="195">
         <v>44767</v>
       </c>
-      <c r="G19" s="198">
+      <c r="G19" s="196">
         <v>8500</v>
       </c>
       <c r="H19" s="18">
@@ -5439,10 +5448,10 @@
       <c r="E22" s="20">
         <v>12311</v>
       </c>
-      <c r="F22" s="197">
+      <c r="F22" s="195">
         <v>44767</v>
       </c>
-      <c r="G22" s="198">
+      <c r="G22" s="196">
         <v>12311</v>
       </c>
       <c r="H22" s="18">
@@ -5685,10 +5694,10 @@
       <c r="E32" s="20">
         <v>16229</v>
       </c>
-      <c r="F32" s="197">
+      <c r="F32" s="195">
         <v>44767</v>
       </c>
-      <c r="G32" s="198">
+      <c r="G32" s="196">
         <v>16229</v>
       </c>
       <c r="H32" s="18">
@@ -5710,10 +5719,10 @@
       <c r="E33" s="20">
         <v>10085</v>
       </c>
-      <c r="F33" s="197">
+      <c r="F33" s="195">
         <v>44767</v>
       </c>
-      <c r="G33" s="198">
+      <c r="G33" s="196">
         <v>10085</v>
       </c>
       <c r="H33" s="18">
@@ -5735,10 +5744,10 @@
       <c r="E34" s="20">
         <v>19131</v>
       </c>
-      <c r="F34" s="197">
+      <c r="F34" s="195">
         <v>44767</v>
       </c>
-      <c r="G34" s="198">
+      <c r="G34" s="196">
         <v>19131</v>
       </c>
       <c r="H34" s="18">
@@ -5754,17 +5763,21 @@
         <v>405</v>
       </c>
       <c r="C35" s="24"/>
-      <c r="D35" s="212" t="s">
+      <c r="D35" s="208" t="s">
         <v>20</v>
       </c>
       <c r="E35" s="182">
         <v>74746</v>
       </c>
-      <c r="F35" s="195"/>
-      <c r="G35" s="196"/>
+      <c r="F35" s="189">
+        <v>44777</v>
+      </c>
+      <c r="G35" s="212">
+        <v>74746</v>
+      </c>
       <c r="H35" s="18">
         <f t="shared" si="1"/>
-        <v>74746</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5959,7 +5972,7 @@
       <c r="A44" s="23"/>
       <c r="B44" s="13"/>
       <c r="C44" s="24"/>
-      <c r="D44" s="207"/>
+      <c r="D44" s="205"/>
       <c r="E44" s="60"/>
       <c r="F44" s="61"/>
       <c r="G44" s="62"/>
@@ -5972,7 +5985,7 @@
       <c r="A45" s="31"/>
       <c r="B45" s="100"/>
       <c r="C45" s="32"/>
-      <c r="D45" s="200"/>
+      <c r="D45" s="198"/>
       <c r="E45" s="34">
         <v>0</v>
       </c>
@@ -5987,7 +6000,7 @@
     <row r="46" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B46" s="37"/>
       <c r="C46" s="38"/>
-      <c r="D46" s="201"/>
+      <c r="D46" s="199"/>
       <c r="E46" s="39">
         <f>SUM(E4:E45)</f>
         <v>624329</v>
@@ -5995,18 +6008,18 @@
       <c r="F46" s="39"/>
       <c r="G46" s="39">
         <f>SUM(G4:G45)</f>
-        <v>549583</v>
+        <v>624329</v>
       </c>
       <c r="H46" s="40">
         <f>SUM(H4:H45)</f>
-        <v>74746</v>
+        <v>0</v>
       </c>
       <c r="I46" s="2"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" s="37"/>
       <c r="C47" s="38"/>
-      <c r="D47" s="201"/>
+      <c r="D47" s="199"/>
       <c r="E47" s="41"/>
       <c r="F47" s="42"/>
       <c r="G47" s="43"/>
@@ -6016,7 +6029,7 @@
     <row r="48" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B48" s="37"/>
       <c r="C48" s="38"/>
-      <c r="D48" s="201"/>
+      <c r="D48" s="199"/>
       <c r="E48" s="45" t="s">
         <v>6</v>
       </c>
@@ -6030,7 +6043,7 @@
     <row r="49" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="37"/>
       <c r="C49" s="38"/>
-      <c r="D49" s="201"/>
+      <c r="D49" s="199"/>
       <c r="E49" s="45"/>
       <c r="F49" s="42"/>
       <c r="G49" s="46"/>
@@ -6040,19 +6053,19 @@
     <row r="50" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B50" s="37"/>
       <c r="C50" s="38"/>
-      <c r="D50" s="201"/>
-      <c r="E50" s="216">
+      <c r="D50" s="199"/>
+      <c r="E50" s="218">
         <f>E46-G46</f>
-        <v>74746</v>
-      </c>
-      <c r="F50" s="217"/>
-      <c r="G50" s="218"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="219"/>
+      <c r="G50" s="220"/>
       <c r="I50" s="2"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B51" s="37"/>
       <c r="C51" s="38"/>
-      <c r="D51" s="201"/>
+      <c r="D51" s="199"/>
       <c r="E51" s="41"/>
       <c r="F51" s="42"/>
       <c r="G51" s="43"/>
@@ -6061,19 +6074,19 @@
     <row r="52" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B52" s="37"/>
       <c r="C52" s="38"/>
-      <c r="D52" s="201"/>
-      <c r="E52" s="219" t="s">
+      <c r="D52" s="199"/>
+      <c r="E52" s="221" t="s">
         <v>8</v>
       </c>
-      <c r="F52" s="219"/>
-      <c r="G52" s="219"/>
+      <c r="F52" s="221"/>
+      <c r="G52" s="221"/>
       <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="111"/>
       <c r="B53" s="112"/>
       <c r="C53" s="113"/>
-      <c r="D53" s="202"/>
+      <c r="D53" s="200"/>
       <c r="E53" s="115"/>
       <c r="F53" s="116"/>
       <c r="G53" s="117"/>
@@ -6083,7 +6096,7 @@
       <c r="A54" s="101"/>
       <c r="B54" s="102"/>
       <c r="C54" s="103"/>
-      <c r="D54" s="203"/>
+      <c r="D54" s="201"/>
       <c r="E54" s="50"/>
       <c r="F54" s="51"/>
       <c r="G54" s="50"/>
@@ -6094,7 +6107,7 @@
       <c r="A55" s="118"/>
       <c r="B55" s="119"/>
       <c r="C55" s="120"/>
-      <c r="D55" s="204"/>
+      <c r="D55" s="202"/>
       <c r="E55" s="122"/>
       <c r="F55" s="123"/>
       <c r="G55" s="124"/>
@@ -6105,7 +6118,7 @@
       <c r="A56" s="118"/>
       <c r="B56" s="119"/>
       <c r="C56" s="120"/>
-      <c r="D56" s="204"/>
+      <c r="D56" s="202"/>
       <c r="E56" s="122"/>
       <c r="F56" s="123"/>
       <c r="G56" s="124"/>
@@ -6116,7 +6129,7 @@
       <c r="A57" s="118"/>
       <c r="B57" s="119"/>
       <c r="C57" s="120"/>
-      <c r="D57" s="204"/>
+      <c r="D57" s="202"/>
       <c r="E57" s="122"/>
       <c r="F57" s="123"/>
       <c r="G57" s="124"/>
@@ -6127,7 +6140,7 @@
       <c r="A58" s="118"/>
       <c r="B58" s="119"/>
       <c r="C58" s="120"/>
-      <c r="D58" s="204"/>
+      <c r="D58" s="202"/>
       <c r="E58" s="122"/>
       <c r="F58" s="123"/>
       <c r="G58" s="124"/>
@@ -6138,7 +6151,7 @@
       <c r="A59" s="118"/>
       <c r="B59" s="119"/>
       <c r="C59" s="120"/>
-      <c r="D59" s="204"/>
+      <c r="D59" s="202"/>
       <c r="E59" s="122"/>
       <c r="F59" s="123"/>
       <c r="G59" s="124"/>
@@ -6149,7 +6162,7 @@
       <c r="A60" s="118"/>
       <c r="B60" s="119"/>
       <c r="C60" s="120"/>
-      <c r="D60" s="204"/>
+      <c r="D60" s="202"/>
       <c r="E60" s="122"/>
       <c r="F60" s="123"/>
       <c r="G60" s="124"/>
@@ -6160,7 +6173,7 @@
       <c r="A61" s="118"/>
       <c r="B61" s="119"/>
       <c r="C61" s="120"/>
-      <c r="D61" s="204"/>
+      <c r="D61" s="202"/>
       <c r="E61" s="122"/>
       <c r="F61" s="123"/>
       <c r="G61" s="124"/>
@@ -6171,7 +6184,7 @@
       <c r="A62" s="118"/>
       <c r="B62" s="119"/>
       <c r="C62" s="120"/>
-      <c r="D62" s="204"/>
+      <c r="D62" s="202"/>
       <c r="E62" s="122"/>
       <c r="F62" s="123"/>
       <c r="G62" s="124"/>
@@ -6182,7 +6195,7 @@
       <c r="A63" s="118"/>
       <c r="B63" s="119"/>
       <c r="C63" s="120"/>
-      <c r="D63" s="204"/>
+      <c r="D63" s="202"/>
       <c r="E63" s="122"/>
       <c r="F63" s="123"/>
       <c r="G63" s="124"/>
@@ -6193,7 +6206,7 @@
       <c r="A64" s="118"/>
       <c r="B64" s="119"/>
       <c r="C64" s="120"/>
-      <c r="D64" s="204"/>
+      <c r="D64" s="202"/>
       <c r="E64" s="122"/>
       <c r="F64" s="123"/>
       <c r="G64" s="124"/>
@@ -6203,7 +6216,7 @@
       <c r="A65" s="105"/>
       <c r="B65" s="106"/>
       <c r="C65" s="107"/>
-      <c r="D65" s="205"/>
+      <c r="D65" s="203"/>
       <c r="E65" s="108"/>
       <c r="F65" s="109"/>
       <c r="G65" s="110"/>
@@ -6264,18 +6277,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="Q1" s="226"/>
-      <c r="R1" s="227"/>
-      <c r="S1" s="227"/>
-      <c r="T1" s="227"/>
-      <c r="U1" s="227"/>
-      <c r="V1" s="227"/>
-      <c r="W1" s="227"/>
-      <c r="X1" s="227"/>
-      <c r="Y1" s="227"/>
-      <c r="Z1" s="227"/>
-      <c r="AA1" s="227"/>
-      <c r="AB1" s="227"/>
+      <c r="Q1" s="228"/>
+      <c r="R1" s="229"/>
+      <c r="S1" s="229"/>
+      <c r="T1" s="229"/>
+      <c r="U1" s="229"/>
+      <c r="V1" s="229"/>
+      <c r="W1" s="229"/>
+      <c r="X1" s="229"/>
+      <c r="Y1" s="229"/>
+      <c r="Z1" s="229"/>
+      <c r="AA1" s="229"/>
+      <c r="AB1" s="229"/>
     </row>
     <row r="2" spans="2:35" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="156" t="s">
@@ -6827,7 +6840,7 @@
       <c r="R16" s="128"/>
       <c r="S16" s="134"/>
       <c r="T16" s="20"/>
-      <c r="U16" s="214">
+      <c r="U16" s="210">
         <f t="shared" si="1"/>
         <v>540817</v>
       </c>
@@ -6929,10 +6942,10 @@
         <v>101</v>
       </c>
       <c r="R19" s="128"/>
-      <c r="S19" s="232" t="s">
+      <c r="S19" s="234" t="s">
         <v>95</v>
       </c>
-      <c r="T19" s="233"/>
+      <c r="T19" s="235"/>
       <c r="U19" s="77">
         <f t="shared" si="1"/>
         <v>11454.260000000009</v>
@@ -7311,20 +7324,20 @@
       </c>
     </row>
     <row r="36" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="234" t="s">
+      <c r="B36" s="236" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="235"/>
-      <c r="D36" s="236"/>
+      <c r="C36" s="237"/>
+      <c r="D36" s="238"/>
       <c r="E36" s="184">
         <f t="shared" si="0"/>
         <v>0.31000000005587935</v>
       </c>
     </row>
     <row r="37" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="237"/>
-      <c r="C37" s="238"/>
-      <c r="D37" s="239"/>
+      <c r="B37" s="239"/>
+      <c r="C37" s="240"/>
+      <c r="D37" s="241"/>
     </row>
     <row r="38" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7588,8 +7601,8 @@
       <c r="AB63" s="121"/>
     </row>
     <row r="64" spans="17:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AA64" s="230"/>
-      <c r="AB64" s="231"/>
+      <c r="AA64" s="232"/>
+      <c r="AB64" s="233"/>
     </row>
     <row r="69" spans="27:27" x14ac:dyDescent="0.3">
       <c r="AA69" s="54"/>
@@ -7614,8 +7627,8 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A10" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7623,7 +7636,7 @@
     <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="52" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="53" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="206" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" style="204" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" style="54" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="55" customWidth="1"/>
     <col min="7" max="7" width="18" style="56" customWidth="1"/>
@@ -7632,25 +7645,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="223" t="s">
+      <c r="B1" s="225" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="225"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -7820,8 +7833,8 @@
       <c r="E9" s="20">
         <v>73994</v>
       </c>
-      <c r="F9" s="210"/>
-      <c r="G9" s="211"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="86"/>
       <c r="H9" s="18">
         <f t="shared" si="0"/>
         <v>73994</v>
@@ -8012,10 +8025,10 @@
       <c r="E17" s="20">
         <v>409</v>
       </c>
-      <c r="F17" s="208">
+      <c r="F17" s="206">
         <v>44767</v>
       </c>
-      <c r="G17" s="209">
+      <c r="G17" s="207">
         <v>409</v>
       </c>
       <c r="H17" s="18">
@@ -8435,8 +8448,8 @@
       <c r="E34" s="20">
         <v>26596</v>
       </c>
-      <c r="F34" s="125"/>
-      <c r="G34" s="22"/>
+      <c r="F34" s="211"/>
+      <c r="G34" s="86"/>
       <c r="H34" s="18">
         <v>0</v>
       </c>
@@ -8476,8 +8489,8 @@
       <c r="E36" s="20">
         <v>2640</v>
       </c>
-      <c r="F36" s="21"/>
-      <c r="G36" s="22"/>
+      <c r="F36" s="85"/>
+      <c r="G36" s="86"/>
       <c r="H36" s="18">
         <f t="shared" si="0"/>
         <v>2640</v>
@@ -8497,10 +8510,10 @@
       <c r="E37" s="20">
         <v>1414</v>
       </c>
-      <c r="F37" s="208">
+      <c r="F37" s="206">
         <v>44767</v>
       </c>
-      <c r="G37" s="209">
+      <c r="G37" s="207">
         <v>1414</v>
       </c>
       <c r="H37" s="18">
@@ -8547,8 +8560,8 @@
       <c r="E39" s="20">
         <v>3100</v>
       </c>
-      <c r="F39" s="21"/>
-      <c r="G39" s="22"/>
+      <c r="F39" s="85"/>
+      <c r="G39" s="86"/>
       <c r="H39" s="18">
         <f t="shared" si="0"/>
         <v>3100</v>
@@ -8568,8 +8581,8 @@
       <c r="E40" s="20">
         <v>728</v>
       </c>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
+      <c r="F40" s="85"/>
+      <c r="G40" s="86"/>
       <c r="H40" s="18">
         <f t="shared" si="0"/>
         <v>728</v>
@@ -8589,8 +8602,8 @@
       <c r="E41" s="20">
         <v>0</v>
       </c>
-      <c r="F41" s="21"/>
-      <c r="G41" s="22"/>
+      <c r="F41" s="85"/>
+      <c r="G41" s="86"/>
       <c r="H41" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8610,8 +8623,8 @@
       <c r="E42" s="20">
         <v>7875</v>
       </c>
-      <c r="F42" s="21"/>
-      <c r="G42" s="22"/>
+      <c r="F42" s="85"/>
+      <c r="G42" s="86"/>
       <c r="H42" s="18">
         <f t="shared" si="0"/>
         <v>7875</v>
@@ -8631,8 +8644,8 @@
       <c r="E43" s="20">
         <v>11843</v>
       </c>
-      <c r="F43" s="21"/>
-      <c r="G43" s="22"/>
+      <c r="F43" s="85"/>
+      <c r="G43" s="86"/>
       <c r="H43" s="18">
         <f t="shared" si="0"/>
         <v>11843</v>
@@ -8652,11 +8665,15 @@
       <c r="E44" s="20">
         <v>1646</v>
       </c>
-      <c r="F44" s="21"/>
-      <c r="G44" s="22"/>
+      <c r="F44" s="85">
+        <v>44776</v>
+      </c>
+      <c r="G44" s="86">
+        <v>1646</v>
+      </c>
       <c r="H44" s="18">
         <f t="shared" si="0"/>
-        <v>1646</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8673,8 +8690,8 @@
       <c r="E45" s="20">
         <v>2446</v>
       </c>
-      <c r="F45" s="21"/>
-      <c r="G45" s="22"/>
+      <c r="F45" s="85"/>
+      <c r="G45" s="86"/>
       <c r="H45" s="18">
         <f t="shared" si="0"/>
         <v>2446</v>
@@ -8694,8 +8711,8 @@
       <c r="E46" s="20">
         <v>18102</v>
       </c>
-      <c r="F46" s="21"/>
-      <c r="G46" s="22"/>
+      <c r="F46" s="85"/>
+      <c r="G46" s="86"/>
       <c r="H46" s="18">
         <f t="shared" si="0"/>
         <v>18102</v>
@@ -8731,7 +8748,7 @@
       <c r="A49" s="23"/>
       <c r="B49" s="13"/>
       <c r="C49" s="24"/>
-      <c r="D49" s="207"/>
+      <c r="D49" s="205"/>
       <c r="E49" s="60"/>
       <c r="F49" s="61"/>
       <c r="G49" s="62"/>
@@ -8744,7 +8761,7 @@
       <c r="A50" s="31"/>
       <c r="B50" s="100"/>
       <c r="C50" s="32"/>
-      <c r="D50" s="200"/>
+      <c r="D50" s="198"/>
       <c r="E50" s="34">
         <v>0</v>
       </c>
@@ -8759,7 +8776,7 @@
     <row r="51" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B51" s="37"/>
       <c r="C51" s="38"/>
-      <c r="D51" s="201"/>
+      <c r="D51" s="199"/>
       <c r="E51" s="39">
         <f>SUM(E4:E50)</f>
         <v>923458</v>
@@ -8767,18 +8784,18 @@
       <c r="F51" s="39"/>
       <c r="G51" s="39">
         <f>SUM(G4:G50)</f>
-        <v>774488</v>
+        <v>776134</v>
       </c>
       <c r="H51" s="40">
         <f>SUM(H4:H50)</f>
-        <v>122374</v>
+        <v>120728</v>
       </c>
       <c r="I51" s="2"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B52" s="37"/>
       <c r="C52" s="38"/>
-      <c r="D52" s="201"/>
+      <c r="D52" s="199"/>
       <c r="E52" s="41"/>
       <c r="F52" s="42"/>
       <c r="G52" s="43"/>
@@ -8788,7 +8805,7 @@
     <row r="53" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B53" s="37"/>
       <c r="C53" s="38"/>
-      <c r="D53" s="201"/>
+      <c r="D53" s="199"/>
       <c r="E53" s="45" t="s">
         <v>6</v>
       </c>
@@ -8802,7 +8819,7 @@
     <row r="54" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="37"/>
       <c r="C54" s="38"/>
-      <c r="D54" s="201"/>
+      <c r="D54" s="199"/>
       <c r="E54" s="45"/>
       <c r="F54" s="42"/>
       <c r="G54" s="46"/>
@@ -8812,19 +8829,19 @@
     <row r="55" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B55" s="37"/>
       <c r="C55" s="38"/>
-      <c r="D55" s="201"/>
-      <c r="E55" s="216">
+      <c r="D55" s="199"/>
+      <c r="E55" s="218">
         <f>E51-G51</f>
-        <v>148970</v>
-      </c>
-      <c r="F55" s="217"/>
-      <c r="G55" s="218"/>
+        <v>147324</v>
+      </c>
+      <c r="F55" s="219"/>
+      <c r="G55" s="220"/>
       <c r="I55" s="2"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B56" s="37"/>
       <c r="C56" s="38"/>
-      <c r="D56" s="201"/>
+      <c r="D56" s="199"/>
       <c r="E56" s="41"/>
       <c r="F56" s="42"/>
       <c r="G56" s="43"/>
@@ -8833,19 +8850,19 @@
     <row r="57" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B57" s="37"/>
       <c r="C57" s="38"/>
-      <c r="D57" s="201"/>
-      <c r="E57" s="219" t="s">
+      <c r="D57" s="199"/>
+      <c r="E57" s="221" t="s">
         <v>8</v>
       </c>
-      <c r="F57" s="219"/>
-      <c r="G57" s="219"/>
+      <c r="F57" s="221"/>
+      <c r="G57" s="221"/>
       <c r="I57" s="2"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="111"/>
       <c r="B58" s="112"/>
       <c r="C58" s="113"/>
-      <c r="D58" s="202"/>
+      <c r="D58" s="200"/>
       <c r="E58" s="115"/>
       <c r="F58" s="116"/>
       <c r="G58" s="117"/>
@@ -8855,7 +8872,7 @@
       <c r="A59" s="101"/>
       <c r="B59" s="102"/>
       <c r="C59" s="103"/>
-      <c r="D59" s="203"/>
+      <c r="D59" s="201"/>
       <c r="E59" s="50"/>
       <c r="F59" s="51"/>
       <c r="G59" s="50"/>
@@ -8866,7 +8883,7 @@
       <c r="A60" s="118"/>
       <c r="B60" s="119"/>
       <c r="C60" s="120"/>
-      <c r="D60" s="204"/>
+      <c r="D60" s="202"/>
       <c r="E60" s="122"/>
       <c r="F60" s="123"/>
       <c r="G60" s="124"/>
@@ -8877,7 +8894,7 @@
       <c r="A61" s="118"/>
       <c r="B61" s="119"/>
       <c r="C61" s="120"/>
-      <c r="D61" s="204"/>
+      <c r="D61" s="202"/>
       <c r="E61" s="122"/>
       <c r="F61" s="123"/>
       <c r="G61" s="124"/>
@@ -8888,7 +8905,7 @@
       <c r="A62" s="118"/>
       <c r="B62" s="119"/>
       <c r="C62" s="120"/>
-      <c r="D62" s="204"/>
+      <c r="D62" s="202"/>
       <c r="E62" s="122"/>
       <c r="F62" s="123"/>
       <c r="G62" s="124"/>
@@ -8899,7 +8916,7 @@
       <c r="A63" s="118"/>
       <c r="B63" s="119"/>
       <c r="C63" s="120"/>
-      <c r="D63" s="204"/>
+      <c r="D63" s="202"/>
       <c r="E63" s="122"/>
       <c r="F63" s="123"/>
       <c r="G63" s="124"/>
@@ -8910,7 +8927,7 @@
       <c r="A64" s="118"/>
       <c r="B64" s="119"/>
       <c r="C64" s="120"/>
-      <c r="D64" s="204"/>
+      <c r="D64" s="202"/>
       <c r="E64" s="122"/>
       <c r="F64" s="123"/>
       <c r="G64" s="124"/>
@@ -8921,7 +8938,7 @@
       <c r="A65" s="118"/>
       <c r="B65" s="119"/>
       <c r="C65" s="120"/>
-      <c r="D65" s="204"/>
+      <c r="D65" s="202"/>
       <c r="E65" s="122"/>
       <c r="F65" s="123"/>
       <c r="G65" s="124"/>
@@ -8932,7 +8949,7 @@
       <c r="A66" s="118"/>
       <c r="B66" s="119"/>
       <c r="C66" s="120"/>
-      <c r="D66" s="204"/>
+      <c r="D66" s="202"/>
       <c r="E66" s="122"/>
       <c r="F66" s="123"/>
       <c r="G66" s="124"/>
@@ -8943,7 +8960,7 @@
       <c r="A67" s="118"/>
       <c r="B67" s="119"/>
       <c r="C67" s="120"/>
-      <c r="D67" s="204"/>
+      <c r="D67" s="202"/>
       <c r="E67" s="122"/>
       <c r="F67" s="123"/>
       <c r="G67" s="124"/>
@@ -8954,7 +8971,7 @@
       <c r="A68" s="118"/>
       <c r="B68" s="119"/>
       <c r="C68" s="120"/>
-      <c r="D68" s="204"/>
+      <c r="D68" s="202"/>
       <c r="E68" s="122"/>
       <c r="F68" s="123"/>
       <c r="G68" s="124"/>
@@ -8965,7 +8982,7 @@
       <c r="A69" s="118"/>
       <c r="B69" s="119"/>
       <c r="C69" s="120"/>
-      <c r="D69" s="204"/>
+      <c r="D69" s="202"/>
       <c r="E69" s="122"/>
       <c r="F69" s="123"/>
       <c r="G69" s="124"/>
@@ -8975,7 +8992,7 @@
       <c r="A70" s="105"/>
       <c r="B70" s="106"/>
       <c r="C70" s="107"/>
-      <c r="D70" s="205"/>
+      <c r="D70" s="203"/>
       <c r="E70" s="108"/>
       <c r="F70" s="109"/>
       <c r="G70" s="110"/>
@@ -9004,7 +9021,7 @@
   </sheetPr>
   <dimension ref="B1:AJ69"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
@@ -9015,7 +9032,7 @@
     <col min="3" max="3" width="11.42578125" style="114"/>
     <col min="4" max="4" width="15" style="114" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" style="114" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="213"/>
+    <col min="6" max="6" width="11.42578125" style="209"/>
     <col min="7" max="12" width="11.42578125" style="114"/>
     <col min="13" max="14" width="39.140625" style="114" customWidth="1"/>
     <col min="15" max="15" width="31.5703125" style="114" customWidth="1"/>
@@ -9037,18 +9054,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="R1" s="226"/>
-      <c r="S1" s="227"/>
-      <c r="T1" s="227"/>
-      <c r="U1" s="227"/>
-      <c r="V1" s="227"/>
-      <c r="W1" s="227"/>
-      <c r="X1" s="227"/>
-      <c r="Y1" s="227"/>
-      <c r="Z1" s="227"/>
-      <c r="AA1" s="227"/>
-      <c r="AB1" s="227"/>
-      <c r="AC1" s="227"/>
+      <c r="R1" s="228"/>
+      <c r="S1" s="229"/>
+      <c r="T1" s="229"/>
+      <c r="U1" s="229"/>
+      <c r="V1" s="229"/>
+      <c r="W1" s="229"/>
+      <c r="X1" s="229"/>
+      <c r="Y1" s="229"/>
+      <c r="Z1" s="229"/>
+      <c r="AA1" s="229"/>
+      <c r="AB1" s="229"/>
+      <c r="AC1" s="229"/>
     </row>
     <row r="2" spans="2:36" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="156" t="s">
@@ -9171,7 +9188,7 @@
         <f>E4+D5</f>
         <v>121232</v>
       </c>
-      <c r="F5" s="213" t="s">
+      <c r="F5" s="209" t="s">
         <v>105</v>
       </c>
       <c r="S5" s="128">
@@ -9213,7 +9230,7 @@
         <f t="shared" ref="E6:E12" si="0">E5+D6</f>
         <v>193535.5</v>
       </c>
-      <c r="F6" s="213" t="s">
+      <c r="F6" s="209" t="s">
         <v>107</v>
       </c>
       <c r="S6" s="128">
@@ -9255,7 +9272,7 @@
         <f t="shared" si="0"/>
         <v>229640.5</v>
       </c>
-      <c r="F7" s="213" t="s">
+      <c r="F7" s="209" t="s">
         <v>107</v>
       </c>
       <c r="S7" s="128">
@@ -9297,7 +9314,7 @@
         <f t="shared" si="0"/>
         <v>233150.5</v>
       </c>
-      <c r="F8" s="213" t="s">
+      <c r="F8" s="209" t="s">
         <v>107</v>
       </c>
       <c r="S8" s="128">
@@ -9339,7 +9356,7 @@
         <f t="shared" si="0"/>
         <v>250706.5</v>
       </c>
-      <c r="F9" s="213" t="s">
+      <c r="F9" s="209" t="s">
         <v>46</v>
       </c>
       <c r="S9" s="128">
@@ -9381,7 +9398,7 @@
         <f t="shared" si="0"/>
         <v>292346.5</v>
       </c>
-      <c r="F10" s="213" t="s">
+      <c r="F10" s="209" t="s">
         <v>46</v>
       </c>
       <c r="S10" s="128">
@@ -9691,10 +9708,10 @@
       </c>
       <c r="F19" s="186"/>
       <c r="S19" s="128"/>
-      <c r="T19" s="232" t="s">
+      <c r="T19" s="234" t="s">
         <v>95</v>
       </c>
-      <c r="U19" s="233"/>
+      <c r="U19" s="235"/>
       <c r="V19" s="77">
         <f t="shared" si="1"/>
         <v>11454.260000000009</v>
@@ -9992,20 +10009,20 @@
       </c>
     </row>
     <row r="36" spans="2:29" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="240" t="s">
+      <c r="B36" s="242" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="241"/>
-      <c r="D36" s="242"/>
+      <c r="C36" s="243"/>
+      <c r="D36" s="244"/>
       <c r="E36" s="184">
         <f t="shared" si="2"/>
         <v>-1314888.83</v>
       </c>
     </row>
     <row r="37" spans="2:29" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="243"/>
-      <c r="C37" s="244"/>
-      <c r="D37" s="245"/>
+      <c r="B37" s="245"/>
+      <c r="C37" s="246"/>
+      <c r="D37" s="247"/>
     </row>
     <row r="38" spans="2:29" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="2:29" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10269,8 +10286,8 @@
       <c r="AC63" s="121"/>
     </row>
     <row r="64" spans="18:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AB64" s="230"/>
-      <c r="AC64" s="231"/>
+      <c r="AB64" s="232"/>
+      <c r="AC64" s="233"/>
     </row>
     <row r="69" spans="28:28" x14ac:dyDescent="0.3">
       <c r="AB69" s="54"/>
@@ -10296,7 +10313,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10304,7 +10321,7 @@
     <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="52" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="53" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="206" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" style="204" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" style="54" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="55" customWidth="1"/>
     <col min="7" max="7" width="18" style="56" customWidth="1"/>
@@ -10313,25 +10330,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="223" t="s">
+      <c r="B1" s="225" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="225"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -10362,124 +10379,176 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="12">
+        <v>44775</v>
+      </c>
       <c r="B4" s="13">
         <v>456</v>
       </c>
       <c r="C4" s="14"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="15"/>
+      <c r="D4" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="15">
+        <v>18423</v>
+      </c>
       <c r="F4" s="16"/>
       <c r="G4" s="17"/>
       <c r="H4" s="18">
         <f t="shared" ref="H4:H50" si="0">E4-G4</f>
-        <v>0</v>
+        <v>18423</v>
       </c>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+      <c r="A5" s="12">
+        <v>44776</v>
+      </c>
       <c r="B5" s="13">
         <v>457</v>
       </c>
       <c r="C5" s="14"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="D5" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="20">
+        <v>1485</v>
+      </c>
+      <c r="F5" s="21">
+        <v>44783</v>
+      </c>
+      <c r="G5" s="22">
+        <v>1485</v>
+      </c>
       <c r="H5" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="12">
+        <v>44777</v>
+      </c>
       <c r="B6" s="13">
         <v>458</v>
       </c>
       <c r="C6" s="14"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="20"/>
+      <c r="D6" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="20">
+        <v>44375</v>
+      </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
       <c r="H6" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>44375</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="23">
+        <v>44778</v>
+      </c>
       <c r="B7" s="13">
         <v>459</v>
       </c>
       <c r="C7" s="14"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="20">
+        <v>15089</v>
+      </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
       <c r="H7" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15089</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="81"/>
+      <c r="A8" s="81">
+        <v>44779</v>
+      </c>
       <c r="B8" s="13">
         <v>460</v>
       </c>
       <c r="C8" s="82"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="20"/>
+      <c r="D8" s="74" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="20">
+        <v>12716</v>
+      </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
       <c r="H8" s="75">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12716</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13">
+      <c r="A9" s="213">
+        <v>44781</v>
+      </c>
+      <c r="B9" s="214">
         <v>461</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="20"/>
+      <c r="C9" s="215"/>
+      <c r="D9" s="216" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="67">
+        <v>16538</v>
+      </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
       <c r="H9" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16538</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="12">
+        <v>44783</v>
+      </c>
       <c r="B10" s="13">
         <v>462</v>
       </c>
       <c r="C10" s="14"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="20"/>
+      <c r="D10" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="20">
+        <v>30178</v>
+      </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
       <c r="H10" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30178</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="12">
+        <v>44783</v>
+      </c>
       <c r="B11" s="13">
         <v>463</v>
       </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="20"/>
+      <c r="D11" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="20">
+        <v>1307</v>
+      </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
       <c r="H11" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -11038,7 +11107,7 @@
       <c r="A49" s="23"/>
       <c r="B49" s="13"/>
       <c r="C49" s="24"/>
-      <c r="D49" s="207"/>
+      <c r="D49" s="205"/>
       <c r="E49" s="60"/>
       <c r="F49" s="61"/>
       <c r="G49" s="62"/>
@@ -11051,7 +11120,7 @@
       <c r="A50" s="31"/>
       <c r="B50" s="100"/>
       <c r="C50" s="32"/>
-      <c r="D50" s="200"/>
+      <c r="D50" s="198"/>
       <c r="E50" s="34">
         <v>0</v>
       </c>
@@ -11066,26 +11135,26 @@
     <row r="51" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B51" s="37"/>
       <c r="C51" s="38"/>
-      <c r="D51" s="201"/>
+      <c r="D51" s="199"/>
       <c r="E51" s="39">
         <f>SUM(E4:E50)</f>
-        <v>0</v>
+        <v>140111</v>
       </c>
       <c r="F51" s="39"/>
       <c r="G51" s="39">
         <f>SUM(G4:G50)</f>
-        <v>0</v>
+        <v>1485</v>
       </c>
       <c r="H51" s="40">
         <f>SUM(H4:H50)</f>
-        <v>0</v>
+        <v>138626</v>
       </c>
       <c r="I51" s="2"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B52" s="37"/>
       <c r="C52" s="38"/>
-      <c r="D52" s="201"/>
+      <c r="D52" s="199"/>
       <c r="E52" s="41"/>
       <c r="F52" s="42"/>
       <c r="G52" s="43"/>
@@ -11095,7 +11164,7 @@
     <row r="53" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B53" s="37"/>
       <c r="C53" s="38"/>
-      <c r="D53" s="201"/>
+      <c r="D53" s="199"/>
       <c r="E53" s="45" t="s">
         <v>6</v>
       </c>
@@ -11109,7 +11178,7 @@
     <row r="54" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="37"/>
       <c r="C54" s="38"/>
-      <c r="D54" s="201"/>
+      <c r="D54" s="199"/>
       <c r="E54" s="45"/>
       <c r="F54" s="42"/>
       <c r="G54" s="46"/>
@@ -11119,19 +11188,19 @@
     <row r="55" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B55" s="37"/>
       <c r="C55" s="38"/>
-      <c r="D55" s="201"/>
-      <c r="E55" s="216">
+      <c r="D55" s="199"/>
+      <c r="E55" s="218">
         <f>E51-G51</f>
-        <v>0</v>
-      </c>
-      <c r="F55" s="217"/>
-      <c r="G55" s="218"/>
+        <v>138626</v>
+      </c>
+      <c r="F55" s="219"/>
+      <c r="G55" s="220"/>
       <c r="I55" s="2"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B56" s="37"/>
       <c r="C56" s="38"/>
-      <c r="D56" s="201"/>
+      <c r="D56" s="199"/>
       <c r="E56" s="41"/>
       <c r="F56" s="42"/>
       <c r="G56" s="43"/>
@@ -11140,19 +11209,19 @@
     <row r="57" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B57" s="37"/>
       <c r="C57" s="38"/>
-      <c r="D57" s="201"/>
-      <c r="E57" s="219" t="s">
+      <c r="D57" s="199"/>
+      <c r="E57" s="221" t="s">
         <v>8</v>
       </c>
-      <c r="F57" s="219"/>
-      <c r="G57" s="219"/>
+      <c r="F57" s="221"/>
+      <c r="G57" s="221"/>
       <c r="I57" s="2"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="111"/>
       <c r="B58" s="112"/>
       <c r="C58" s="113"/>
-      <c r="D58" s="202"/>
+      <c r="D58" s="200"/>
       <c r="E58" s="115"/>
       <c r="F58" s="116"/>
       <c r="G58" s="117"/>
@@ -11162,7 +11231,7 @@
       <c r="A59" s="101"/>
       <c r="B59" s="102"/>
       <c r="C59" s="103"/>
-      <c r="D59" s="203"/>
+      <c r="D59" s="201"/>
       <c r="E59" s="50"/>
       <c r="F59" s="51"/>
       <c r="G59" s="50"/>
@@ -11173,7 +11242,7 @@
       <c r="A60" s="118"/>
       <c r="B60" s="119"/>
       <c r="C60" s="120"/>
-      <c r="D60" s="204"/>
+      <c r="D60" s="202"/>
       <c r="E60" s="122"/>
       <c r="F60" s="123"/>
       <c r="G60" s="124"/>
@@ -11184,7 +11253,7 @@
       <c r="A61" s="118"/>
       <c r="B61" s="119"/>
       <c r="C61" s="120"/>
-      <c r="D61" s="204"/>
+      <c r="D61" s="202"/>
       <c r="E61" s="122"/>
       <c r="F61" s="123"/>
       <c r="G61" s="124"/>
@@ -11195,7 +11264,7 @@
       <c r="A62" s="118"/>
       <c r="B62" s="119"/>
       <c r="C62" s="120"/>
-      <c r="D62" s="204"/>
+      <c r="D62" s="202"/>
       <c r="E62" s="122"/>
       <c r="F62" s="123"/>
       <c r="G62" s="124"/>
@@ -11206,7 +11275,7 @@
       <c r="A63" s="118"/>
       <c r="B63" s="119"/>
       <c r="C63" s="120"/>
-      <c r="D63" s="204"/>
+      <c r="D63" s="202"/>
       <c r="E63" s="122"/>
       <c r="F63" s="123"/>
       <c r="G63" s="124"/>
@@ -11217,7 +11286,7 @@
       <c r="A64" s="118"/>
       <c r="B64" s="119"/>
       <c r="C64" s="120"/>
-      <c r="D64" s="204"/>
+      <c r="D64" s="202"/>
       <c r="E64" s="122"/>
       <c r="F64" s="123"/>
       <c r="G64" s="124"/>
@@ -11228,7 +11297,7 @@
       <c r="A65" s="118"/>
       <c r="B65" s="119"/>
       <c r="C65" s="120"/>
-      <c r="D65" s="204"/>
+      <c r="D65" s="202"/>
       <c r="E65" s="122"/>
       <c r="F65" s="123"/>
       <c r="G65" s="124"/>
@@ -11239,7 +11308,7 @@
       <c r="A66" s="118"/>
       <c r="B66" s="119"/>
       <c r="C66" s="120"/>
-      <c r="D66" s="204"/>
+      <c r="D66" s="202"/>
       <c r="E66" s="122"/>
       <c r="F66" s="123"/>
       <c r="G66" s="124"/>
@@ -11250,7 +11319,7 @@
       <c r="A67" s="118"/>
       <c r="B67" s="119"/>
       <c r="C67" s="120"/>
-      <c r="D67" s="204"/>
+      <c r="D67" s="202"/>
       <c r="E67" s="122"/>
       <c r="F67" s="123"/>
       <c r="G67" s="124"/>
@@ -11261,7 +11330,7 @@
       <c r="A68" s="118"/>
       <c r="B68" s="119"/>
       <c r="C68" s="120"/>
-      <c r="D68" s="204"/>
+      <c r="D68" s="202"/>
       <c r="E68" s="122"/>
       <c r="F68" s="123"/>
       <c r="G68" s="124"/>
@@ -11272,7 +11341,7 @@
       <c r="A69" s="118"/>
       <c r="B69" s="119"/>
       <c r="C69" s="120"/>
-      <c r="D69" s="204"/>
+      <c r="D69" s="202"/>
       <c r="E69" s="122"/>
       <c r="F69" s="123"/>
       <c r="G69" s="124"/>
@@ -11282,7 +11351,7 @@
       <c r="A70" s="105"/>
       <c r="B70" s="106"/>
       <c r="C70" s="107"/>
-      <c r="D70" s="205"/>
+      <c r="D70" s="203"/>
       <c r="E70" s="108"/>
       <c r="F70" s="109"/>
       <c r="G70" s="110"/>
@@ -11350,25 +11419,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="220" t="s">
+      <c r="B1" s="222" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="221"/>
-      <c r="D1" s="221"/>
-      <c r="E1" s="221"/>
-      <c r="F1" s="221"/>
-      <c r="G1" s="222"/>
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="223"/>
+      <c r="G1" s="224"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -13098,12 +13167,12 @@
       <c r="B76" s="37"/>
       <c r="C76" s="38"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="216">
+      <c r="E76" s="218">
         <f>E72-G72</f>
         <v>0</v>
       </c>
-      <c r="F76" s="217"/>
-      <c r="G76" s="218"/>
+      <c r="F76" s="219"/>
+      <c r="G76" s="220"/>
       <c r="I76" s="2"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -13119,11 +13188,11 @@
       <c r="B78" s="37"/>
       <c r="C78" s="38"/>
       <c r="D78" s="2"/>
-      <c r="E78" s="219" t="s">
+      <c r="E78" s="221" t="s">
         <v>8</v>
       </c>
-      <c r="F78" s="219"/>
-      <c r="G78" s="219"/>
+      <c r="F78" s="221"/>
+      <c r="G78" s="221"/>
       <c r="I78" s="2"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -13264,25 +13333,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="220" t="s">
+      <c r="B1" s="222" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="221"/>
-      <c r="D1" s="221"/>
-      <c r="E1" s="221"/>
-      <c r="F1" s="221"/>
-      <c r="G1" s="222"/>
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="223"/>
+      <c r="G1" s="224"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -14131,12 +14200,12 @@
       <c r="B41" s="37"/>
       <c r="C41" s="38"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="216">
+      <c r="E41" s="218">
         <f>E37-G37</f>
         <v>0</v>
       </c>
-      <c r="F41" s="217"/>
-      <c r="G41" s="218"/>
+      <c r="F41" s="219"/>
+      <c r="G41" s="220"/>
       <c r="I41" s="2"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -14152,11 +14221,11 @@
       <c r="B43" s="37"/>
       <c r="C43" s="38"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="219" t="s">
+      <c r="E43" s="221" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="219"/>
-      <c r="G43" s="219"/>
+      <c r="F43" s="221"/>
+      <c r="G43" s="221"/>
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -14300,25 +14369,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="223" t="s">
+      <c r="B1" s="225" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="225"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -15658,12 +15727,12 @@
       <c r="B60" s="37"/>
       <c r="C60" s="38"/>
       <c r="D60" s="2"/>
-      <c r="E60" s="216">
+      <c r="E60" s="218">
         <f>E56-G56</f>
         <v>0</v>
       </c>
-      <c r="F60" s="217"/>
-      <c r="G60" s="218"/>
+      <c r="F60" s="219"/>
+      <c r="G60" s="220"/>
       <c r="I60" s="2"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -15679,11 +15748,11 @@
       <c r="B62" s="37"/>
       <c r="C62" s="38"/>
       <c r="D62" s="2"/>
-      <c r="E62" s="219" t="s">
+      <c r="E62" s="221" t="s">
         <v>8</v>
       </c>
-      <c r="F62" s="219"/>
-      <c r="G62" s="219"/>
+      <c r="F62" s="221"/>
+      <c r="G62" s="221"/>
       <c r="I62" s="2"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -15824,25 +15893,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="223" t="s">
+      <c r="B1" s="225" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="225"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -17243,12 +17312,12 @@
       <c r="B61" s="37"/>
       <c r="C61" s="38"/>
       <c r="D61" s="2"/>
-      <c r="E61" s="216">
+      <c r="E61" s="218">
         <f>E57-G57</f>
         <v>0</v>
       </c>
-      <c r="F61" s="217"/>
-      <c r="G61" s="218"/>
+      <c r="F61" s="219"/>
+      <c r="G61" s="220"/>
       <c r="I61" s="2"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -17264,11 +17333,11 @@
       <c r="B63" s="37"/>
       <c r="C63" s="38"/>
       <c r="D63" s="2"/>
-      <c r="E63" s="219" t="s">
+      <c r="E63" s="221" t="s">
         <v>8</v>
       </c>
-      <c r="F63" s="219"/>
-      <c r="G63" s="219"/>
+      <c r="F63" s="221"/>
+      <c r="G63" s="221"/>
       <c r="I63" s="2"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -17409,25 +17478,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="223" t="s">
+      <c r="B1" s="225" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="225"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -18877,12 +18946,12 @@
       <c r="B64" s="37"/>
       <c r="C64" s="38"/>
       <c r="D64" s="2"/>
-      <c r="E64" s="216">
+      <c r="E64" s="218">
         <f>E60-G60</f>
         <v>0</v>
       </c>
-      <c r="F64" s="217"/>
-      <c r="G64" s="218"/>
+      <c r="F64" s="219"/>
+      <c r="G64" s="220"/>
       <c r="I64" s="2"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -18898,11 +18967,11 @@
       <c r="B66" s="37"/>
       <c r="C66" s="38"/>
       <c r="D66" s="2"/>
-      <c r="E66" s="219" t="s">
+      <c r="E66" s="221" t="s">
         <v>8</v>
       </c>
-      <c r="F66" s="219"/>
-      <c r="G66" s="219"/>
+      <c r="F66" s="221"/>
+      <c r="G66" s="221"/>
       <c r="I66" s="2"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -19034,7 +19103,7 @@
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="13.140625" style="52" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="53" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="206" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" style="204" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" style="54" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="55" customWidth="1"/>
     <col min="7" max="7" width="18" style="56" customWidth="1"/>
@@ -19043,25 +19112,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="223" t="s">
+      <c r="B1" s="225" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="225"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -19200,7 +19269,7 @@
         <v>289</v>
       </c>
       <c r="C8" s="82"/>
-      <c r="D8" s="199" t="s">
+      <c r="D8" s="197" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="20">
@@ -19912,10 +19981,10 @@
       <c r="E37" s="20">
         <v>7615</v>
       </c>
-      <c r="F37" s="197">
+      <c r="F37" s="195">
         <v>44767</v>
       </c>
-      <c r="G37" s="198">
+      <c r="G37" s="196">
         <v>7615</v>
       </c>
       <c r="H37" s="18">
@@ -20087,10 +20156,10 @@
       <c r="E44" s="20">
         <v>2351</v>
       </c>
-      <c r="F44" s="197">
+      <c r="F44" s="195">
         <v>44767</v>
       </c>
-      <c r="G44" s="198">
+      <c r="G44" s="196">
         <v>2351</v>
       </c>
       <c r="H44" s="18">
@@ -20187,10 +20256,10 @@
       <c r="E48" s="20">
         <v>7600</v>
       </c>
-      <c r="F48" s="197">
+      <c r="F48" s="195">
         <v>44767</v>
       </c>
-      <c r="G48" s="198">
+      <c r="G48" s="196">
         <v>7600</v>
       </c>
       <c r="H48" s="18">
@@ -20237,10 +20306,10 @@
       <c r="E50" s="20">
         <v>1954</v>
       </c>
-      <c r="F50" s="197">
+      <c r="F50" s="195">
         <v>44767</v>
       </c>
-      <c r="G50" s="198">
+      <c r="G50" s="196">
         <v>1954</v>
       </c>
       <c r="H50" s="18">
@@ -20354,10 +20423,10 @@
       <c r="E55" s="20">
         <v>12525</v>
       </c>
-      <c r="F55" s="197">
+      <c r="F55" s="195">
         <v>44767</v>
       </c>
-      <c r="G55" s="198">
+      <c r="G55" s="196">
         <v>12525</v>
       </c>
       <c r="H55" s="18">
@@ -20457,7 +20526,7 @@
       <c r="A60" s="31"/>
       <c r="B60" s="100"/>
       <c r="C60" s="32"/>
-      <c r="D60" s="200"/>
+      <c r="D60" s="198"/>
       <c r="E60" s="34">
         <v>0</v>
       </c>
@@ -20472,7 +20541,7 @@
     <row r="61" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B61" s="37"/>
       <c r="C61" s="38"/>
-      <c r="D61" s="201"/>
+      <c r="D61" s="199"/>
       <c r="E61" s="39">
         <f>SUM(E4:E60)</f>
         <v>938122</v>
@@ -20491,7 +20560,7 @@
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B62" s="37"/>
       <c r="C62" s="38"/>
-      <c r="D62" s="201"/>
+      <c r="D62" s="199"/>
       <c r="E62" s="41"/>
       <c r="F62" s="42"/>
       <c r="G62" s="43"/>
@@ -20501,7 +20570,7 @@
     <row r="63" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B63" s="37"/>
       <c r="C63" s="38"/>
-      <c r="D63" s="201"/>
+      <c r="D63" s="199"/>
       <c r="E63" s="45" t="s">
         <v>6</v>
       </c>
@@ -20515,7 +20584,7 @@
     <row r="64" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="37"/>
       <c r="C64" s="38"/>
-      <c r="D64" s="201"/>
+      <c r="D64" s="199"/>
       <c r="E64" s="45"/>
       <c r="F64" s="42"/>
       <c r="G64" s="46"/>
@@ -20525,19 +20594,19 @@
     <row r="65" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B65" s="37"/>
       <c r="C65" s="38"/>
-      <c r="D65" s="201"/>
-      <c r="E65" s="216">
+      <c r="D65" s="199"/>
+      <c r="E65" s="218">
         <f>E61-G61</f>
         <v>0</v>
       </c>
-      <c r="F65" s="217"/>
-      <c r="G65" s="218"/>
+      <c r="F65" s="219"/>
+      <c r="G65" s="220"/>
       <c r="I65" s="2"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B66" s="37"/>
       <c r="C66" s="38"/>
-      <c r="D66" s="201"/>
+      <c r="D66" s="199"/>
       <c r="E66" s="41"/>
       <c r="F66" s="42"/>
       <c r="G66" s="43"/>
@@ -20546,19 +20615,19 @@
     <row r="67" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B67" s="37"/>
       <c r="C67" s="38"/>
-      <c r="D67" s="201"/>
-      <c r="E67" s="219" t="s">
+      <c r="D67" s="199"/>
+      <c r="E67" s="221" t="s">
         <v>8</v>
       </c>
-      <c r="F67" s="219"/>
-      <c r="G67" s="219"/>
+      <c r="F67" s="221"/>
+      <c r="G67" s="221"/>
       <c r="I67" s="2"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="111"/>
       <c r="B68" s="112"/>
       <c r="C68" s="113"/>
-      <c r="D68" s="202"/>
+      <c r="D68" s="200"/>
       <c r="E68" s="115"/>
       <c r="F68" s="116"/>
       <c r="G68" s="117"/>
@@ -20568,7 +20637,7 @@
       <c r="A69" s="101"/>
       <c r="B69" s="102"/>
       <c r="C69" s="103"/>
-      <c r="D69" s="203"/>
+      <c r="D69" s="201"/>
       <c r="E69" s="50"/>
       <c r="F69" s="51"/>
       <c r="G69" s="50"/>
@@ -20579,7 +20648,7 @@
       <c r="A70" s="118"/>
       <c r="B70" s="119"/>
       <c r="C70" s="120"/>
-      <c r="D70" s="204"/>
+      <c r="D70" s="202"/>
       <c r="E70" s="122"/>
       <c r="F70" s="123"/>
       <c r="G70" s="124"/>
@@ -20590,7 +20659,7 @@
       <c r="A71" s="118"/>
       <c r="B71" s="119"/>
       <c r="C71" s="120"/>
-      <c r="D71" s="204"/>
+      <c r="D71" s="202"/>
       <c r="E71" s="122"/>
       <c r="F71" s="123"/>
       <c r="G71" s="124"/>
@@ -20601,7 +20670,7 @@
       <c r="A72" s="118"/>
       <c r="B72" s="119"/>
       <c r="C72" s="120"/>
-      <c r="D72" s="204"/>
+      <c r="D72" s="202"/>
       <c r="E72" s="122"/>
       <c r="F72" s="123"/>
       <c r="G72" s="124"/>
@@ -20612,7 +20681,7 @@
       <c r="A73" s="118"/>
       <c r="B73" s="119"/>
       <c r="C73" s="120"/>
-      <c r="D73" s="204"/>
+      <c r="D73" s="202"/>
       <c r="E73" s="122"/>
       <c r="F73" s="123"/>
       <c r="G73" s="124"/>
@@ -20623,7 +20692,7 @@
       <c r="A74" s="118"/>
       <c r="B74" s="119"/>
       <c r="C74" s="120"/>
-      <c r="D74" s="204"/>
+      <c r="D74" s="202"/>
       <c r="E74" s="122"/>
       <c r="F74" s="123"/>
       <c r="G74" s="124"/>
@@ -20634,7 +20703,7 @@
       <c r="A75" s="118"/>
       <c r="B75" s="119"/>
       <c r="C75" s="120"/>
-      <c r="D75" s="204"/>
+      <c r="D75" s="202"/>
       <c r="E75" s="122"/>
       <c r="F75" s="123"/>
       <c r="G75" s="124"/>
@@ -20645,7 +20714,7 @@
       <c r="A76" s="118"/>
       <c r="B76" s="119"/>
       <c r="C76" s="120"/>
-      <c r="D76" s="204"/>
+      <c r="D76" s="202"/>
       <c r="E76" s="122"/>
       <c r="F76" s="123"/>
       <c r="G76" s="124"/>
@@ -20656,7 +20725,7 @@
       <c r="A77" s="118"/>
       <c r="B77" s="119"/>
       <c r="C77" s="120"/>
-      <c r="D77" s="204"/>
+      <c r="D77" s="202"/>
       <c r="E77" s="122"/>
       <c r="F77" s="123"/>
       <c r="G77" s="124"/>
@@ -20667,7 +20736,7 @@
       <c r="A78" s="118"/>
       <c r="B78" s="119"/>
       <c r="C78" s="120"/>
-      <c r="D78" s="204"/>
+      <c r="D78" s="202"/>
       <c r="E78" s="122"/>
       <c r="F78" s="123"/>
       <c r="G78" s="124"/>
@@ -20678,7 +20747,7 @@
       <c r="A79" s="118"/>
       <c r="B79" s="119"/>
       <c r="C79" s="120"/>
-      <c r="D79" s="204"/>
+      <c r="D79" s="202"/>
       <c r="E79" s="122"/>
       <c r="F79" s="123"/>
       <c r="G79" s="124"/>
@@ -20688,7 +20757,7 @@
       <c r="A80" s="105"/>
       <c r="B80" s="106"/>
       <c r="C80" s="107"/>
-      <c r="D80" s="205"/>
+      <c r="D80" s="203"/>
       <c r="E80" s="108"/>
       <c r="F80" s="109"/>
       <c r="G80" s="110"/>
@@ -20733,25 +20802,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="223" t="s">
+      <c r="B1" s="225" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="225"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -20945,10 +21014,10 @@
       <c r="E10" s="20">
         <v>9568</v>
       </c>
-      <c r="F10" s="197">
+      <c r="F10" s="195">
         <v>44767</v>
       </c>
-      <c r="G10" s="198">
+      <c r="G10" s="196">
         <v>9568</v>
       </c>
       <c r="H10" s="18">
@@ -21168,10 +21237,10 @@
       <c r="E19" s="20">
         <v>80</v>
       </c>
-      <c r="F19" s="197">
+      <c r="F19" s="195">
         <v>44767</v>
       </c>
-      <c r="G19" s="198">
+      <c r="G19" s="196">
         <v>80</v>
       </c>
       <c r="H19" s="18">
@@ -21218,10 +21287,10 @@
       <c r="E21" s="20">
         <v>1273</v>
       </c>
-      <c r="F21" s="197">
+      <c r="F21" s="195">
         <v>44767</v>
       </c>
-      <c r="G21" s="198">
+      <c r="G21" s="196">
         <v>1273</v>
       </c>
       <c r="H21" s="18">
@@ -21702,12 +21771,12 @@
       <c r="B43" s="37"/>
       <c r="C43" s="38"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="216">
+      <c r="E43" s="218">
         <f>E39-G39</f>
         <v>0</v>
       </c>
-      <c r="F43" s="217"/>
-      <c r="G43" s="218"/>
+      <c r="F43" s="219"/>
+      <c r="G43" s="220"/>
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -21723,11 +21792,11 @@
       <c r="B45" s="37"/>
       <c r="C45" s="38"/>
       <c r="D45" s="2"/>
-      <c r="E45" s="219" t="s">
+      <c r="E45" s="221" t="s">
         <v>8</v>
       </c>
-      <c r="F45" s="219"/>
-      <c r="G45" s="219"/>
+      <c r="F45" s="221"/>
+      <c r="G45" s="221"/>
       <c r="I45" s="2"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -21913,18 +21982,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="226"/>
-      <c r="B1" s="227"/>
-      <c r="C1" s="227"/>
-      <c r="D1" s="227"/>
-      <c r="E1" s="227"/>
-      <c r="F1" s="227"/>
-      <c r="G1" s="227"/>
-      <c r="H1" s="227"/>
-      <c r="I1" s="227"/>
-      <c r="J1" s="227"/>
-      <c r="K1" s="227"/>
-      <c r="L1" s="227"/>
+      <c r="A1" s="228"/>
+      <c r="B1" s="229"/>
+      <c r="C1" s="229"/>
+      <c r="D1" s="229"/>
+      <c r="E1" s="229"/>
+      <c r="F1" s="229"/>
+      <c r="G1" s="229"/>
+      <c r="H1" s="229"/>
+      <c r="I1" s="229"/>
+      <c r="J1" s="229"/>
+      <c r="K1" s="229"/>
+      <c r="L1" s="229"/>
     </row>
     <row r="2" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="156" t="s">
@@ -23163,11 +23232,11 @@
       <c r="L62" s="121"/>
     </row>
     <row r="63" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K63" s="228">
+      <c r="K63" s="230">
         <f>SUM(K39:K62)</f>
         <v>850487.21</v>
       </c>
-      <c r="L63" s="229"/>
+      <c r="L63" s="231"/>
     </row>
     <row r="68" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K68" s="54"/>

</xml_diff>

<commit_message>
cierre 29 agosto 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #08  AGOSTO 2022/CREDITOS  4 CARNES   ZAVALETA   AGOSTO     2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #08  AGOSTO 2022/CREDITOS  4 CARNES   ZAVALETA   AGOSTO     2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="13" activeTab="13"/>
+    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="12" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="REMISIONES OCTUBRE  2021     " sheetId="4" r:id="rId1"/>
@@ -1077,7 +1077,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -1457,12 +1457,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="306">
+  <cellXfs count="305">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1897,8 +1906,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="28" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="28" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1947,7 +1954,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1977,7 +1983,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="7" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2083,6 +2088,11 @@
     <xf numFmtId="0" fontId="15" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2533,16 +2543,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>737565</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>403464</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>117135</xdr:rowOff>
+      <xdr:rowOff>107610</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2571,16 +2581,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>21981</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>58615</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>632167</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>1824</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>297099</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3967,24 +3977,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="276" t="s">
+      <c r="B1" s="272" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="277"/>
-      <c r="D1" s="277"/>
-      <c r="E1" s="277"/>
-      <c r="F1" s="278"/>
+      <c r="C1" s="273"/>
+      <c r="D1" s="273"/>
+      <c r="E1" s="273"/>
+      <c r="F1" s="274"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="271" t="s">
+      <c r="B2" s="267" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="267"/>
+      <c r="E2" s="267"/>
+      <c r="F2" s="267"/>
       <c r="G2" s="5"/>
       <c r="H2" s="2"/>
     </row>
@@ -5130,12 +5140,12 @@
     <row r="55" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B55" s="37"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="272">
+      <c r="D55" s="268">
         <f>D51-F51</f>
         <v>0</v>
       </c>
-      <c r="E55" s="273"/>
-      <c r="F55" s="274"/>
+      <c r="E55" s="269"/>
+      <c r="F55" s="270"/>
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -5149,11 +5159,11 @@
     <row r="57" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B57" s="37"/>
       <c r="C57" s="2"/>
-      <c r="D57" s="275" t="s">
+      <c r="D57" s="271" t="s">
         <v>8</v>
       </c>
-      <c r="E57" s="275"/>
-      <c r="F57" s="275"/>
+      <c r="E57" s="271"/>
+      <c r="F57" s="271"/>
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -5282,25 +5292,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="279" t="s">
+      <c r="B1" s="275" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="280"/>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="281"/>
+      <c r="C1" s="276"/>
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="276"/>
+      <c r="G1" s="277"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="271" t="s">
+      <c r="B2" s="267" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="267"/>
+      <c r="E2" s="267"/>
+      <c r="F2" s="267"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -6397,12 +6407,12 @@
       <c r="B50" s="37"/>
       <c r="C50" s="38"/>
       <c r="D50" s="198"/>
-      <c r="E50" s="272">
+      <c r="E50" s="268">
         <f>E46-G46</f>
         <v>0</v>
       </c>
-      <c r="F50" s="273"/>
-      <c r="G50" s="274"/>
+      <c r="F50" s="269"/>
+      <c r="G50" s="270"/>
       <c r="I50" s="2"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -6418,11 +6428,11 @@
       <c r="B52" s="37"/>
       <c r="C52" s="38"/>
       <c r="D52" s="198"/>
-      <c r="E52" s="275" t="s">
+      <c r="E52" s="271" t="s">
         <v>8</v>
       </c>
-      <c r="F52" s="275"/>
-      <c r="G52" s="275"/>
+      <c r="F52" s="271"/>
+      <c r="G52" s="271"/>
       <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -6621,18 +6631,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="Q1" s="282"/>
-      <c r="R1" s="283"/>
-      <c r="S1" s="283"/>
-      <c r="T1" s="283"/>
-      <c r="U1" s="283"/>
-      <c r="V1" s="283"/>
-      <c r="W1" s="283"/>
-      <c r="X1" s="283"/>
-      <c r="Y1" s="283"/>
-      <c r="Z1" s="283"/>
-      <c r="AA1" s="283"/>
-      <c r="AB1" s="283"/>
+      <c r="Q1" s="278"/>
+      <c r="R1" s="279"/>
+      <c r="S1" s="279"/>
+      <c r="T1" s="279"/>
+      <c r="U1" s="279"/>
+      <c r="V1" s="279"/>
+      <c r="W1" s="279"/>
+      <c r="X1" s="279"/>
+      <c r="Y1" s="279"/>
+      <c r="Z1" s="279"/>
+      <c r="AA1" s="279"/>
+      <c r="AB1" s="279"/>
     </row>
     <row r="2" spans="2:35" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="155" t="s">
@@ -7286,10 +7296,10 @@
         <v>101</v>
       </c>
       <c r="R19" s="128"/>
-      <c r="S19" s="286" t="s">
+      <c r="S19" s="282" t="s">
         <v>95</v>
       </c>
-      <c r="T19" s="287"/>
+      <c r="T19" s="283"/>
       <c r="U19" s="77">
         <f t="shared" si="1"/>
         <v>11454.260000000009</v>
@@ -7659,7 +7669,7 @@
       <c r="C35" s="175" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="223">
+      <c r="D35" s="221">
         <v>-1210693.69</v>
       </c>
       <c r="E35" s="20">
@@ -7668,94 +7678,94 @@
       </c>
     </row>
     <row r="36" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="288" t="s">
+      <c r="B36" s="284" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="289"/>
-      <c r="D36" s="290"/>
+      <c r="C36" s="285"/>
+      <c r="D36" s="286"/>
       <c r="E36" s="183">
         <f t="shared" si="0"/>
         <v>0.31000000005587935</v>
       </c>
     </row>
     <row r="37" spans="1:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="291"/>
-      <c r="C37" s="292"/>
-      <c r="D37" s="293"/>
+      <c r="B37" s="287"/>
+      <c r="C37" s="288"/>
+      <c r="D37" s="289"/>
     </row>
     <row r="38" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="40" spans="1:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="231"/>
-      <c r="B40" s="232"/>
-      <c r="C40" s="232"/>
-      <c r="D40" s="232"/>
-      <c r="E40" s="232"/>
-      <c r="F40" s="233"/>
+      <c r="A40" s="229"/>
+      <c r="B40" s="230"/>
+      <c r="C40" s="230"/>
+      <c r="D40" s="230"/>
+      <c r="E40" s="230"/>
+      <c r="F40" s="231"/>
     </row>
     <row r="41" spans="1:28" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="234"/>
-      <c r="B41" s="294" t="s">
+      <c r="A41" s="232"/>
+      <c r="B41" s="290" t="s">
         <v>108</v>
       </c>
-      <c r="C41" s="295"/>
-      <c r="D41" s="295"/>
-      <c r="E41" s="296"/>
-      <c r="F41" s="235"/>
+      <c r="C41" s="291"/>
+      <c r="D41" s="291"/>
+      <c r="E41" s="292"/>
+      <c r="F41" s="233"/>
       <c r="AA41" s="173"/>
     </row>
     <row r="42" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="234"/>
-      <c r="B42" s="236"/>
-      <c r="C42" s="237"/>
+      <c r="A42" s="232"/>
+      <c r="B42" s="234"/>
+      <c r="C42" s="235"/>
       <c r="D42" s="62"/>
-      <c r="E42" s="238"/>
-      <c r="F42" s="235"/>
+      <c r="E42" s="236"/>
+      <c r="F42" s="233"/>
       <c r="AA42" s="173"/>
     </row>
     <row r="43" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="234"/>
-      <c r="B43" s="224">
+      <c r="A43" s="232"/>
+      <c r="B43" s="222">
         <v>44723</v>
       </c>
-      <c r="C43" s="225" t="s">
+      <c r="C43" s="223" t="s">
         <v>109</v>
       </c>
-      <c r="D43" s="226">
+      <c r="D43" s="224">
         <v>75251.399999999994</v>
       </c>
-      <c r="E43" s="238"/>
-      <c r="F43" s="235"/>
+      <c r="E43" s="236"/>
+      <c r="F43" s="233"/>
       <c r="AA43" s="173"/>
     </row>
     <row r="44" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A44" s="234"/>
-      <c r="B44" s="224">
+      <c r="A44" s="232"/>
+      <c r="B44" s="222">
         <v>44725</v>
       </c>
-      <c r="C44" s="225" t="s">
+      <c r="C44" s="223" t="s">
         <v>110</v>
       </c>
-      <c r="D44" s="226">
+      <c r="D44" s="224">
         <v>59986.66</v>
       </c>
-      <c r="E44" s="238"/>
-      <c r="F44" s="235"/>
+      <c r="E44" s="236"/>
+      <c r="F44" s="233"/>
       <c r="AA44" s="173"/>
     </row>
     <row r="45" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A45" s="234"/>
-      <c r="B45" s="224">
+      <c r="A45" s="232"/>
+      <c r="B45" s="222">
         <v>44726</v>
       </c>
-      <c r="C45" s="225" t="s">
+      <c r="C45" s="223" t="s">
         <v>111</v>
       </c>
-      <c r="D45" s="226">
+      <c r="D45" s="224">
         <v>28057.52</v>
       </c>
-      <c r="E45" s="238"/>
-      <c r="F45" s="235"/>
+      <c r="E45" s="236"/>
+      <c r="F45" s="233"/>
       <c r="Q45" s="121"/>
       <c r="R45" s="121"/>
       <c r="S45" s="121"/>
@@ -7767,18 +7777,18 @@
       <c r="AA45" s="173"/>
     </row>
     <row r="46" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A46" s="234"/>
-      <c r="B46" s="224">
+      <c r="A46" s="232"/>
+      <c r="B46" s="222">
         <v>44726</v>
       </c>
-      <c r="C46" s="225" t="s">
+      <c r="C46" s="223" t="s">
         <v>112</v>
       </c>
-      <c r="D46" s="226">
+      <c r="D46" s="224">
         <v>4554</v>
       </c>
-      <c r="E46" s="238"/>
-      <c r="F46" s="235"/>
+      <c r="E46" s="236"/>
+      <c r="F46" s="233"/>
       <c r="Q46" s="121"/>
       <c r="R46" s="121"/>
       <c r="S46" s="121"/>
@@ -7793,18 +7803,18 @@
       <c r="AB46" s="60"/>
     </row>
     <row r="47" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A47" s="234"/>
-      <c r="B47" s="224">
+      <c r="A47" s="232"/>
+      <c r="B47" s="222">
         <v>44727</v>
       </c>
-      <c r="C47" s="225" t="s">
+      <c r="C47" s="223" t="s">
         <v>113</v>
       </c>
-      <c r="D47" s="226">
+      <c r="D47" s="224">
         <v>20506.8</v>
       </c>
-      <c r="E47" s="238"/>
-      <c r="F47" s="235"/>
+      <c r="E47" s="236"/>
+      <c r="F47" s="233"/>
       <c r="Q47" s="121"/>
       <c r="R47" s="121"/>
       <c r="S47" s="121"/>
@@ -7819,18 +7829,18 @@
       <c r="AB47" s="60"/>
     </row>
     <row r="48" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A48" s="234"/>
-      <c r="B48" s="224">
+      <c r="A48" s="232"/>
+      <c r="B48" s="222">
         <v>44728</v>
       </c>
-      <c r="C48" s="225" t="s">
+      <c r="C48" s="223" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="226">
+      <c r="D48" s="224">
         <v>70754.91</v>
       </c>
-      <c r="E48" s="238"/>
-      <c r="F48" s="235"/>
+      <c r="E48" s="236"/>
+      <c r="F48" s="233"/>
       <c r="Q48" s="121"/>
       <c r="R48" s="121"/>
       <c r="S48" s="121"/>
@@ -7845,18 +7855,18 @@
       <c r="AB48" s="60"/>
     </row>
     <row r="49" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A49" s="234"/>
-      <c r="B49" s="224">
+      <c r="A49" s="232"/>
+      <c r="B49" s="222">
         <v>44729</v>
       </c>
-      <c r="C49" s="225" t="s">
+      <c r="C49" s="223" t="s">
         <v>115</v>
       </c>
-      <c r="D49" s="226">
+      <c r="D49" s="224">
         <v>102195.9</v>
       </c>
-      <c r="E49" s="238"/>
-      <c r="F49" s="235"/>
+      <c r="E49" s="236"/>
+      <c r="F49" s="233"/>
       <c r="Q49" s="121"/>
       <c r="R49" s="121"/>
       <c r="S49" s="121"/>
@@ -7871,18 +7881,18 @@
       <c r="AB49" s="60"/>
     </row>
     <row r="50" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A50" s="234"/>
-      <c r="B50" s="224">
+      <c r="A50" s="232"/>
+      <c r="B50" s="222">
         <v>44730</v>
       </c>
-      <c r="C50" s="227" t="s">
+      <c r="C50" s="225" t="s">
         <v>116</v>
       </c>
-      <c r="D50" s="226">
+      <c r="D50" s="224">
         <v>64559.72</v>
       </c>
-      <c r="E50" s="238"/>
-      <c r="F50" s="235"/>
+      <c r="E50" s="236"/>
+      <c r="F50" s="233"/>
       <c r="Q50" s="121"/>
       <c r="R50" s="121"/>
       <c r="S50" s="121"/>
@@ -7897,18 +7907,18 @@
       <c r="AB50" s="60"/>
     </row>
     <row r="51" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A51" s="234"/>
-      <c r="B51" s="224">
+      <c r="A51" s="232"/>
+      <c r="B51" s="222">
         <v>44732</v>
       </c>
-      <c r="C51" s="225" t="s">
+      <c r="C51" s="223" t="s">
         <v>117</v>
       </c>
-      <c r="D51" s="226">
+      <c r="D51" s="224">
         <v>68026</v>
       </c>
-      <c r="E51" s="238"/>
-      <c r="F51" s="235"/>
+      <c r="E51" s="236"/>
+      <c r="F51" s="233"/>
       <c r="Q51" s="121"/>
       <c r="R51" s="121"/>
       <c r="S51" s="121"/>
@@ -7923,18 +7933,18 @@
       <c r="AB51" s="60"/>
     </row>
     <row r="52" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A52" s="234"/>
-      <c r="B52" s="224">
+      <c r="A52" s="232"/>
+      <c r="B52" s="222">
         <v>44733</v>
       </c>
-      <c r="C52" s="225" t="s">
+      <c r="C52" s="223" t="s">
         <v>118</v>
       </c>
-      <c r="D52" s="226">
+      <c r="D52" s="224">
         <v>66413.16</v>
       </c>
-      <c r="E52" s="238"/>
-      <c r="F52" s="235"/>
+      <c r="E52" s="236"/>
+      <c r="F52" s="233"/>
       <c r="Q52" s="121"/>
       <c r="R52" s="121"/>
       <c r="S52" s="121"/>
@@ -7949,18 +7959,18 @@
       <c r="AB52" s="60"/>
     </row>
     <row r="53" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A53" s="234"/>
-      <c r="B53" s="224">
+      <c r="A53" s="232"/>
+      <c r="B53" s="222">
         <v>44733</v>
       </c>
-      <c r="C53" s="225" t="s">
+      <c r="C53" s="223" t="s">
         <v>119</v>
       </c>
-      <c r="D53" s="226">
+      <c r="D53" s="224">
         <v>2197.8000000000002</v>
       </c>
-      <c r="E53" s="253"/>
-      <c r="F53" s="235"/>
+      <c r="E53" s="251"/>
+      <c r="F53" s="233"/>
       <c r="Q53" s="121"/>
       <c r="R53" s="121"/>
       <c r="S53" s="121"/>
@@ -7975,18 +7985,18 @@
       <c r="AB53" s="60"/>
     </row>
     <row r="54" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A54" s="234"/>
-      <c r="B54" s="224">
+      <c r="A54" s="232"/>
+      <c r="B54" s="222">
         <v>44734</v>
       </c>
-      <c r="C54" s="225" t="s">
+      <c r="C54" s="223" t="s">
         <v>120</v>
       </c>
-      <c r="D54" s="226">
+      <c r="D54" s="224">
         <v>55732.800000000003</v>
       </c>
-      <c r="E54" s="253"/>
-      <c r="F54" s="235"/>
+      <c r="E54" s="251"/>
+      <c r="F54" s="233"/>
       <c r="Q54" s="121"/>
       <c r="R54" s="121"/>
       <c r="S54" s="121"/>
@@ -8001,18 +8011,18 @@
       <c r="AB54" s="60"/>
     </row>
     <row r="55" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A55" s="234"/>
-      <c r="B55" s="224">
+      <c r="A55" s="232"/>
+      <c r="B55" s="222">
         <v>44735</v>
       </c>
-      <c r="C55" s="225" t="s">
+      <c r="C55" s="223" t="s">
         <v>121</v>
       </c>
-      <c r="D55" s="226">
+      <c r="D55" s="224">
         <v>106959.76</v>
       </c>
-      <c r="E55" s="238"/>
-      <c r="F55" s="235"/>
+      <c r="E55" s="236"/>
+      <c r="F55" s="233"/>
       <c r="Q55" s="121"/>
       <c r="R55" s="121"/>
       <c r="S55" s="121"/>
@@ -8027,18 +8037,18 @@
       <c r="AB55" s="60"/>
     </row>
     <row r="56" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A56" s="234"/>
-      <c r="B56" s="224">
+      <c r="A56" s="232"/>
+      <c r="B56" s="222">
         <v>44736</v>
       </c>
-      <c r="C56" s="225" t="s">
+      <c r="C56" s="223" t="s">
         <v>122</v>
       </c>
-      <c r="D56" s="226">
+      <c r="D56" s="224">
         <v>69961.259999999995</v>
       </c>
-      <c r="E56" s="238"/>
-      <c r="F56" s="235"/>
+      <c r="E56" s="236"/>
+      <c r="F56" s="233"/>
       <c r="Q56" s="121"/>
       <c r="R56" s="121"/>
       <c r="S56" s="121"/>
@@ -8053,18 +8063,18 @@
       <c r="AB56" s="60"/>
     </row>
     <row r="57" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A57" s="234"/>
-      <c r="B57" s="224">
+      <c r="A57" s="232"/>
+      <c r="B57" s="222">
         <v>44737</v>
       </c>
-      <c r="C57" s="225" t="s">
+      <c r="C57" s="223" t="s">
         <v>123</v>
       </c>
-      <c r="D57" s="226">
+      <c r="D57" s="224">
         <v>81212.86</v>
       </c>
-      <c r="E57" s="238"/>
-      <c r="F57" s="235"/>
+      <c r="E57" s="236"/>
+      <c r="F57" s="233"/>
       <c r="Q57" s="121"/>
       <c r="R57" s="121"/>
       <c r="S57" s="121"/>
@@ -8079,20 +8089,20 @@
       <c r="AB57" s="60"/>
     </row>
     <row r="58" spans="1:28" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A58" s="234"/>
-      <c r="B58" s="228">
+      <c r="A58" s="232"/>
+      <c r="B58" s="226">
         <v>44739</v>
       </c>
-      <c r="C58" s="225" t="s">
+      <c r="C58" s="223" t="s">
         <v>124</v>
       </c>
-      <c r="D58" s="226">
+      <c r="D58" s="224">
         <v>24074.75</v>
       </c>
-      <c r="E58" s="252" t="s">
+      <c r="E58" s="250" t="s">
         <v>128</v>
       </c>
-      <c r="F58" s="235"/>
+      <c r="F58" s="233"/>
       <c r="Q58" s="121"/>
       <c r="R58" s="121"/>
       <c r="S58" s="121"/>
@@ -8107,14 +8117,14 @@
       <c r="AB58" s="60"/>
     </row>
     <row r="59" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A59" s="234"/>
-      <c r="B59" s="239"/>
-      <c r="C59" s="240"/>
-      <c r="D59" s="241">
-        <v>0</v>
-      </c>
-      <c r="E59" s="238"/>
-      <c r="F59" s="235"/>
+      <c r="A59" s="232"/>
+      <c r="B59" s="237"/>
+      <c r="C59" s="238"/>
+      <c r="D59" s="239">
+        <v>0</v>
+      </c>
+      <c r="E59" s="236"/>
+      <c r="F59" s="233"/>
       <c r="Q59" s="121"/>
       <c r="R59" s="121"/>
       <c r="S59" s="121"/>
@@ -8129,15 +8139,15 @@
       <c r="AB59" s="60"/>
     </row>
     <row r="60" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A60" s="234"/>
-      <c r="B60" s="239"/>
-      <c r="C60" s="240"/>
-      <c r="D60" s="242">
+      <c r="A60" s="232"/>
+      <c r="B60" s="237"/>
+      <c r="C60" s="238"/>
+      <c r="D60" s="240">
         <f>SUM(D43:D59)</f>
         <v>900445.3</v>
       </c>
-      <c r="E60" s="238"/>
-      <c r="F60" s="235"/>
+      <c r="E60" s="236"/>
+      <c r="F60" s="233"/>
       <c r="Q60" s="121"/>
       <c r="R60" s="121"/>
       <c r="S60" s="121"/>
@@ -8152,18 +8162,18 @@
       <c r="AB60" s="60"/>
     </row>
     <row r="61" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="A61" s="234"/>
-      <c r="B61" s="239">
+      <c r="A61" s="232"/>
+      <c r="B61" s="237">
         <v>44769</v>
       </c>
-      <c r="C61" s="243" t="s">
+      <c r="C61" s="241" t="s">
         <v>125</v>
       </c>
-      <c r="D61" s="244">
+      <c r="D61" s="242">
         <v>-789400</v>
       </c>
-      <c r="E61" s="238"/>
-      <c r="F61" s="235"/>
+      <c r="E61" s="236"/>
+      <c r="F61" s="233"/>
       <c r="Q61" s="121"/>
       <c r="R61" s="121"/>
       <c r="S61" s="121"/>
@@ -8178,55 +8188,55 @@
       <c r="AB61" s="60"/>
     </row>
     <row r="62" spans="1:28" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="234"/>
-      <c r="B62" s="239">
+      <c r="A62" s="232"/>
+      <c r="B62" s="237">
         <v>44769</v>
       </c>
-      <c r="C62" s="245" t="s">
+      <c r="C62" s="243" t="s">
         <v>126</v>
       </c>
-      <c r="D62" s="244">
+      <c r="D62" s="242">
         <v>-111045.3</v>
       </c>
-      <c r="E62" s="238"/>
-      <c r="F62" s="235"/>
+      <c r="E62" s="236"/>
+      <c r="F62" s="233"/>
       <c r="AA62" s="173"/>
       <c r="AB62" s="60"/>
     </row>
     <row r="63" spans="1:28" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="234"/>
-      <c r="B63" s="239"/>
-      <c r="C63" s="229" t="s">
+      <c r="A63" s="232"/>
+      <c r="B63" s="237"/>
+      <c r="C63" s="227" t="s">
         <v>127</v>
       </c>
-      <c r="D63" s="230">
+      <c r="D63" s="228">
         <f>D60+D61+D62</f>
         <v>0</v>
       </c>
-      <c r="E63" s="238"/>
-      <c r="F63" s="235"/>
+      <c r="E63" s="236"/>
+      <c r="F63" s="233"/>
       <c r="AA63" s="173"/>
       <c r="AB63" s="127"/>
     </row>
     <row r="64" spans="1:28" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="234"/>
-      <c r="B64" s="239"/>
-      <c r="C64" s="240"/>
-      <c r="D64" s="241"/>
-      <c r="E64" s="238"/>
-      <c r="F64" s="235"/>
+      <c r="A64" s="232"/>
+      <c r="B64" s="237"/>
+      <c r="C64" s="238"/>
+      <c r="D64" s="239"/>
+      <c r="E64" s="236"/>
+      <c r="F64" s="233"/>
       <c r="AA64" s="173"/>
       <c r="AB64" s="121"/>
     </row>
     <row r="65" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="246"/>
-      <c r="B65" s="247"/>
-      <c r="C65" s="248"/>
-      <c r="D65" s="249"/>
-      <c r="E65" s="250"/>
-      <c r="F65" s="251"/>
-      <c r="AA65" s="284"/>
-      <c r="AB65" s="285"/>
+      <c r="A65" s="244"/>
+      <c r="B65" s="245"/>
+      <c r="C65" s="246"/>
+      <c r="D65" s="247"/>
+      <c r="E65" s="248"/>
+      <c r="F65" s="249"/>
+      <c r="AA65" s="280"/>
+      <c r="AB65" s="281"/>
     </row>
     <row r="70" spans="1:28" x14ac:dyDescent="0.3">
       <c r="AA70" s="54"/>
@@ -8270,25 +8280,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="279" t="s">
+      <c r="B1" s="275" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="280"/>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="281"/>
+      <c r="C1" s="276"/>
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="276"/>
+      <c r="G1" s="277"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="271" t="s">
+      <c r="B2" s="267" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="267"/>
+      <c r="E2" s="267"/>
+      <c r="F2" s="267"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -9471,12 +9481,12 @@
       <c r="B55" s="37"/>
       <c r="C55" s="38"/>
       <c r="D55" s="198"/>
-      <c r="E55" s="272">
+      <c r="E55" s="268">
         <f>E51-G51</f>
         <v>40994</v>
       </c>
-      <c r="F55" s="273"/>
-      <c r="G55" s="274"/>
+      <c r="F55" s="269"/>
+      <c r="G55" s="270"/>
       <c r="I55" s="2"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -9492,11 +9502,11 @@
       <c r="B57" s="37"/>
       <c r="C57" s="38"/>
       <c r="D57" s="198"/>
-      <c r="E57" s="275" t="s">
+      <c r="E57" s="271" t="s">
         <v>8</v>
       </c>
-      <c r="F57" s="275"/>
-      <c r="G57" s="275"/>
+      <c r="F57" s="271"/>
+      <c r="G57" s="271"/>
       <c r="I57" s="2"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -9660,10 +9670,10 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B1:AJ78"/>
+  <dimension ref="B1:AN78"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -9672,80 +9682,88 @@
     <col min="2" max="2" width="14" style="114" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="114"/>
     <col min="4" max="4" width="15" style="114" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="114" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="208"/>
-    <col min="7" max="12" width="11.42578125" style="114"/>
-    <col min="13" max="13" width="39.140625" style="114" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="114" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" style="114" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="114" customWidth="1"/>
-    <col min="17" max="17" width="20" style="114" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" style="114" customWidth="1"/>
-    <col min="19" max="19" width="15.140625" style="114" customWidth="1"/>
-    <col min="20" max="20" width="14.85546875" style="114" customWidth="1"/>
-    <col min="21" max="21" width="18.28515625" style="114" customWidth="1"/>
-    <col min="22" max="22" width="19.28515625" style="114" customWidth="1"/>
-    <col min="23" max="26" width="11.42578125" style="114"/>
-    <col min="27" max="27" width="14.85546875" style="136" customWidth="1"/>
-    <col min="28" max="28" width="16.7109375" style="115" customWidth="1"/>
-    <col min="29" max="29" width="15.5703125" style="114" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.42578125" style="140"/>
-    <col min="31" max="32" width="11.42578125" style="114"/>
-    <col min="33" max="33" width="13.85546875" style="114" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.42578125" style="114"/>
-    <col min="35" max="35" width="17.42578125" style="114" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="11.42578125" style="114"/>
+    <col min="5" max="5" width="16.85546875" style="114" customWidth="1"/>
+    <col min="6" max="6" width="3.140625" style="208" customWidth="1"/>
+    <col min="7" max="8" width="11.42578125" style="208"/>
+    <col min="9" max="9" width="14.140625" style="208" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" style="208" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="11.42578125" style="114"/>
+    <col min="17" max="17" width="39.140625" style="114" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="114" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" style="114" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" style="114" customWidth="1"/>
+    <col min="21" max="21" width="20" style="114" customWidth="1"/>
+    <col min="22" max="22" width="14.7109375" style="114" customWidth="1"/>
+    <col min="23" max="23" width="15.140625" style="114" customWidth="1"/>
+    <col min="24" max="24" width="14.85546875" style="114" customWidth="1"/>
+    <col min="25" max="25" width="18.28515625" style="114" customWidth="1"/>
+    <col min="26" max="26" width="19.28515625" style="114" customWidth="1"/>
+    <col min="27" max="30" width="11.42578125" style="114"/>
+    <col min="31" max="31" width="14.85546875" style="136" customWidth="1"/>
+    <col min="32" max="32" width="16.7109375" style="115" customWidth="1"/>
+    <col min="33" max="33" width="15.5703125" style="114" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.42578125" style="140"/>
+    <col min="35" max="36" width="11.42578125" style="114"/>
+    <col min="37" max="37" width="13.85546875" style="114" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.42578125" style="114"/>
+    <col min="39" max="39" width="17.42578125" style="114" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="11.42578125" style="114"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:36" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="R1" s="268"/>
-      <c r="S1" s="219"/>
-      <c r="T1" s="219"/>
-      <c r="U1" s="219"/>
-      <c r="V1" s="219"/>
-      <c r="W1" s="219"/>
-      <c r="X1" s="219"/>
-      <c r="Y1" s="219"/>
-      <c r="Z1" s="219"/>
-      <c r="AA1" s="219"/>
-      <c r="AB1" s="219"/>
-      <c r="AC1" s="219"/>
-    </row>
-    <row r="2" spans="2:36" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="155" t="s">
+    <row r="1" spans="2:40" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V1" s="265"/>
+      <c r="W1" s="217"/>
+      <c r="X1" s="217"/>
+      <c r="Y1" s="217"/>
+      <c r="Z1" s="217"/>
+      <c r="AA1" s="217"/>
+      <c r="AB1" s="217"/>
+      <c r="AC1" s="217"/>
+      <c r="AD1" s="217"/>
+      <c r="AE1" s="217"/>
+      <c r="AF1" s="217"/>
+      <c r="AG1" s="217"/>
+    </row>
+    <row r="2" spans="2:40" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="302" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="O2" s="303" t="s">
+      <c r="C2" s="302"/>
+      <c r="D2" s="302"/>
+      <c r="E2" s="302"/>
+      <c r="F2" s="302"/>
+      <c r="G2" s="302"/>
+      <c r="H2" s="302"/>
+      <c r="I2" s="302"/>
+      <c r="J2" s="302"/>
+      <c r="S2" s="299" t="s">
         <v>160</v>
       </c>
-      <c r="P2" s="304"/>
-      <c r="Q2" s="305"/>
-      <c r="R2" s="269"/>
-      <c r="S2" s="170" t="s">
+      <c r="T2" s="300"/>
+      <c r="U2" s="301"/>
+      <c r="V2" s="266"/>
+      <c r="W2" s="170" t="s">
         <v>91</v>
       </c>
-      <c r="T2" s="171"/>
-      <c r="U2" s="171"/>
-      <c r="V2" s="171"/>
-      <c r="W2" s="154"/>
-      <c r="X2" s="154"/>
-      <c r="Y2" s="154"/>
-      <c r="Z2" s="154"/>
+      <c r="X2" s="171"/>
+      <c r="Y2" s="171"/>
+      <c r="Z2" s="171"/>
       <c r="AA2" s="154"/>
       <c r="AB2" s="154"/>
       <c r="AC2" s="154"/>
-      <c r="AD2" s="161"/>
-      <c r="AE2" s="163"/>
-      <c r="AF2" s="164"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="165"/>
-      <c r="AI2" s="62"/>
-      <c r="AJ2" s="121"/>
-    </row>
-    <row r="3" spans="2:36" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AD2" s="154"/>
+      <c r="AE2" s="154"/>
+      <c r="AF2" s="154"/>
+      <c r="AG2" s="154"/>
+      <c r="AH2" s="161"/>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
+      <c r="AK2" s="62"/>
+      <c r="AL2" s="165"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="121"/>
+    </row>
+    <row r="3" spans="2:40" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="130" t="s">
         <v>44</v>
       </c>
@@ -9758,41 +9776,41 @@
       <c r="E3" s="172" t="s">
         <v>94</v>
       </c>
-      <c r="O3" s="263">
+      <c r="S3" s="260">
         <v>44739</v>
       </c>
-      <c r="P3" s="264" t="s">
+      <c r="T3" s="261" t="s">
         <v>124</v>
       </c>
-      <c r="Q3" s="265">
+      <c r="U3" s="262">
         <v>25454.05</v>
       </c>
-      <c r="R3" s="269"/>
-      <c r="S3" s="266" t="s">
+      <c r="V3" s="266"/>
+      <c r="W3" s="263" t="s">
         <v>44</v>
       </c>
-      <c r="T3" s="132" t="s">
+      <c r="X3" s="132" t="s">
         <v>45</v>
       </c>
-      <c r="U3" s="137" t="s">
+      <c r="Y3" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="131" t="s">
+      <c r="Z3" s="131" t="s">
         <v>92</v>
       </c>
-      <c r="Z3" s="101"/>
-      <c r="AA3" s="135"/>
-      <c r="AB3" s="162"/>
-      <c r="AC3" s="166"/>
-      <c r="AD3" s="161"/>
-      <c r="AE3" s="163"/>
-      <c r="AF3" s="164"/>
-      <c r="AG3" s="62"/>
-      <c r="AH3" s="165"/>
-      <c r="AI3" s="62"/>
-      <c r="AJ3" s="121"/>
-    </row>
-    <row r="4" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD3" s="101"/>
+      <c r="AE3" s="135"/>
+      <c r="AF3" s="162"/>
+      <c r="AG3" s="166"/>
+      <c r="AH3" s="161"/>
+      <c r="AI3" s="163"/>
+      <c r="AJ3" s="164"/>
+      <c r="AK3" s="62"/>
+      <c r="AL3" s="165"/>
+      <c r="AM3" s="62"/>
+      <c r="AN3" s="121"/>
+    </row>
+    <row r="4" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="128">
         <v>44763</v>
       </c>
@@ -9809,42 +9827,55 @@
       <c r="F4" s="187" t="s">
         <v>104</v>
       </c>
-      <c r="O4" s="255">
+      <c r="G4" s="178">
+        <v>44787</v>
+      </c>
+      <c r="H4" s="215">
+        <v>44793</v>
+      </c>
+      <c r="I4" s="179">
+        <v>71526</v>
+      </c>
+      <c r="J4" s="20">
+        <f>E28+I4</f>
+        <v>1332568</v>
+      </c>
+      <c r="S4" s="252">
         <v>44739</v>
       </c>
-      <c r="P4" s="256" t="s">
+      <c r="T4" s="253" t="s">
         <v>129</v>
       </c>
-      <c r="Q4" s="22">
+      <c r="U4" s="22">
         <v>9215.3700000000008</v>
       </c>
-      <c r="R4" s="269"/>
-      <c r="S4" s="267">
+      <c r="V4" s="266"/>
+      <c r="W4" s="264">
         <v>44720</v>
       </c>
-      <c r="T4" s="133">
+      <c r="X4" s="133">
         <v>44722</v>
       </c>
-      <c r="U4" s="129">
+      <c r="Y4" s="129">
         <v>45730</v>
       </c>
-      <c r="V4" s="129">
-        <f>U4</f>
+      <c r="Z4" s="129">
+        <f>Y4</f>
         <v>45730</v>
       </c>
-      <c r="Z4" s="101"/>
-      <c r="AA4" s="135"/>
-      <c r="AB4" s="60"/>
-      <c r="AC4" s="60"/>
-      <c r="AD4" s="161"/>
-      <c r="AE4" s="163"/>
-      <c r="AF4" s="164"/>
-      <c r="AG4" s="62"/>
-      <c r="AH4" s="165"/>
-      <c r="AI4" s="62"/>
-      <c r="AJ4" s="121"/>
-    </row>
-    <row r="5" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD4" s="101"/>
+      <c r="AE4" s="135"/>
+      <c r="AF4" s="60"/>
+      <c r="AG4" s="60"/>
+      <c r="AH4" s="161"/>
+      <c r="AI4" s="163"/>
+      <c r="AJ4" s="164"/>
+      <c r="AK4" s="62"/>
+      <c r="AL4" s="165"/>
+      <c r="AM4" s="62"/>
+      <c r="AN4" s="121"/>
+    </row>
+    <row r="5" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="128">
         <v>44764</v>
       </c>
@@ -9861,42 +9892,55 @@
       <c r="F5" s="208" t="s">
         <v>104</v>
       </c>
-      <c r="O5" s="255">
+      <c r="G5" s="178">
+        <v>44787</v>
+      </c>
+      <c r="H5" s="215">
+        <v>44798</v>
+      </c>
+      <c r="I5" s="179">
+        <v>500</v>
+      </c>
+      <c r="J5" s="20">
+        <f t="shared" ref="J4:J20" si="0">J4+I5</f>
+        <v>1333068</v>
+      </c>
+      <c r="S5" s="252">
         <v>44740</v>
       </c>
-      <c r="P5" s="256" t="s">
+      <c r="T5" s="253" t="s">
         <v>130</v>
       </c>
-      <c r="Q5" s="22">
+      <c r="U5" s="22">
         <v>96875.6</v>
       </c>
-      <c r="R5" s="269"/>
-      <c r="S5" s="267">
+      <c r="V5" s="266"/>
+      <c r="W5" s="264">
         <v>44721</v>
       </c>
-      <c r="T5" s="134">
+      <c r="X5" s="134">
         <v>44722</v>
       </c>
-      <c r="U5" s="20">
+      <c r="Y5" s="20">
         <v>44700</v>
       </c>
-      <c r="V5" s="20">
-        <f>V4+U5</f>
+      <c r="Z5" s="20">
+        <f>Z4+Y5</f>
         <v>90430</v>
       </c>
-      <c r="Z5" s="101"/>
-      <c r="AA5" s="135"/>
-      <c r="AB5" s="60"/>
-      <c r="AC5" s="60"/>
-      <c r="AD5" s="161"/>
-      <c r="AE5" s="163"/>
-      <c r="AF5" s="164"/>
-      <c r="AG5" s="62"/>
-      <c r="AH5" s="165"/>
-      <c r="AI5" s="62"/>
-      <c r="AJ5" s="121"/>
-    </row>
-    <row r="6" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD5" s="101"/>
+      <c r="AE5" s="135"/>
+      <c r="AF5" s="60"/>
+      <c r="AG5" s="60"/>
+      <c r="AH5" s="161"/>
+      <c r="AI5" s="163"/>
+      <c r="AJ5" s="164"/>
+      <c r="AK5" s="62"/>
+      <c r="AL5" s="165"/>
+      <c r="AM5" s="62"/>
+      <c r="AN5" s="121"/>
+    </row>
+    <row r="6" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="128">
         <v>44765</v>
       </c>
@@ -9907,48 +9951,61 @@
         <v>72303.5</v>
       </c>
       <c r="E6" s="20">
-        <f t="shared" ref="E6:E12" si="0">E5+D6</f>
+        <f t="shared" ref="E6:E12" si="1">E5+D6</f>
         <v>193535.5</v>
       </c>
       <c r="F6" s="208" t="s">
         <v>106</v>
       </c>
-      <c r="O6" s="255">
+      <c r="G6" s="178">
+        <v>44788</v>
+      </c>
+      <c r="H6" s="215">
+        <v>44793</v>
+      </c>
+      <c r="I6" s="179">
+        <v>50554</v>
+      </c>
+      <c r="J6" s="20">
+        <f t="shared" si="0"/>
+        <v>1383622</v>
+      </c>
+      <c r="S6" s="252">
         <v>44741</v>
       </c>
-      <c r="P6" s="256" t="s">
+      <c r="T6" s="253" t="s">
         <v>131</v>
       </c>
-      <c r="Q6" s="22">
+      <c r="U6" s="22">
         <v>26574.6</v>
       </c>
-      <c r="R6" s="269"/>
-      <c r="S6" s="267">
+      <c r="V6" s="266"/>
+      <c r="W6" s="264">
         <v>44722</v>
       </c>
-      <c r="T6" s="134">
+      <c r="X6" s="134">
         <v>44725</v>
       </c>
-      <c r="U6" s="20">
+      <c r="Y6" s="20">
         <v>45943</v>
       </c>
-      <c r="V6" s="20">
-        <f>V5+U6</f>
+      <c r="Z6" s="20">
+        <f>Z5+Y6</f>
         <v>136373</v>
       </c>
-      <c r="Z6" s="101"/>
-      <c r="AA6" s="135"/>
-      <c r="AB6" s="60"/>
-      <c r="AC6" s="60"/>
-      <c r="AD6" s="161"/>
-      <c r="AE6" s="163"/>
-      <c r="AF6" s="164"/>
-      <c r="AG6" s="62"/>
-      <c r="AH6" s="165"/>
-      <c r="AI6" s="62"/>
-      <c r="AJ6" s="121"/>
-    </row>
-    <row r="7" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD6" s="101"/>
+      <c r="AE6" s="135"/>
+      <c r="AF6" s="60"/>
+      <c r="AG6" s="60"/>
+      <c r="AH6" s="161"/>
+      <c r="AI6" s="163"/>
+      <c r="AJ6" s="164"/>
+      <c r="AK6" s="62"/>
+      <c r="AL6" s="165"/>
+      <c r="AM6" s="62"/>
+      <c r="AN6" s="121"/>
+    </row>
+    <row r="7" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="128">
         <v>44766</v>
       </c>
@@ -9959,48 +10016,61 @@
         <v>36105</v>
       </c>
       <c r="E7" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>229640.5</v>
       </c>
       <c r="F7" s="208" t="s">
         <v>106</v>
       </c>
-      <c r="O7" s="255">
+      <c r="G7" s="178">
+        <v>44789</v>
+      </c>
+      <c r="H7" s="215">
+        <v>44793</v>
+      </c>
+      <c r="I7" s="179">
+        <v>22615</v>
+      </c>
+      <c r="J7" s="20">
+        <f t="shared" si="0"/>
+        <v>1406237</v>
+      </c>
+      <c r="S7" s="252">
         <v>44742</v>
       </c>
-      <c r="P7" s="256" t="s">
+      <c r="T7" s="253" t="s">
         <v>132</v>
       </c>
-      <c r="Q7" s="22">
+      <c r="U7" s="22">
         <v>110618.06</v>
       </c>
-      <c r="R7" s="269"/>
-      <c r="S7" s="267">
+      <c r="V7" s="266"/>
+      <c r="W7" s="264">
         <v>44723</v>
       </c>
-      <c r="T7" s="134">
+      <c r="X7" s="134">
         <v>44725</v>
       </c>
-      <c r="U7" s="20">
+      <c r="Y7" s="20">
         <v>16613.5</v>
       </c>
-      <c r="V7" s="20">
-        <f t="shared" ref="V7:V22" si="1">V6+U7</f>
+      <c r="Z7" s="20">
+        <f t="shared" ref="Z7:Z22" si="2">Z6+Y7</f>
         <v>152986.5</v>
       </c>
-      <c r="Z7" s="101"/>
-      <c r="AA7" s="135"/>
-      <c r="AB7" s="60"/>
-      <c r="AC7" s="60"/>
-      <c r="AD7" s="161"/>
-      <c r="AE7" s="163"/>
-      <c r="AF7" s="164"/>
-      <c r="AG7" s="62"/>
-      <c r="AH7" s="165"/>
-      <c r="AI7" s="62"/>
-      <c r="AJ7" s="121"/>
-    </row>
-    <row r="8" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD7" s="101"/>
+      <c r="AE7" s="135"/>
+      <c r="AF7" s="60"/>
+      <c r="AG7" s="60"/>
+      <c r="AH7" s="161"/>
+      <c r="AI7" s="163"/>
+      <c r="AJ7" s="164"/>
+      <c r="AK7" s="62"/>
+      <c r="AL7" s="165"/>
+      <c r="AM7" s="62"/>
+      <c r="AN7" s="121"/>
+    </row>
+    <row r="8" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="128">
         <v>44767</v>
       </c>
@@ -10011,48 +10081,61 @@
         <v>3510</v>
       </c>
       <c r="E8" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>233150.5</v>
       </c>
       <c r="F8" s="208" t="s">
         <v>106</v>
       </c>
-      <c r="O8" s="257">
+      <c r="G8" s="178">
+        <v>44790</v>
+      </c>
+      <c r="H8" s="215">
+        <v>44793</v>
+      </c>
+      <c r="I8" s="184">
+        <v>21525</v>
+      </c>
+      <c r="J8" s="20">
+        <f t="shared" si="0"/>
+        <v>1427762</v>
+      </c>
+      <c r="S8" s="254">
         <v>44742</v>
       </c>
-      <c r="P8" s="258" t="s">
+      <c r="T8" s="255" t="s">
         <v>133</v>
       </c>
-      <c r="Q8" s="22">
+      <c r="U8" s="22">
         <v>3223.2</v>
       </c>
-      <c r="R8" s="269"/>
-      <c r="S8" s="267">
+      <c r="V8" s="266"/>
+      <c r="W8" s="264">
         <v>44724</v>
       </c>
-      <c r="T8" s="134">
+      <c r="X8" s="134">
         <v>44725</v>
       </c>
-      <c r="U8" s="20">
+      <c r="Y8" s="20">
         <v>17154</v>
       </c>
-      <c r="V8" s="20">
-        <f t="shared" si="1"/>
+      <c r="Z8" s="20">
+        <f t="shared" si="2"/>
         <v>170140.5</v>
       </c>
-      <c r="Z8" s="101"/>
-      <c r="AA8" s="135"/>
-      <c r="AB8" s="60"/>
-      <c r="AC8" s="60"/>
-      <c r="AD8" s="161"/>
-      <c r="AE8" s="163"/>
-      <c r="AF8" s="164"/>
-      <c r="AG8" s="62"/>
-      <c r="AH8" s="165"/>
-      <c r="AI8" s="62"/>
-      <c r="AJ8" s="121"/>
-    </row>
-    <row r="9" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD8" s="101"/>
+      <c r="AE8" s="135"/>
+      <c r="AF8" s="60"/>
+      <c r="AG8" s="60"/>
+      <c r="AH8" s="161"/>
+      <c r="AI8" s="163"/>
+      <c r="AJ8" s="164"/>
+      <c r="AK8" s="62"/>
+      <c r="AL8" s="165"/>
+      <c r="AM8" s="62"/>
+      <c r="AN8" s="121"/>
+    </row>
+    <row r="9" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="128">
         <v>44768</v>
       </c>
@@ -10063,48 +10146,61 @@
         <v>17556</v>
       </c>
       <c r="E9" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>250706.5</v>
       </c>
       <c r="F9" s="208" t="s">
         <v>46</v>
       </c>
-      <c r="O9" s="257">
+      <c r="G9" s="178">
+        <v>44791</v>
+      </c>
+      <c r="H9" s="215">
+        <v>44793</v>
+      </c>
+      <c r="I9" s="184">
+        <v>46128.5</v>
+      </c>
+      <c r="J9" s="20">
+        <f t="shared" si="0"/>
+        <v>1473890.5</v>
+      </c>
+      <c r="S9" s="254">
         <v>44743</v>
       </c>
-      <c r="P9" s="258" t="s">
+      <c r="T9" s="255" t="s">
         <v>134</v>
       </c>
-      <c r="Q9" s="22">
+      <c r="U9" s="22">
         <v>65436.19</v>
       </c>
-      <c r="R9" s="269"/>
-      <c r="S9" s="267">
+      <c r="V9" s="266"/>
+      <c r="W9" s="264">
         <v>44725</v>
       </c>
-      <c r="T9" s="134">
+      <c r="X9" s="134">
         <v>44728</v>
       </c>
-      <c r="U9" s="20">
+      <c r="Y9" s="20">
         <v>50350</v>
       </c>
-      <c r="V9" s="20">
-        <f t="shared" si="1"/>
+      <c r="Z9" s="20">
+        <f t="shared" si="2"/>
         <v>220490.5</v>
       </c>
-      <c r="Z9" s="101"/>
-      <c r="AA9" s="135"/>
-      <c r="AB9" s="60"/>
-      <c r="AC9" s="60"/>
-      <c r="AD9" s="161"/>
-      <c r="AE9" s="163"/>
-      <c r="AF9" s="164"/>
-      <c r="AG9" s="62"/>
-      <c r="AH9" s="165"/>
-      <c r="AI9" s="62"/>
-      <c r="AJ9" s="121"/>
-    </row>
-    <row r="10" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD9" s="101"/>
+      <c r="AE9" s="135"/>
+      <c r="AF9" s="60"/>
+      <c r="AG9" s="60"/>
+      <c r="AH9" s="161"/>
+      <c r="AI9" s="163"/>
+      <c r="AJ9" s="164"/>
+      <c r="AK9" s="62"/>
+      <c r="AL9" s="165"/>
+      <c r="AM9" s="62"/>
+      <c r="AN9" s="121"/>
+    </row>
+    <row r="10" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="128">
         <v>44769</v>
       </c>
@@ -10115,48 +10211,61 @@
         <v>41640</v>
       </c>
       <c r="E10" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>292346.5</v>
       </c>
       <c r="F10" s="208" t="s">
         <v>46</v>
       </c>
-      <c r="O10" s="257">
+      <c r="G10" s="178">
+        <v>44792</v>
+      </c>
+      <c r="H10" s="215">
+        <v>44793</v>
+      </c>
+      <c r="I10" s="184">
+        <v>58983.5</v>
+      </c>
+      <c r="J10" s="20">
+        <f t="shared" si="0"/>
+        <v>1532874</v>
+      </c>
+      <c r="S10" s="254">
         <v>44744</v>
       </c>
-      <c r="P10" s="258" t="s">
+      <c r="T10" s="255" t="s">
         <v>135</v>
       </c>
-      <c r="Q10" s="22">
+      <c r="U10" s="22">
         <v>60853.03</v>
       </c>
-      <c r="R10" s="269"/>
-      <c r="S10" s="267">
+      <c r="V10" s="266"/>
+      <c r="W10" s="264">
         <v>44726</v>
       </c>
-      <c r="T10" s="134">
+      <c r="X10" s="134">
         <v>44728</v>
       </c>
-      <c r="U10" s="20">
+      <c r="Y10" s="20">
         <v>44920</v>
       </c>
-      <c r="V10" s="20">
-        <f t="shared" si="1"/>
+      <c r="Z10" s="20">
+        <f t="shared" si="2"/>
         <v>265410.5</v>
       </c>
-      <c r="Z10" s="101"/>
-      <c r="AA10" s="135"/>
-      <c r="AB10" s="60"/>
-      <c r="AC10" s="60"/>
-      <c r="AD10" s="161"/>
-      <c r="AE10" s="163"/>
-      <c r="AF10" s="164"/>
-      <c r="AG10" s="62"/>
-      <c r="AH10" s="165"/>
-      <c r="AI10" s="62"/>
-      <c r="AJ10" s="121"/>
-    </row>
-    <row r="11" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD10" s="101"/>
+      <c r="AE10" s="135"/>
+      <c r="AF10" s="60"/>
+      <c r="AG10" s="60"/>
+      <c r="AH10" s="161"/>
+      <c r="AI10" s="163"/>
+      <c r="AJ10" s="164"/>
+      <c r="AK10" s="62"/>
+      <c r="AL10" s="165"/>
+      <c r="AM10" s="62"/>
+      <c r="AN10" s="121"/>
+    </row>
+    <row r="11" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="128">
         <v>44770</v>
       </c>
@@ -10167,45 +10276,58 @@
         <v>37988.5</v>
       </c>
       <c r="E11" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>330335</v>
       </c>
-      <c r="O11" s="257">
+      <c r="G11" s="178">
+        <v>44793</v>
+      </c>
+      <c r="H11" s="215">
+        <v>44798</v>
+      </c>
+      <c r="I11" s="184">
+        <v>100977</v>
+      </c>
+      <c r="J11" s="20">
+        <f t="shared" si="0"/>
+        <v>1633851</v>
+      </c>
+      <c r="S11" s="254">
         <v>44744</v>
       </c>
-      <c r="P11" s="258" t="s">
+      <c r="T11" s="255" t="s">
         <v>136</v>
       </c>
-      <c r="Q11" s="22">
+      <c r="U11" s="22">
         <v>5205</v>
       </c>
-      <c r="R11" s="269"/>
-      <c r="S11" s="267">
+      <c r="V11" s="266"/>
+      <c r="W11" s="264">
         <v>44727</v>
       </c>
-      <c r="T11" s="134">
+      <c r="X11" s="134">
         <v>44728</v>
       </c>
-      <c r="U11" s="20">
+      <c r="Y11" s="20">
         <v>36290.5</v>
       </c>
-      <c r="V11" s="20">
-        <f t="shared" si="1"/>
+      <c r="Z11" s="20">
+        <f t="shared" si="2"/>
         <v>301701</v>
       </c>
-      <c r="Z11" s="101"/>
-      <c r="AA11" s="135"/>
-      <c r="AB11" s="60"/>
-      <c r="AC11" s="60"/>
-      <c r="AD11" s="161"/>
-      <c r="AE11" s="163"/>
-      <c r="AF11" s="164"/>
-      <c r="AG11" s="62"/>
-      <c r="AH11" s="165"/>
-      <c r="AI11" s="62"/>
-      <c r="AJ11" s="121"/>
-    </row>
-    <row r="12" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD11" s="101"/>
+      <c r="AE11" s="135"/>
+      <c r="AF11" s="60"/>
+      <c r="AG11" s="60"/>
+      <c r="AH11" s="161"/>
+      <c r="AI11" s="163"/>
+      <c r="AJ11" s="164"/>
+      <c r="AK11" s="62"/>
+      <c r="AL11" s="165"/>
+      <c r="AM11" s="62"/>
+      <c r="AN11" s="121"/>
+    </row>
+    <row r="12" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="128">
         <v>44771</v>
       </c>
@@ -10216,45 +10338,58 @@
         <v>56000</v>
       </c>
       <c r="E12" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>386335</v>
       </c>
-      <c r="O12" s="255">
+      <c r="G12" s="178">
+        <v>44794</v>
+      </c>
+      <c r="H12" s="215">
+        <v>44798</v>
+      </c>
+      <c r="I12" s="184">
+        <v>53500.5</v>
+      </c>
+      <c r="J12" s="20">
+        <f t="shared" si="0"/>
+        <v>1687351.5</v>
+      </c>
+      <c r="S12" s="252">
         <v>44746</v>
       </c>
-      <c r="P12" s="256" t="s">
+      <c r="T12" s="253" t="s">
         <v>137</v>
       </c>
-      <c r="Q12" s="22">
+      <c r="U12" s="22">
         <v>67911.399999999994</v>
       </c>
-      <c r="R12" s="269"/>
-      <c r="S12" s="267">
+      <c r="V12" s="266"/>
+      <c r="W12" s="264">
         <v>44728</v>
       </c>
-      <c r="T12" s="134">
+      <c r="X12" s="134">
         <v>44732</v>
       </c>
-      <c r="U12" s="20">
+      <c r="Y12" s="20">
         <v>49576</v>
       </c>
-      <c r="V12" s="20">
-        <f t="shared" si="1"/>
+      <c r="Z12" s="20">
+        <f t="shared" si="2"/>
         <v>351277</v>
       </c>
-      <c r="Z12" s="101"/>
-      <c r="AA12" s="135"/>
-      <c r="AB12" s="60"/>
-      <c r="AC12" s="60"/>
-      <c r="AD12" s="161"/>
-      <c r="AE12" s="163"/>
-      <c r="AF12" s="164"/>
-      <c r="AG12" s="62"/>
-      <c r="AH12" s="165"/>
-      <c r="AI12" s="62"/>
-      <c r="AJ12" s="121"/>
-    </row>
-    <row r="13" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD12" s="101"/>
+      <c r="AE12" s="135"/>
+      <c r="AF12" s="60"/>
+      <c r="AG12" s="60"/>
+      <c r="AH12" s="161"/>
+      <c r="AI12" s="163"/>
+      <c r="AJ12" s="164"/>
+      <c r="AK12" s="62"/>
+      <c r="AL12" s="165"/>
+      <c r="AM12" s="62"/>
+      <c r="AN12" s="121"/>
+    </row>
+    <row r="13" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="128">
         <v>44772</v>
       </c>
@@ -10265,45 +10400,58 @@
         <v>50983</v>
       </c>
       <c r="E13" s="20">
-        <f t="shared" ref="E13:E45" si="2">E12+D13</f>
+        <f t="shared" ref="E13:E45" si="3">E12+D13</f>
         <v>437318</v>
       </c>
-      <c r="O13" s="255">
+      <c r="G13" s="178">
+        <v>44795</v>
+      </c>
+      <c r="H13" s="215">
+        <v>44798</v>
+      </c>
+      <c r="I13" s="184">
+        <v>23209.5</v>
+      </c>
+      <c r="J13" s="20">
+        <f t="shared" si="0"/>
+        <v>1710561</v>
+      </c>
+      <c r="S13" s="252">
         <v>44746</v>
       </c>
-      <c r="P13" s="256" t="s">
+      <c r="T13" s="253" t="s">
         <v>138</v>
       </c>
-      <c r="Q13" s="22">
+      <c r="U13" s="22">
         <v>73363.8</v>
       </c>
-      <c r="R13" s="269"/>
-      <c r="S13" s="267">
+      <c r="V13" s="266"/>
+      <c r="W13" s="264">
         <v>44729</v>
       </c>
-      <c r="T13" s="134">
+      <c r="X13" s="134">
         <v>44732</v>
       </c>
-      <c r="U13" s="22">
+      <c r="Y13" s="22">
         <v>48123</v>
       </c>
-      <c r="V13" s="20">
-        <f t="shared" si="1"/>
+      <c r="Z13" s="20">
+        <f t="shared" si="2"/>
         <v>399400</v>
       </c>
-      <c r="Z13" s="101"/>
-      <c r="AA13" s="135"/>
-      <c r="AB13" s="62"/>
-      <c r="AC13" s="60"/>
-      <c r="AD13" s="161"/>
-      <c r="AE13" s="163"/>
-      <c r="AF13" s="164"/>
-      <c r="AG13" s="62"/>
-      <c r="AH13" s="165"/>
-      <c r="AI13" s="62"/>
-      <c r="AJ13" s="121"/>
-    </row>
-    <row r="14" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD13" s="101"/>
+      <c r="AE13" s="135"/>
+      <c r="AF13" s="62"/>
+      <c r="AG13" s="60"/>
+      <c r="AH13" s="161"/>
+      <c r="AI13" s="163"/>
+      <c r="AJ13" s="164"/>
+      <c r="AK13" s="62"/>
+      <c r="AL13" s="165"/>
+      <c r="AM13" s="62"/>
+      <c r="AN13" s="121"/>
+    </row>
+    <row r="14" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="128">
         <v>44773</v>
       </c>
@@ -10314,45 +10462,58 @@
         <v>46721</v>
       </c>
       <c r="E14" s="20">
+        <f t="shared" si="3"/>
+        <v>484039</v>
+      </c>
+      <c r="G14" s="178">
+        <v>44704</v>
+      </c>
+      <c r="H14" s="215">
+        <v>44798</v>
+      </c>
+      <c r="I14" s="184">
+        <v>10000</v>
+      </c>
+      <c r="J14" s="20">
+        <f t="shared" si="0"/>
+        <v>1720561</v>
+      </c>
+      <c r="S14" s="252">
+        <v>44747</v>
+      </c>
+      <c r="T14" s="253" t="s">
+        <v>139</v>
+      </c>
+      <c r="U14" s="22">
+        <v>31164.35</v>
+      </c>
+      <c r="V14" s="266"/>
+      <c r="W14" s="264">
+        <v>44730</v>
+      </c>
+      <c r="X14" s="134">
+        <v>44732</v>
+      </c>
+      <c r="Y14" s="20">
+        <v>66300</v>
+      </c>
+      <c r="Z14" s="20">
         <f t="shared" si="2"/>
-        <v>484039</v>
-      </c>
-      <c r="O14" s="255">
-        <v>44747</v>
-      </c>
-      <c r="P14" s="256" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q14" s="22">
-        <v>31164.35</v>
-      </c>
-      <c r="R14" s="269"/>
-      <c r="S14" s="267">
-        <v>44730</v>
-      </c>
-      <c r="T14" s="134">
-        <v>44732</v>
-      </c>
-      <c r="U14" s="20">
-        <v>66300</v>
-      </c>
-      <c r="V14" s="20">
-        <f t="shared" si="1"/>
         <v>465700</v>
       </c>
-      <c r="Z14" s="101"/>
-      <c r="AA14" s="135"/>
-      <c r="AB14" s="60"/>
-      <c r="AC14" s="60"/>
-      <c r="AD14" s="161"/>
-      <c r="AE14" s="163"/>
-      <c r="AF14" s="164"/>
-      <c r="AG14" s="62"/>
-      <c r="AH14" s="165"/>
-      <c r="AI14" s="62"/>
-      <c r="AJ14" s="121"/>
-    </row>
-    <row r="15" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD14" s="101"/>
+      <c r="AE14" s="135"/>
+      <c r="AF14" s="60"/>
+      <c r="AG14" s="60"/>
+      <c r="AH14" s="161"/>
+      <c r="AI14" s="163"/>
+      <c r="AJ14" s="164"/>
+      <c r="AK14" s="62"/>
+      <c r="AL14" s="165"/>
+      <c r="AM14" s="62"/>
+      <c r="AN14" s="121"/>
+    </row>
+    <row r="15" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="128">
         <v>44774</v>
       </c>
@@ -10363,45 +10524,58 @@
         <v>79607</v>
       </c>
       <c r="E15" s="20">
+        <f t="shared" si="3"/>
+        <v>563646</v>
+      </c>
+      <c r="G15" s="178">
+        <v>44797</v>
+      </c>
+      <c r="H15" s="215">
+        <v>44798</v>
+      </c>
+      <c r="I15" s="184">
+        <v>63665</v>
+      </c>
+      <c r="J15" s="20">
+        <f t="shared" si="0"/>
+        <v>1784226</v>
+      </c>
+      <c r="S15" s="252">
+        <v>44748</v>
+      </c>
+      <c r="T15" s="253" t="s">
+        <v>140</v>
+      </c>
+      <c r="U15" s="22">
+        <v>58616</v>
+      </c>
+      <c r="V15" s="266"/>
+      <c r="W15" s="264">
+        <v>44731</v>
+      </c>
+      <c r="X15" s="134">
+        <v>44732</v>
+      </c>
+      <c r="Y15" s="20">
+        <v>75117</v>
+      </c>
+      <c r="Z15" s="20">
         <f t="shared" si="2"/>
-        <v>563646</v>
-      </c>
-      <c r="O15" s="255">
-        <v>44748</v>
-      </c>
-      <c r="P15" s="256" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q15" s="22">
-        <v>58616</v>
-      </c>
-      <c r="R15" s="269"/>
-      <c r="S15" s="267">
-        <v>44731</v>
-      </c>
-      <c r="T15" s="134">
-        <v>44732</v>
-      </c>
-      <c r="U15" s="20">
-        <v>75117</v>
-      </c>
-      <c r="V15" s="20">
-        <f t="shared" si="1"/>
         <v>540817</v>
       </c>
-      <c r="Z15" s="101"/>
-      <c r="AA15" s="135"/>
-      <c r="AB15" s="60"/>
-      <c r="AC15" s="60"/>
-      <c r="AD15" s="161"/>
-      <c r="AE15" s="163"/>
-      <c r="AF15" s="164"/>
-      <c r="AG15" s="62"/>
-      <c r="AH15" s="165"/>
-      <c r="AI15" s="62"/>
-      <c r="AJ15" s="121"/>
-    </row>
-    <row r="16" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD15" s="101"/>
+      <c r="AE15" s="135"/>
+      <c r="AF15" s="60"/>
+      <c r="AG15" s="60"/>
+      <c r="AH15" s="161"/>
+      <c r="AI15" s="163"/>
+      <c r="AJ15" s="164"/>
+      <c r="AK15" s="62"/>
+      <c r="AL15" s="165"/>
+      <c r="AM15" s="62"/>
+      <c r="AN15" s="121"/>
+    </row>
+    <row r="16" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="128">
         <v>44775</v>
       </c>
@@ -10412,39 +10586,52 @@
         <v>64513</v>
       </c>
       <c r="E16" s="20">
+        <f t="shared" si="3"/>
+        <v>628159</v>
+      </c>
+      <c r="G16" s="178">
+        <v>44798</v>
+      </c>
+      <c r="H16" s="215">
+        <v>44798</v>
+      </c>
+      <c r="I16" s="184">
+        <v>14701</v>
+      </c>
+      <c r="J16" s="20">
+        <f t="shared" si="0"/>
+        <v>1798927</v>
+      </c>
+      <c r="S16" s="252">
+        <v>44749</v>
+      </c>
+      <c r="T16" s="253" t="s">
+        <v>141</v>
+      </c>
+      <c r="U16" s="22">
+        <v>106705.96</v>
+      </c>
+      <c r="V16" s="266"/>
+      <c r="W16" s="264"/>
+      <c r="X16" s="134"/>
+      <c r="Y16" s="20"/>
+      <c r="Z16" s="20">
         <f t="shared" si="2"/>
-        <v>628159</v>
-      </c>
-      <c r="O16" s="255">
-        <v>44749</v>
-      </c>
-      <c r="P16" s="256" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q16" s="22">
-        <v>106705.96</v>
-      </c>
-      <c r="R16" s="269"/>
-      <c r="S16" s="267"/>
-      <c r="T16" s="134"/>
-      <c r="U16" s="20"/>
-      <c r="V16" s="20">
-        <f t="shared" si="1"/>
         <v>540817</v>
       </c>
-      <c r="Z16" s="101"/>
-      <c r="AA16" s="135"/>
-      <c r="AB16" s="60"/>
-      <c r="AC16" s="60"/>
-      <c r="AD16" s="161"/>
-      <c r="AE16" s="163"/>
-      <c r="AF16" s="164"/>
-      <c r="AG16" s="62"/>
-      <c r="AH16" s="165"/>
-      <c r="AI16" s="62"/>
-      <c r="AJ16" s="121"/>
-    </row>
-    <row r="17" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD16" s="101"/>
+      <c r="AE16" s="135"/>
+      <c r="AF16" s="60"/>
+      <c r="AG16" s="60"/>
+      <c r="AH16" s="161"/>
+      <c r="AI16" s="163"/>
+      <c r="AJ16" s="164"/>
+      <c r="AK16" s="62"/>
+      <c r="AL16" s="165"/>
+      <c r="AM16" s="62"/>
+      <c r="AN16" s="121"/>
+    </row>
+    <row r="17" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="128">
         <v>44776</v>
       </c>
@@ -10455,41 +10642,48 @@
         <v>45403</v>
       </c>
       <c r="E17" s="20">
+        <f t="shared" si="3"/>
+        <v>673562</v>
+      </c>
+      <c r="G17" s="178"/>
+      <c r="H17" s="215"/>
+      <c r="I17" s="184"/>
+      <c r="J17" s="20">
+        <f t="shared" si="0"/>
+        <v>1798927</v>
+      </c>
+      <c r="S17" s="252">
+        <v>44750</v>
+      </c>
+      <c r="T17" s="253" t="s">
+        <v>142</v>
+      </c>
+      <c r="U17" s="22">
+        <v>68357.89</v>
+      </c>
+      <c r="V17" s="266"/>
+      <c r="W17" s="264"/>
+      <c r="X17" s="134"/>
+      <c r="Y17" s="20">
+        <v>-529362.74</v>
+      </c>
+      <c r="Z17" s="20">
         <f t="shared" si="2"/>
-        <v>673562</v>
-      </c>
-      <c r="O17" s="255">
-        <v>44750</v>
-      </c>
-      <c r="P17" s="256" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q17" s="22">
-        <v>68357.89</v>
-      </c>
-      <c r="R17" s="269"/>
-      <c r="S17" s="267"/>
-      <c r="T17" s="134"/>
-      <c r="U17" s="20">
-        <v>-529362.74</v>
-      </c>
-      <c r="V17" s="20">
-        <f t="shared" si="1"/>
         <v>11454.260000000009</v>
       </c>
-      <c r="Z17" s="101"/>
-      <c r="AA17" s="135"/>
-      <c r="AB17" s="60"/>
-      <c r="AC17" s="60"/>
-      <c r="AD17" s="161"/>
-      <c r="AE17" s="163"/>
-      <c r="AF17" s="164"/>
-      <c r="AG17" s="62"/>
-      <c r="AH17" s="165"/>
-      <c r="AI17" s="62"/>
-      <c r="AJ17" s="121"/>
-    </row>
-    <row r="18" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD17" s="101"/>
+      <c r="AE17" s="135"/>
+      <c r="AF17" s="60"/>
+      <c r="AG17" s="60"/>
+      <c r="AH17" s="161"/>
+      <c r="AI17" s="163"/>
+      <c r="AJ17" s="164"/>
+      <c r="AK17" s="62"/>
+      <c r="AL17" s="165"/>
+      <c r="AM17" s="62"/>
+      <c r="AN17" s="121"/>
+    </row>
+    <row r="18" spans="2:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="128">
         <v>44777</v>
       </c>
@@ -10500,39 +10694,46 @@
         <v>156941</v>
       </c>
       <c r="E18" s="20">
+        <f t="shared" si="3"/>
+        <v>830503</v>
+      </c>
+      <c r="G18" s="178"/>
+      <c r="H18" s="177"/>
+      <c r="I18" s="182"/>
+      <c r="J18" s="20">
+        <f t="shared" si="0"/>
+        <v>1798927</v>
+      </c>
+      <c r="S18" s="252">
+        <v>44751</v>
+      </c>
+      <c r="T18" s="253" t="s">
+        <v>143</v>
+      </c>
+      <c r="U18" s="22">
+        <v>39927.050000000003</v>
+      </c>
+      <c r="V18" s="266"/>
+      <c r="W18" s="264"/>
+      <c r="X18" s="134"/>
+      <c r="Y18" s="20"/>
+      <c r="Z18" s="20">
         <f t="shared" si="2"/>
-        <v>830503</v>
-      </c>
-      <c r="O18" s="255">
-        <v>44751</v>
-      </c>
-      <c r="P18" s="256" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q18" s="22">
-        <v>39927.050000000003</v>
-      </c>
-      <c r="R18" s="269"/>
-      <c r="S18" s="267"/>
-      <c r="T18" s="134"/>
-      <c r="U18" s="20"/>
-      <c r="V18" s="20">
-        <f t="shared" si="1"/>
         <v>11454.260000000009</v>
       </c>
-      <c r="Z18" s="101"/>
-      <c r="AA18" s="135"/>
-      <c r="AB18" s="60"/>
-      <c r="AC18" s="167"/>
-      <c r="AD18" s="161"/>
-      <c r="AE18" s="163"/>
-      <c r="AF18" s="164"/>
-      <c r="AG18" s="62"/>
-      <c r="AH18" s="165"/>
-      <c r="AI18" s="62"/>
-      <c r="AJ18" s="121"/>
-    </row>
-    <row r="19" spans="2:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD18" s="101"/>
+      <c r="AE18" s="135"/>
+      <c r="AF18" s="60"/>
+      <c r="AG18" s="167"/>
+      <c r="AH18" s="161"/>
+      <c r="AI18" s="163"/>
+      <c r="AJ18" s="164"/>
+      <c r="AK18" s="62"/>
+      <c r="AL18" s="165"/>
+      <c r="AM18" s="62"/>
+      <c r="AN18" s="121"/>
+    </row>
+    <row r="19" spans="2:40" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="128">
         <v>44778</v>
       </c>
@@ -10543,42 +10744,55 @@
         <v>72825</v>
       </c>
       <c r="E19" s="20">
+        <f t="shared" si="3"/>
+        <v>903328</v>
+      </c>
+      <c r="F19" s="185"/>
+      <c r="G19" s="186" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="175" t="s">
+        <v>96</v>
+      </c>
+      <c r="I19" s="174">
+        <v>-1798927.83</v>
+      </c>
+      <c r="J19" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.83000000007450581</v>
+      </c>
+      <c r="S19" s="252">
+        <v>44753</v>
+      </c>
+      <c r="T19" s="253" t="s">
+        <v>144</v>
+      </c>
+      <c r="U19" s="22">
+        <v>121513</v>
+      </c>
+      <c r="V19" s="266"/>
+      <c r="W19" s="264"/>
+      <c r="X19" s="282" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y19" s="283"/>
+      <c r="Z19" s="77">
         <f t="shared" si="2"/>
-        <v>903328</v>
-      </c>
-      <c r="F19" s="185"/>
-      <c r="O19" s="255">
-        <v>44753</v>
-      </c>
-      <c r="P19" s="256" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q19" s="22">
-        <v>121513</v>
-      </c>
-      <c r="R19" s="269"/>
-      <c r="S19" s="267"/>
-      <c r="T19" s="286" t="s">
-        <v>95</v>
-      </c>
-      <c r="U19" s="287"/>
-      <c r="V19" s="77">
-        <f t="shared" si="1"/>
         <v>11454.260000000009</v>
       </c>
-      <c r="Z19" s="101"/>
-      <c r="AA19" s="135"/>
-      <c r="AB19" s="60"/>
-      <c r="AC19" s="60"/>
-      <c r="AD19" s="161"/>
-      <c r="AE19" s="163"/>
-      <c r="AF19" s="164"/>
-      <c r="AG19" s="62"/>
-      <c r="AH19" s="165"/>
-      <c r="AI19" s="62"/>
-      <c r="AJ19" s="121"/>
-    </row>
-    <row r="20" spans="2:36" ht="21" x14ac:dyDescent="0.35">
+      <c r="AD19" s="101"/>
+      <c r="AE19" s="135"/>
+      <c r="AF19" s="60"/>
+      <c r="AG19" s="60"/>
+      <c r="AH19" s="161"/>
+      <c r="AI19" s="163"/>
+      <c r="AJ19" s="164"/>
+      <c r="AK19" s="62"/>
+      <c r="AL19" s="165"/>
+      <c r="AM19" s="62"/>
+      <c r="AN19" s="121"/>
+    </row>
+    <row r="20" spans="2:40" ht="21" x14ac:dyDescent="0.35">
       <c r="B20" s="128">
         <v>44778</v>
       </c>
@@ -10589,42 +10803,51 @@
         <v>500</v>
       </c>
       <c r="E20" s="20">
+        <f t="shared" si="3"/>
+        <v>903828</v>
+      </c>
+      <c r="G20" s="293" t="s">
+        <v>159</v>
+      </c>
+      <c r="H20" s="294"/>
+      <c r="I20" s="295"/>
+      <c r="J20" s="183">
+        <f t="shared" si="0"/>
+        <v>-0.83000000007450581</v>
+      </c>
+      <c r="S20" s="252">
+        <v>44754</v>
+      </c>
+      <c r="T20" s="253" t="s">
+        <v>145</v>
+      </c>
+      <c r="U20" s="22">
+        <v>60297.8</v>
+      </c>
+      <c r="V20" s="266"/>
+      <c r="W20" s="264"/>
+      <c r="X20" s="134"/>
+      <c r="Y20" s="20"/>
+      <c r="Z20" s="20">
         <f t="shared" si="2"/>
-        <v>903828</v>
-      </c>
-      <c r="O20" s="255">
-        <v>44754</v>
-      </c>
-      <c r="P20" s="256" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q20" s="22">
-        <v>60297.8</v>
-      </c>
-      <c r="R20" s="269"/>
-      <c r="S20" s="267"/>
-      <c r="T20" s="134"/>
-      <c r="U20" s="20"/>
-      <c r="V20" s="20">
-        <f t="shared" si="1"/>
         <v>11454.260000000009</v>
       </c>
-      <c r="W20" s="121"/>
-      <c r="X20" s="121"/>
-      <c r="Y20" s="121"/>
-      <c r="Z20" s="168"/>
-      <c r="AA20" s="135"/>
-      <c r="AB20" s="60"/>
-      <c r="AC20" s="60"/>
-      <c r="AD20" s="161"/>
-      <c r="AE20" s="163"/>
-      <c r="AF20" s="164"/>
-      <c r="AG20" s="62"/>
-      <c r="AH20" s="165"/>
-      <c r="AI20" s="62"/>
-      <c r="AJ20" s="121"/>
-    </row>
-    <row r="21" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AA20" s="121"/>
+      <c r="AB20" s="121"/>
+      <c r="AC20" s="121"/>
+      <c r="AD20" s="168"/>
+      <c r="AE20" s="135"/>
+      <c r="AF20" s="60"/>
+      <c r="AG20" s="60"/>
+      <c r="AH20" s="161"/>
+      <c r="AI20" s="163"/>
+      <c r="AJ20" s="164"/>
+      <c r="AK20" s="62"/>
+      <c r="AL20" s="165"/>
+      <c r="AM20" s="62"/>
+      <c r="AN20" s="121"/>
+    </row>
+    <row r="21" spans="2:40" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="128">
         <v>44779</v>
       </c>
@@ -10635,42 +10858,46 @@
         <v>33319</v>
       </c>
       <c r="E21" s="20">
+        <f t="shared" si="3"/>
+        <v>937147</v>
+      </c>
+      <c r="G21" s="296"/>
+      <c r="H21" s="297"/>
+      <c r="I21" s="298"/>
+      <c r="J21" s="114"/>
+      <c r="S21" s="252">
+        <v>44755</v>
+      </c>
+      <c r="T21" s="253" t="s">
+        <v>146</v>
+      </c>
+      <c r="U21" s="22">
+        <v>105453.7</v>
+      </c>
+      <c r="V21" s="266"/>
+      <c r="W21" s="264"/>
+      <c r="X21" s="134"/>
+      <c r="Y21" s="20"/>
+      <c r="Z21" s="20">
         <f t="shared" si="2"/>
-        <v>937147</v>
-      </c>
-      <c r="O21" s="255">
-        <v>44755</v>
-      </c>
-      <c r="P21" s="256" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q21" s="22">
-        <v>105453.7</v>
-      </c>
-      <c r="R21" s="269"/>
-      <c r="S21" s="267"/>
-      <c r="T21" s="134"/>
-      <c r="U21" s="20"/>
-      <c r="V21" s="20">
-        <f t="shared" si="1"/>
         <v>11454.260000000009</v>
       </c>
-      <c r="W21" s="121"/>
-      <c r="X21" s="121"/>
-      <c r="Y21" s="121"/>
-      <c r="Z21" s="101"/>
-      <c r="AA21" s="135"/>
-      <c r="AB21" s="60"/>
-      <c r="AC21" s="60"/>
-      <c r="AD21" s="161"/>
-      <c r="AE21" s="163"/>
-      <c r="AF21" s="164"/>
-      <c r="AG21" s="62"/>
-      <c r="AH21" s="165"/>
-      <c r="AI21" s="62"/>
-      <c r="AJ21" s="121"/>
-    </row>
-    <row r="22" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AA21" s="121"/>
+      <c r="AB21" s="121"/>
+      <c r="AC21" s="121"/>
+      <c r="AD21" s="101"/>
+      <c r="AE21" s="135"/>
+      <c r="AF21" s="60"/>
+      <c r="AG21" s="60"/>
+      <c r="AH21" s="161"/>
+      <c r="AI21" s="163"/>
+      <c r="AJ21" s="164"/>
+      <c r="AK21" s="62"/>
+      <c r="AL21" s="165"/>
+      <c r="AM21" s="62"/>
+      <c r="AN21" s="121"/>
+    </row>
+    <row r="22" spans="2:40" x14ac:dyDescent="0.3">
       <c r="B22" s="128">
         <v>44780</v>
       </c>
@@ -10681,42 +10908,42 @@
         <v>44630</v>
       </c>
       <c r="E22" s="20">
+        <f t="shared" si="3"/>
+        <v>981777</v>
+      </c>
+      <c r="S22" s="252">
+        <v>44756</v>
+      </c>
+      <c r="T22" s="253" t="s">
+        <v>147</v>
+      </c>
+      <c r="U22" s="22">
+        <v>65012.85</v>
+      </c>
+      <c r="V22" s="266"/>
+      <c r="W22" s="264"/>
+      <c r="X22" s="134"/>
+      <c r="Y22" s="20"/>
+      <c r="Z22" s="157">
         <f t="shared" si="2"/>
-        <v>981777</v>
-      </c>
-      <c r="O22" s="255">
-        <v>44756</v>
-      </c>
-      <c r="P22" s="256" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q22" s="22">
-        <v>65012.85</v>
-      </c>
-      <c r="R22" s="269"/>
-      <c r="S22" s="267"/>
-      <c r="T22" s="134"/>
-      <c r="U22" s="20"/>
-      <c r="V22" s="157">
-        <f t="shared" si="1"/>
         <v>11454.260000000009</v>
       </c>
-      <c r="W22" s="121"/>
-      <c r="X22" s="121"/>
-      <c r="Y22" s="121"/>
-      <c r="Z22" s="101"/>
-      <c r="AA22" s="135"/>
-      <c r="AB22" s="60"/>
-      <c r="AC22" s="60"/>
-      <c r="AD22" s="161"/>
-      <c r="AE22" s="163"/>
-      <c r="AF22" s="164"/>
-      <c r="AG22" s="62"/>
-      <c r="AH22" s="165"/>
-      <c r="AI22" s="62"/>
-      <c r="AJ22" s="127"/>
-    </row>
-    <row r="23" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AA22" s="121"/>
+      <c r="AB22" s="121"/>
+      <c r="AC22" s="121"/>
+      <c r="AD22" s="101"/>
+      <c r="AE22" s="135"/>
+      <c r="AF22" s="60"/>
+      <c r="AG22" s="60"/>
+      <c r="AH22" s="161"/>
+      <c r="AI22" s="163"/>
+      <c r="AJ22" s="164"/>
+      <c r="AK22" s="62"/>
+      <c r="AL22" s="165"/>
+      <c r="AM22" s="62"/>
+      <c r="AN22" s="127"/>
+    </row>
+    <row r="23" spans="2:40" x14ac:dyDescent="0.3">
       <c r="B23" s="128">
         <v>44781</v>
       </c>
@@ -10727,39 +10954,39 @@
         <v>47182</v>
       </c>
       <c r="E23" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1028959</v>
       </c>
-      <c r="O23" s="255">
+      <c r="S23" s="252">
         <v>44757</v>
       </c>
-      <c r="P23" s="256" t="s">
+      <c r="T23" s="253" t="s">
         <v>148</v>
       </c>
-      <c r="Q23" s="22">
+      <c r="U23" s="22">
         <v>83843.7</v>
       </c>
-      <c r="R23" s="269"/>
-      <c r="S23" s="267"/>
-      <c r="T23" s="134"/>
-      <c r="U23" s="20"/>
-      <c r="V23" s="20"/>
-      <c r="W23" s="121"/>
-      <c r="X23" s="121"/>
-      <c r="Y23" s="121"/>
-      <c r="Z23" s="101"/>
-      <c r="AA23" s="135"/>
-      <c r="AB23" s="60"/>
-      <c r="AC23" s="60"/>
-      <c r="AD23" s="161"/>
-      <c r="AE23" s="121"/>
-      <c r="AF23" s="121"/>
-      <c r="AG23" s="121"/>
-      <c r="AH23" s="121"/>
-      <c r="AI23" s="169"/>
+      <c r="V23" s="266"/>
+      <c r="W23" s="264"/>
+      <c r="X23" s="134"/>
+      <c r="Y23" s="20"/>
+      <c r="Z23" s="20"/>
+      <c r="AA23" s="121"/>
+      <c r="AB23" s="121"/>
+      <c r="AC23" s="121"/>
+      <c r="AD23" s="101"/>
+      <c r="AE23" s="135"/>
+      <c r="AF23" s="60"/>
+      <c r="AG23" s="60"/>
+      <c r="AH23" s="161"/>
+      <c r="AI23" s="121"/>
       <c r="AJ23" s="121"/>
-    </row>
-    <row r="24" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AK23" s="121"/>
+      <c r="AL23" s="121"/>
+      <c r="AM23" s="169"/>
+      <c r="AN23" s="121"/>
+    </row>
+    <row r="24" spans="2:40" x14ac:dyDescent="0.3">
       <c r="B24" s="128">
         <v>44782</v>
       </c>
@@ -10770,39 +10997,39 @@
         <v>54684</v>
       </c>
       <c r="E24" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1083643</v>
       </c>
-      <c r="O24" s="255">
+      <c r="S24" s="252">
         <v>44757</v>
       </c>
-      <c r="P24" s="256" t="s">
+      <c r="T24" s="253" t="s">
         <v>149</v>
       </c>
-      <c r="Q24" s="22">
+      <c r="U24" s="22">
         <v>11248</v>
       </c>
-      <c r="R24" s="269"/>
-      <c r="S24" s="267"/>
-      <c r="T24" s="134"/>
-      <c r="U24" s="20"/>
-      <c r="V24" s="20"/>
-      <c r="W24" s="121"/>
-      <c r="X24" s="121"/>
-      <c r="Y24" s="121"/>
-      <c r="Z24" s="101"/>
-      <c r="AA24" s="135"/>
-      <c r="AB24" s="60"/>
-      <c r="AC24" s="60"/>
-      <c r="AD24" s="161"/>
-      <c r="AE24" s="121"/>
-      <c r="AF24" s="121"/>
-      <c r="AG24" s="121"/>
-      <c r="AH24" s="121"/>
+      <c r="V24" s="266"/>
+      <c r="W24" s="264"/>
+      <c r="X24" s="134"/>
+      <c r="Y24" s="20"/>
+      <c r="Z24" s="20"/>
+      <c r="AA24" s="121"/>
+      <c r="AB24" s="121"/>
+      <c r="AC24" s="121"/>
+      <c r="AD24" s="101"/>
+      <c r="AE24" s="135"/>
+      <c r="AF24" s="60"/>
+      <c r="AG24" s="60"/>
+      <c r="AH24" s="161"/>
       <c r="AI24" s="121"/>
       <c r="AJ24" s="121"/>
-    </row>
-    <row r="25" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AK24" s="121"/>
+      <c r="AL24" s="121"/>
+      <c r="AM24" s="121"/>
+      <c r="AN24" s="121"/>
+    </row>
+    <row r="25" spans="2:40" x14ac:dyDescent="0.3">
       <c r="B25" s="176">
         <v>44783</v>
       </c>
@@ -10813,32 +11040,32 @@
         <v>40412</v>
       </c>
       <c r="E25" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1124055</v>
       </c>
-      <c r="O25" s="255">
+      <c r="S25" s="252">
         <v>44758</v>
       </c>
-      <c r="P25" s="256" t="s">
+      <c r="T25" s="253" t="s">
         <v>150</v>
       </c>
-      <c r="Q25" s="22">
+      <c r="U25" s="22">
         <v>30498.9</v>
       </c>
-      <c r="R25" s="269"/>
-      <c r="S25" s="267"/>
-      <c r="T25" s="134"/>
-      <c r="U25" s="20"/>
-      <c r="V25" s="22"/>
-      <c r="W25" s="121"/>
-      <c r="X25" s="121"/>
-      <c r="Y25" s="121"/>
-      <c r="Z25" s="101"/>
-      <c r="AA25" s="135"/>
-      <c r="AB25" s="60"/>
-      <c r="AC25" s="60"/>
-    </row>
-    <row r="26" spans="2:36" ht="21" x14ac:dyDescent="0.35">
+      <c r="V25" s="266"/>
+      <c r="W25" s="264"/>
+      <c r="X25" s="134"/>
+      <c r="Y25" s="20"/>
+      <c r="Z25" s="22"/>
+      <c r="AA25" s="121"/>
+      <c r="AB25" s="121"/>
+      <c r="AC25" s="121"/>
+      <c r="AD25" s="101"/>
+      <c r="AE25" s="135"/>
+      <c r="AF25" s="60"/>
+      <c r="AG25" s="60"/>
+    </row>
+    <row r="26" spans="2:40" ht="21" x14ac:dyDescent="0.35">
       <c r="B26" s="178">
         <v>44784</v>
       </c>
@@ -10849,23 +11076,19 @@
         <v>48105</v>
       </c>
       <c r="E26" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1172160</v>
       </c>
-      <c r="O26" s="255">
+      <c r="S26" s="252">
         <v>44758</v>
       </c>
-      <c r="P26" s="256" t="s">
+      <c r="T26" s="253" t="s">
         <v>151</v>
       </c>
-      <c r="Q26" s="22">
+      <c r="U26" s="22">
         <v>4920</v>
       </c>
-      <c r="R26" s="269"/>
-      <c r="S26" s="154"/>
-      <c r="T26" s="154"/>
-      <c r="U26" s="154"/>
-      <c r="V26" s="154"/>
+      <c r="V26" s="266"/>
       <c r="W26" s="154"/>
       <c r="X26" s="154"/>
       <c r="Y26" s="154"/>
@@ -10873,8 +11096,12 @@
       <c r="AA26" s="154"/>
       <c r="AB26" s="154"/>
       <c r="AC26" s="154"/>
-    </row>
-    <row r="27" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AD26" s="154"/>
+      <c r="AE26" s="154"/>
+      <c r="AF26" s="154"/>
+      <c r="AG26" s="154"/>
+    </row>
+    <row r="27" spans="2:40" x14ac:dyDescent="0.3">
       <c r="B27" s="178">
         <v>44785</v>
       </c>
@@ -10885,21 +11112,21 @@
         <v>63682</v>
       </c>
       <c r="E27" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1235842</v>
       </c>
-      <c r="O27" s="255">
+      <c r="S27" s="252">
         <v>44760</v>
       </c>
-      <c r="P27" s="256" t="s">
+      <c r="T27" s="253" t="s">
         <v>152</v>
       </c>
-      <c r="Q27" s="22">
+      <c r="U27" s="22">
         <v>97808.75</v>
       </c>
-      <c r="R27" s="269"/>
-    </row>
-    <row r="28" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V27" s="266"/>
+    </row>
+    <row r="28" spans="2:40" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="178">
         <v>44786</v>
       </c>
@@ -10910,603 +11137,468 @@
         <v>25200</v>
       </c>
       <c r="E28" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1261042</v>
       </c>
-      <c r="O28" s="255">
+      <c r="S28" s="252">
         <v>44761</v>
       </c>
-      <c r="P28" s="256" t="s">
+      <c r="T28" s="253" t="s">
         <v>153</v>
       </c>
-      <c r="Q28" s="22">
+      <c r="U28" s="22">
         <v>70509.3</v>
       </c>
-      <c r="R28" s="269"/>
-    </row>
-    <row r="29" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="178">
-        <v>44787</v>
-      </c>
-      <c r="C29" s="216">
-        <v>44793</v>
-      </c>
-      <c r="D29" s="217">
-        <v>71526</v>
-      </c>
-      <c r="E29" s="20">
-        <f t="shared" si="2"/>
-        <v>1332568</v>
-      </c>
-      <c r="O29" s="255">
+      <c r="V28" s="266"/>
+    </row>
+    <row r="29" spans="2:40" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="303"/>
+      <c r="C29" s="303"/>
+      <c r="D29" s="303"/>
+      <c r="E29" s="303"/>
+      <c r="S29" s="252">
         <v>44762</v>
       </c>
-      <c r="P29" s="256" t="s">
+      <c r="T29" s="253" t="s">
         <v>154</v>
       </c>
-      <c r="Q29" s="22">
+      <c r="U29" s="22">
         <v>72783.5</v>
       </c>
-      <c r="R29" s="269"/>
-    </row>
-    <row r="30" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="178">
-        <v>44787</v>
-      </c>
-      <c r="C30" s="216">
-        <v>44798</v>
-      </c>
-      <c r="D30" s="217">
-        <v>500</v>
-      </c>
-      <c r="E30" s="20">
-        <f t="shared" si="2"/>
-        <v>1333068</v>
-      </c>
-      <c r="N30" s="114" t="s">
+      <c r="V29" s="266"/>
+    </row>
+    <row r="30" spans="2:40" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="304"/>
+      <c r="C30" s="304"/>
+      <c r="D30" s="304"/>
+      <c r="E30" s="304"/>
+      <c r="R30" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="O30" s="255">
+      <c r="S30" s="252">
         <v>44763</v>
       </c>
-      <c r="P30" s="256" t="s">
+      <c r="T30" s="253" t="s">
         <v>155</v>
       </c>
-      <c r="Q30" s="22">
+      <c r="U30" s="22">
         <v>40894.36</v>
       </c>
-      <c r="R30" s="269"/>
-    </row>
-    <row r="31" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="178">
-        <v>44788</v>
-      </c>
-      <c r="C31" s="216">
-        <v>44793</v>
-      </c>
-      <c r="D31" s="217">
-        <v>50554</v>
-      </c>
-      <c r="E31" s="20">
-        <f t="shared" si="2"/>
-        <v>1383622</v>
-      </c>
-      <c r="O31" s="255">
+      <c r="V30" s="266"/>
+    </row>
+    <row r="31" spans="2:40" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="304"/>
+      <c r="C31" s="304"/>
+      <c r="D31" s="304"/>
+      <c r="E31" s="304"/>
+      <c r="S31" s="252">
         <v>44764</v>
       </c>
-      <c r="P31" s="256" t="s">
+      <c r="T31" s="253" t="s">
         <v>156</v>
       </c>
-      <c r="Q31" s="22">
+      <c r="U31" s="22">
         <v>69612.42</v>
       </c>
-      <c r="R31" s="269"/>
-    </row>
-    <row r="32" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="178">
-        <v>44789</v>
-      </c>
-      <c r="C32" s="216">
-        <v>44793</v>
-      </c>
-      <c r="D32" s="217">
-        <v>22615</v>
-      </c>
-      <c r="E32" s="20">
-        <f t="shared" si="2"/>
-        <v>1406237</v>
-      </c>
-      <c r="O32" s="255">
+      <c r="V31" s="266"/>
+    </row>
+    <row r="32" spans="2:40" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="304"/>
+      <c r="C32" s="304"/>
+      <c r="D32" s="304"/>
+      <c r="E32" s="304"/>
+      <c r="S32" s="252">
         <v>44765</v>
       </c>
-      <c r="P32" s="256" t="s">
+      <c r="T32" s="253" t="s">
         <v>157</v>
       </c>
-      <c r="Q32" s="22">
+      <c r="U32" s="22">
         <v>111046</v>
       </c>
-      <c r="R32" s="269"/>
-    </row>
-    <row r="33" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="178">
-        <v>44790</v>
-      </c>
-      <c r="C33" s="216">
-        <v>44793</v>
-      </c>
-      <c r="D33" s="254">
-        <v>21525</v>
-      </c>
-      <c r="E33" s="20">
-        <f t="shared" si="2"/>
-        <v>1427762</v>
-      </c>
-      <c r="O33" s="259">
+      <c r="V32" s="266"/>
+    </row>
+    <row r="33" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="304"/>
+      <c r="C33" s="304"/>
+      <c r="D33" s="304"/>
+      <c r="E33" s="304"/>
+      <c r="S33" s="256">
         <v>44765</v>
       </c>
-      <c r="P33" s="260" t="s">
+      <c r="T33" s="257" t="s">
         <v>158</v>
       </c>
-      <c r="Q33" s="144">
+      <c r="U33" s="144">
         <v>3984</v>
       </c>
-      <c r="R33" s="269"/>
-    </row>
-    <row r="34" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="178">
-        <v>44791</v>
-      </c>
-      <c r="C34" s="216">
-        <v>44793</v>
-      </c>
-      <c r="D34" s="254">
-        <v>46128.5</v>
-      </c>
-      <c r="E34" s="20">
-        <f t="shared" si="2"/>
-        <v>1473890.5</v>
-      </c>
-      <c r="Q34" s="261">
-        <v>0</v>
-      </c>
-      <c r="R34" s="269"/>
-    </row>
-    <row r="35" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="178">
-        <v>44792</v>
-      </c>
-      <c r="C35" s="215">
-        <v>44793</v>
-      </c>
-      <c r="D35" s="184">
-        <v>58983.5</v>
-      </c>
-      <c r="E35" s="20">
-        <f t="shared" si="2"/>
-        <v>1532874</v>
-      </c>
-      <c r="Q35" s="262">
-        <f>SUM(Q3:Q34)</f>
+      <c r="V33" s="266"/>
+    </row>
+    <row r="34" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="304"/>
+      <c r="C34" s="304"/>
+      <c r="D34" s="304"/>
+      <c r="E34" s="304"/>
+      <c r="U34" s="258">
+        <v>0</v>
+      </c>
+      <c r="V34" s="266"/>
+    </row>
+    <row r="35" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="304"/>
+      <c r="C35" s="304"/>
+      <c r="D35" s="304"/>
+      <c r="E35" s="304"/>
+      <c r="U35" s="259">
+        <f>SUM(U3:U34)</f>
         <v>1798927.8300000003</v>
       </c>
-      <c r="R35" s="269"/>
-    </row>
-    <row r="36" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="178">
-        <v>44793</v>
-      </c>
-      <c r="C36" s="215">
-        <v>44798</v>
-      </c>
-      <c r="D36" s="270">
-        <v>100977</v>
-      </c>
-      <c r="E36" s="20">
-        <f t="shared" si="2"/>
-        <v>1633851</v>
-      </c>
-    </row>
-    <row r="37" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="178">
-        <v>44794</v>
-      </c>
-      <c r="C37" s="215">
-        <v>44798</v>
-      </c>
-      <c r="D37" s="270">
-        <v>53500.5</v>
-      </c>
-      <c r="E37" s="20">
-        <f t="shared" si="2"/>
-        <v>1687351.5</v>
-      </c>
-    </row>
-    <row r="38" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="178">
-        <v>44795</v>
-      </c>
-      <c r="C38" s="215">
-        <v>44798</v>
-      </c>
-      <c r="D38" s="270">
-        <v>23209.5</v>
-      </c>
-      <c r="E38" s="20">
-        <f t="shared" si="2"/>
-        <v>1710561</v>
-      </c>
-    </row>
-    <row r="39" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="178">
-        <v>44704</v>
-      </c>
-      <c r="C39" s="215">
-        <v>44798</v>
-      </c>
-      <c r="D39" s="184">
-        <v>10000</v>
-      </c>
-      <c r="E39" s="20">
-        <f t="shared" si="2"/>
-        <v>1720561</v>
-      </c>
-    </row>
-    <row r="40" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="178">
-        <v>44797</v>
-      </c>
-      <c r="C40" s="215">
-        <v>44798</v>
-      </c>
-      <c r="D40" s="184">
-        <v>63665</v>
-      </c>
-      <c r="E40" s="20">
-        <f t="shared" si="2"/>
-        <v>1784226</v>
-      </c>
-    </row>
-    <row r="41" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="178">
-        <v>44798</v>
-      </c>
-      <c r="C41" s="215">
-        <v>44798</v>
-      </c>
-      <c r="D41" s="184">
-        <v>14701</v>
-      </c>
-      <c r="E41" s="20">
-        <f t="shared" si="2"/>
-        <v>1798927</v>
-      </c>
-    </row>
-    <row r="42" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="178"/>
-      <c r="C42" s="215"/>
-      <c r="D42" s="184"/>
-      <c r="E42" s="20">
-        <f t="shared" si="2"/>
-        <v>1798927</v>
-      </c>
-    </row>
-    <row r="43" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="178"/>
-      <c r="C43" s="177"/>
-      <c r="D43" s="182"/>
-      <c r="E43" s="20">
-        <f t="shared" si="2"/>
-        <v>1798927</v>
-      </c>
-    </row>
-    <row r="44" spans="2:18" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="186" t="s">
-        <v>103</v>
-      </c>
-      <c r="C44" s="175" t="s">
-        <v>96</v>
-      </c>
-      <c r="D44" s="174">
-        <v>-1798927.83</v>
-      </c>
-      <c r="E44" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.83000000007450581</v>
-      </c>
-    </row>
-    <row r="45" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="297" t="s">
-        <v>159</v>
-      </c>
-      <c r="C45" s="298"/>
-      <c r="D45" s="299"/>
-      <c r="E45" s="183">
-        <f t="shared" si="2"/>
-        <v>-0.83000000007450581</v>
-      </c>
-    </row>
-    <row r="46" spans="2:18" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="300"/>
-      <c r="C46" s="301"/>
-      <c r="D46" s="302"/>
-    </row>
-    <row r="47" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="18:29" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AB49" s="173"/>
-    </row>
-    <row r="50" spans="18:29" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AB50" s="173"/>
-    </row>
-    <row r="51" spans="18:29" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AB51" s="173"/>
-    </row>
-    <row r="52" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="AB52" s="173"/>
-    </row>
-    <row r="53" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R53" s="121"/>
-      <c r="S53" s="121"/>
-      <c r="T53" s="121"/>
-      <c r="U53" s="121"/>
+      <c r="V35" s="266"/>
+    </row>
+    <row r="36" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="304"/>
+      <c r="C36" s="304"/>
+      <c r="D36" s="304"/>
+      <c r="E36" s="304"/>
+    </row>
+    <row r="37" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="304"/>
+      <c r="C37" s="304"/>
+      <c r="D37" s="304"/>
+      <c r="E37" s="304"/>
+    </row>
+    <row r="38" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="304"/>
+      <c r="C38" s="304"/>
+      <c r="D38" s="304"/>
+      <c r="E38" s="304"/>
+    </row>
+    <row r="39" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="304"/>
+      <c r="C39" s="304"/>
+      <c r="D39" s="304"/>
+      <c r="E39" s="304"/>
+    </row>
+    <row r="40" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="304"/>
+      <c r="C40" s="304"/>
+      <c r="D40" s="304"/>
+      <c r="E40" s="304"/>
+    </row>
+    <row r="41" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="304"/>
+      <c r="C41" s="304"/>
+      <c r="D41" s="304"/>
+      <c r="E41" s="304"/>
+    </row>
+    <row r="42" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="304"/>
+      <c r="C42" s="304"/>
+      <c r="D42" s="304"/>
+      <c r="E42" s="304"/>
+    </row>
+    <row r="43" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="304"/>
+      <c r="C43" s="304"/>
+      <c r="D43" s="304"/>
+      <c r="E43" s="304"/>
+    </row>
+    <row r="44" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="304"/>
+      <c r="C44" s="304"/>
+      <c r="D44" s="304"/>
+      <c r="E44" s="304"/>
+    </row>
+    <row r="45" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="304"/>
+      <c r="C45" s="304"/>
+      <c r="D45" s="304"/>
+      <c r="E45" s="304"/>
+    </row>
+    <row r="46" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="304"/>
+      <c r="C46" s="304"/>
+      <c r="D46" s="304"/>
+      <c r="E46" s="304"/>
+    </row>
+    <row r="47" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="22:33" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AF49" s="173"/>
+    </row>
+    <row r="50" spans="22:33" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AF50" s="173"/>
+    </row>
+    <row r="51" spans="22:33" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AF51" s="173"/>
+    </row>
+    <row r="52" spans="22:33" x14ac:dyDescent="0.3">
+      <c r="AF52" s="173"/>
+    </row>
+    <row r="53" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V53" s="121"/>
       <c r="W53" s="121"/>
       <c r="X53" s="121"/>
       <c r="Y53" s="121"/>
-      <c r="AB53" s="173"/>
-    </row>
-    <row r="54" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R54" s="121"/>
-      <c r="S54" s="121"/>
-      <c r="T54" s="121"/>
-      <c r="U54" s="121"/>
+      <c r="Z53" s="121"/>
+      <c r="AA53" s="121"/>
+      <c r="AB53" s="121"/>
+      <c r="AC53" s="121"/>
+      <c r="AF53" s="173"/>
+    </row>
+    <row r="54" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V54" s="121"/>
       <c r="W54" s="121"/>
       <c r="X54" s="121"/>
       <c r="Y54" s="121"/>
-      <c r="Z54" s="101"/>
-      <c r="AA54" s="135"/>
-      <c r="AB54" s="173"/>
-      <c r="AC54" s="60"/>
-    </row>
-    <row r="55" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R55" s="121"/>
-      <c r="S55" s="121"/>
-      <c r="T55" s="121"/>
-      <c r="U55" s="121"/>
+      <c r="Z54" s="121"/>
+      <c r="AA54" s="121"/>
+      <c r="AB54" s="121"/>
+      <c r="AC54" s="121"/>
+      <c r="AD54" s="101"/>
+      <c r="AE54" s="135"/>
+      <c r="AF54" s="173"/>
+      <c r="AG54" s="60"/>
+    </row>
+    <row r="55" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V55" s="121"/>
       <c r="W55" s="121"/>
       <c r="X55" s="121"/>
       <c r="Y55" s="121"/>
-      <c r="Z55" s="101"/>
-      <c r="AA55" s="135"/>
-      <c r="AB55" s="173"/>
-      <c r="AC55" s="60"/>
-    </row>
-    <row r="56" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R56" s="121"/>
-      <c r="S56" s="121"/>
-      <c r="T56" s="121"/>
-      <c r="U56" s="121"/>
+      <c r="Z55" s="121"/>
+      <c r="AA55" s="121"/>
+      <c r="AB55" s="121"/>
+      <c r="AC55" s="121"/>
+      <c r="AD55" s="101"/>
+      <c r="AE55" s="135"/>
+      <c r="AF55" s="173"/>
+      <c r="AG55" s="60"/>
+    </row>
+    <row r="56" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V56" s="121"/>
       <c r="W56" s="121"/>
       <c r="X56" s="121"/>
       <c r="Y56" s="121"/>
-      <c r="Z56" s="101"/>
-      <c r="AA56" s="135"/>
-      <c r="AB56" s="173"/>
-      <c r="AC56" s="60"/>
-    </row>
-    <row r="57" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R57" s="121"/>
-      <c r="S57" s="121"/>
-      <c r="T57" s="121"/>
-      <c r="U57" s="121"/>
+      <c r="Z56" s="121"/>
+      <c r="AA56" s="121"/>
+      <c r="AB56" s="121"/>
+      <c r="AC56" s="121"/>
+      <c r="AD56" s="101"/>
+      <c r="AE56" s="135"/>
+      <c r="AF56" s="173"/>
+      <c r="AG56" s="60"/>
+    </row>
+    <row r="57" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V57" s="121"/>
       <c r="W57" s="121"/>
       <c r="X57" s="121"/>
       <c r="Y57" s="121"/>
-      <c r="Z57" s="101"/>
-      <c r="AA57" s="135"/>
-      <c r="AB57" s="173"/>
-      <c r="AC57" s="60"/>
-    </row>
-    <row r="58" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R58" s="121"/>
-      <c r="S58" s="121"/>
-      <c r="T58" s="121"/>
-      <c r="U58" s="121"/>
+      <c r="Z57" s="121"/>
+      <c r="AA57" s="121"/>
+      <c r="AB57" s="121"/>
+      <c r="AC57" s="121"/>
+      <c r="AD57" s="101"/>
+      <c r="AE57" s="135"/>
+      <c r="AF57" s="173"/>
+      <c r="AG57" s="60"/>
+    </row>
+    <row r="58" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V58" s="121"/>
       <c r="W58" s="121"/>
       <c r="X58" s="121"/>
       <c r="Y58" s="121"/>
-      <c r="Z58" s="101"/>
-      <c r="AA58" s="135"/>
-      <c r="AB58" s="173"/>
-      <c r="AC58" s="60"/>
-    </row>
-    <row r="59" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R59" s="121"/>
-      <c r="S59" s="121"/>
-      <c r="T59" s="121"/>
-      <c r="U59" s="121"/>
+      <c r="Z58" s="121"/>
+      <c r="AA58" s="121"/>
+      <c r="AB58" s="121"/>
+      <c r="AC58" s="121"/>
+      <c r="AD58" s="101"/>
+      <c r="AE58" s="135"/>
+      <c r="AF58" s="173"/>
+      <c r="AG58" s="60"/>
+    </row>
+    <row r="59" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V59" s="121"/>
       <c r="W59" s="121"/>
       <c r="X59" s="121"/>
       <c r="Y59" s="121"/>
-      <c r="Z59" s="101"/>
-      <c r="AA59" s="135"/>
-      <c r="AB59" s="173"/>
-      <c r="AC59" s="60"/>
-    </row>
-    <row r="60" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R60" s="121"/>
-      <c r="S60" s="121"/>
-      <c r="T60" s="121"/>
-      <c r="U60" s="121"/>
+      <c r="Z59" s="121"/>
+      <c r="AA59" s="121"/>
+      <c r="AB59" s="121"/>
+      <c r="AC59" s="121"/>
+      <c r="AD59" s="101"/>
+      <c r="AE59" s="135"/>
+      <c r="AF59" s="173"/>
+      <c r="AG59" s="60"/>
+    </row>
+    <row r="60" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V60" s="121"/>
       <c r="W60" s="121"/>
       <c r="X60" s="121"/>
       <c r="Y60" s="121"/>
-      <c r="Z60" s="101"/>
-      <c r="AA60" s="135"/>
-      <c r="AB60" s="173"/>
-      <c r="AC60" s="60"/>
-    </row>
-    <row r="61" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R61" s="121"/>
-      <c r="S61" s="121"/>
-      <c r="T61" s="121"/>
-      <c r="U61" s="121"/>
+      <c r="Z60" s="121"/>
+      <c r="AA60" s="121"/>
+      <c r="AB60" s="121"/>
+      <c r="AC60" s="121"/>
+      <c r="AD60" s="101"/>
+      <c r="AE60" s="135"/>
+      <c r="AF60" s="173"/>
+      <c r="AG60" s="60"/>
+    </row>
+    <row r="61" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V61" s="121"/>
       <c r="W61" s="121"/>
       <c r="X61" s="121"/>
       <c r="Y61" s="121"/>
-      <c r="Z61" s="101"/>
-      <c r="AA61" s="135"/>
-      <c r="AB61" s="173"/>
-      <c r="AC61" s="60"/>
-    </row>
-    <row r="62" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R62" s="121"/>
-      <c r="S62" s="121"/>
-      <c r="T62" s="121"/>
-      <c r="U62" s="121"/>
+      <c r="Z61" s="121"/>
+      <c r="AA61" s="121"/>
+      <c r="AB61" s="121"/>
+      <c r="AC61" s="121"/>
+      <c r="AD61" s="101"/>
+      <c r="AE61" s="135"/>
+      <c r="AF61" s="173"/>
+      <c r="AG61" s="60"/>
+    </row>
+    <row r="62" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V62" s="121"/>
       <c r="W62" s="121"/>
       <c r="X62" s="121"/>
       <c r="Y62" s="121"/>
-      <c r="Z62" s="101"/>
-      <c r="AA62" s="135"/>
-      <c r="AB62" s="173"/>
-      <c r="AC62" s="60"/>
-    </row>
-    <row r="63" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R63" s="121"/>
-      <c r="S63" s="121"/>
-      <c r="T63" s="121"/>
-      <c r="U63" s="121"/>
+      <c r="Z62" s="121"/>
+      <c r="AA62" s="121"/>
+      <c r="AB62" s="121"/>
+      <c r="AC62" s="121"/>
+      <c r="AD62" s="101"/>
+      <c r="AE62" s="135"/>
+      <c r="AF62" s="173"/>
+      <c r="AG62" s="60"/>
+    </row>
+    <row r="63" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V63" s="121"/>
       <c r="W63" s="121"/>
       <c r="X63" s="121"/>
       <c r="Y63" s="121"/>
-      <c r="Z63" s="101"/>
-      <c r="AA63" s="135"/>
-      <c r="AB63" s="173"/>
-      <c r="AC63" s="60"/>
-    </row>
-    <row r="64" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R64" s="121"/>
-      <c r="S64" s="121"/>
-      <c r="T64" s="121"/>
-      <c r="U64" s="121"/>
+      <c r="Z63" s="121"/>
+      <c r="AA63" s="121"/>
+      <c r="AB63" s="121"/>
+      <c r="AC63" s="121"/>
+      <c r="AD63" s="101"/>
+      <c r="AE63" s="135"/>
+      <c r="AF63" s="173"/>
+      <c r="AG63" s="60"/>
+    </row>
+    <row r="64" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V64" s="121"/>
       <c r="W64" s="121"/>
       <c r="X64" s="121"/>
       <c r="Y64" s="121"/>
-      <c r="Z64" s="101"/>
-      <c r="AA64" s="135"/>
-      <c r="AB64" s="173"/>
-      <c r="AC64" s="60"/>
-    </row>
-    <row r="65" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R65" s="121"/>
-      <c r="S65" s="121"/>
-      <c r="T65" s="121"/>
-      <c r="U65" s="121"/>
+      <c r="Z64" s="121"/>
+      <c r="AA64" s="121"/>
+      <c r="AB64" s="121"/>
+      <c r="AC64" s="121"/>
+      <c r="AD64" s="101"/>
+      <c r="AE64" s="135"/>
+      <c r="AF64" s="173"/>
+      <c r="AG64" s="60"/>
+    </row>
+    <row r="65" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V65" s="121"/>
       <c r="W65" s="121"/>
       <c r="X65" s="121"/>
       <c r="Y65" s="121"/>
-      <c r="Z65" s="101"/>
-      <c r="AA65" s="135"/>
-      <c r="AB65" s="173"/>
-      <c r="AC65" s="60"/>
-    </row>
-    <row r="66" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R66" s="121"/>
-      <c r="S66" s="121"/>
-      <c r="T66" s="121"/>
-      <c r="U66" s="121"/>
+      <c r="Z65" s="121"/>
+      <c r="AA65" s="121"/>
+      <c r="AB65" s="121"/>
+      <c r="AC65" s="121"/>
+      <c r="AD65" s="101"/>
+      <c r="AE65" s="135"/>
+      <c r="AF65" s="173"/>
+      <c r="AG65" s="60"/>
+    </row>
+    <row r="66" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V66" s="121"/>
       <c r="W66" s="121"/>
       <c r="X66" s="121"/>
       <c r="Y66" s="121"/>
-      <c r="Z66" s="101"/>
-      <c r="AA66" s="135"/>
-      <c r="AB66" s="173"/>
-      <c r="AC66" s="60"/>
-    </row>
-    <row r="67" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R67" s="121"/>
-      <c r="S67" s="121"/>
-      <c r="T67" s="121"/>
-      <c r="U67" s="121"/>
+      <c r="Z66" s="121"/>
+      <c r="AA66" s="121"/>
+      <c r="AB66" s="121"/>
+      <c r="AC66" s="121"/>
+      <c r="AD66" s="101"/>
+      <c r="AE66" s="135"/>
+      <c r="AF66" s="173"/>
+      <c r="AG66" s="60"/>
+    </row>
+    <row r="67" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V67" s="121"/>
       <c r="W67" s="121"/>
       <c r="X67" s="121"/>
       <c r="Y67" s="121"/>
-      <c r="Z67" s="101"/>
-      <c r="AA67" s="135"/>
-      <c r="AB67" s="173"/>
-      <c r="AC67" s="60"/>
-    </row>
-    <row r="68" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R68" s="121"/>
-      <c r="S68" s="121"/>
-      <c r="T68" s="121"/>
-      <c r="U68" s="121"/>
+      <c r="Z67" s="121"/>
+      <c r="AA67" s="121"/>
+      <c r="AB67" s="121"/>
+      <c r="AC67" s="121"/>
+      <c r="AD67" s="101"/>
+      <c r="AE67" s="135"/>
+      <c r="AF67" s="173"/>
+      <c r="AG67" s="60"/>
+    </row>
+    <row r="68" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V68" s="121"/>
       <c r="W68" s="121"/>
       <c r="X68" s="121"/>
       <c r="Y68" s="121"/>
-      <c r="Z68" s="101"/>
-      <c r="AA68" s="135"/>
-      <c r="AB68" s="173"/>
-      <c r="AC68" s="60"/>
-    </row>
-    <row r="69" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="R69" s="121"/>
-      <c r="S69" s="121"/>
-      <c r="T69" s="121"/>
-      <c r="U69" s="121"/>
+      <c r="Z68" s="121"/>
+      <c r="AA68" s="121"/>
+      <c r="AB68" s="121"/>
+      <c r="AC68" s="121"/>
+      <c r="AD68" s="101"/>
+      <c r="AE68" s="135"/>
+      <c r="AF68" s="173"/>
+      <c r="AG68" s="60"/>
+    </row>
+    <row r="69" spans="22:33" x14ac:dyDescent="0.3">
       <c r="V69" s="121"/>
       <c r="W69" s="121"/>
       <c r="X69" s="121"/>
       <c r="Y69" s="121"/>
-      <c r="Z69" s="101"/>
-      <c r="AA69" s="135"/>
-      <c r="AB69" s="173"/>
-      <c r="AC69" s="60"/>
-    </row>
-    <row r="70" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="AB70" s="173"/>
-      <c r="AC70" s="60"/>
-    </row>
-    <row r="71" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="AB71" s="173"/>
-      <c r="AC71" s="127"/>
-    </row>
-    <row r="72" spans="18:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AB72" s="173"/>
-      <c r="AC72" s="121"/>
-    </row>
-    <row r="73" spans="18:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AB73" s="284"/>
-      <c r="AC73" s="285"/>
-    </row>
-    <row r="78" spans="18:29" x14ac:dyDescent="0.3">
-      <c r="AB78" s="54"/>
+      <c r="Z69" s="121"/>
+      <c r="AA69" s="121"/>
+      <c r="AB69" s="121"/>
+      <c r="AC69" s="121"/>
+      <c r="AD69" s="101"/>
+      <c r="AE69" s="135"/>
+      <c r="AF69" s="173"/>
+      <c r="AG69" s="60"/>
+    </row>
+    <row r="70" spans="22:33" x14ac:dyDescent="0.3">
+      <c r="AF70" s="173"/>
+      <c r="AG70" s="60"/>
+    </row>
+    <row r="71" spans="22:33" x14ac:dyDescent="0.3">
+      <c r="AF71" s="173"/>
+      <c r="AG71" s="127"/>
+    </row>
+    <row r="72" spans="22:33" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AF72" s="173"/>
+      <c r="AG72" s="121"/>
+    </row>
+    <row r="73" spans="22:33" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AF73" s="280"/>
+      <c r="AG73" s="281"/>
+    </row>
+    <row r="78" spans="22:33" x14ac:dyDescent="0.3">
+      <c r="AF78" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="T19:U19"/>
-    <mergeCell ref="B45:D46"/>
-    <mergeCell ref="AB73:AC73"/>
-    <mergeCell ref="O2:Q2"/>
+  <mergeCells count="5">
+    <mergeCell ref="X19:Y19"/>
+    <mergeCell ref="AF73:AG73"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="G20:I21"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.15748031496062992" right="0.11811023622047245" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="95" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -11518,7 +11610,7 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -11536,25 +11628,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="279" t="s">
+      <c r="B1" s="275" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="280"/>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="281"/>
+      <c r="C1" s="276"/>
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="276"/>
+      <c r="G1" s="277"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="271" t="s">
+      <c r="B2" s="267" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="267"/>
+      <c r="E2" s="267"/>
+      <c r="F2" s="267"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -12473,12 +12565,12 @@
       <c r="B55" s="37"/>
       <c r="C55" s="38"/>
       <c r="D55" s="198"/>
-      <c r="E55" s="272">
+      <c r="E55" s="268">
         <f>E51-G51</f>
         <v>277681</v>
       </c>
-      <c r="F55" s="273"/>
-      <c r="G55" s="274"/>
+      <c r="F55" s="269"/>
+      <c r="G55" s="270"/>
       <c r="I55" s="2"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -12494,11 +12586,11 @@
       <c r="B57" s="37"/>
       <c r="C57" s="38"/>
       <c r="D57" s="198"/>
-      <c r="E57" s="275" t="s">
+      <c r="E57" s="271" t="s">
         <v>8</v>
       </c>
-      <c r="F57" s="275"/>
-      <c r="G57" s="275"/>
+      <c r="F57" s="271"/>
+      <c r="G57" s="271"/>
       <c r="I57" s="2"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -12703,25 +12795,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="276" t="s">
+      <c r="B1" s="272" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="277"/>
-      <c r="D1" s="277"/>
-      <c r="E1" s="277"/>
-      <c r="F1" s="277"/>
-      <c r="G1" s="278"/>
+      <c r="C1" s="273"/>
+      <c r="D1" s="273"/>
+      <c r="E1" s="273"/>
+      <c r="F1" s="273"/>
+      <c r="G1" s="274"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="271" t="s">
+      <c r="B2" s="267" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="267"/>
+      <c r="E2" s="267"/>
+      <c r="F2" s="267"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -14451,12 +14543,12 @@
       <c r="B76" s="37"/>
       <c r="C76" s="38"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="272">
+      <c r="E76" s="268">
         <f>E72-G72</f>
         <v>0</v>
       </c>
-      <c r="F76" s="273"/>
-      <c r="G76" s="274"/>
+      <c r="F76" s="269"/>
+      <c r="G76" s="270"/>
       <c r="I76" s="2"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -14472,11 +14564,11 @@
       <c r="B78" s="37"/>
       <c r="C78" s="38"/>
       <c r="D78" s="2"/>
-      <c r="E78" s="275" t="s">
+      <c r="E78" s="271" t="s">
         <v>8</v>
       </c>
-      <c r="F78" s="275"/>
-      <c r="G78" s="275"/>
+      <c r="F78" s="271"/>
+      <c r="G78" s="271"/>
       <c r="I78" s="2"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -14617,25 +14709,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="276" t="s">
+      <c r="B1" s="272" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="277"/>
-      <c r="D1" s="277"/>
-      <c r="E1" s="277"/>
-      <c r="F1" s="277"/>
-      <c r="G1" s="278"/>
+      <c r="C1" s="273"/>
+      <c r="D1" s="273"/>
+      <c r="E1" s="273"/>
+      <c r="F1" s="273"/>
+      <c r="G1" s="274"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="271" t="s">
+      <c r="B2" s="267" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="267"/>
+      <c r="E2" s="267"/>
+      <c r="F2" s="267"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -15484,12 +15576,12 @@
       <c r="B41" s="37"/>
       <c r="C41" s="38"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="272">
+      <c r="E41" s="268">
         <f>E37-G37</f>
         <v>0</v>
       </c>
-      <c r="F41" s="273"/>
-      <c r="G41" s="274"/>
+      <c r="F41" s="269"/>
+      <c r="G41" s="270"/>
       <c r="I41" s="2"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -15505,11 +15597,11 @@
       <c r="B43" s="37"/>
       <c r="C43" s="38"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="275" t="s">
+      <c r="E43" s="271" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="275"/>
-      <c r="G43" s="275"/>
+      <c r="F43" s="271"/>
+      <c r="G43" s="271"/>
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -15653,25 +15745,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="279" t="s">
+      <c r="B1" s="275" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="280"/>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="281"/>
+      <c r="C1" s="276"/>
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="276"/>
+      <c r="G1" s="277"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="271" t="s">
+      <c r="B2" s="267" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="267"/>
+      <c r="E2" s="267"/>
+      <c r="F2" s="267"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -17011,12 +17103,12 @@
       <c r="B60" s="37"/>
       <c r="C60" s="38"/>
       <c r="D60" s="2"/>
-      <c r="E60" s="272">
+      <c r="E60" s="268">
         <f>E56-G56</f>
         <v>0</v>
       </c>
-      <c r="F60" s="273"/>
-      <c r="G60" s="274"/>
+      <c r="F60" s="269"/>
+      <c r="G60" s="270"/>
       <c r="I60" s="2"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -17032,11 +17124,11 @@
       <c r="B62" s="37"/>
       <c r="C62" s="38"/>
       <c r="D62" s="2"/>
-      <c r="E62" s="275" t="s">
+      <c r="E62" s="271" t="s">
         <v>8</v>
       </c>
-      <c r="F62" s="275"/>
-      <c r="G62" s="275"/>
+      <c r="F62" s="271"/>
+      <c r="G62" s="271"/>
       <c r="I62" s="2"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -17177,25 +17269,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="279" t="s">
+      <c r="B1" s="275" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="280"/>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="281"/>
+      <c r="C1" s="276"/>
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="276"/>
+      <c r="G1" s="277"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="271" t="s">
+      <c r="B2" s="267" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="267"/>
+      <c r="E2" s="267"/>
+      <c r="F2" s="267"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -18596,12 +18688,12 @@
       <c r="B61" s="37"/>
       <c r="C61" s="38"/>
       <c r="D61" s="2"/>
-      <c r="E61" s="272">
+      <c r="E61" s="268">
         <f>E57-G57</f>
         <v>0</v>
       </c>
-      <c r="F61" s="273"/>
-      <c r="G61" s="274"/>
+      <c r="F61" s="269"/>
+      <c r="G61" s="270"/>
       <c r="I61" s="2"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -18617,11 +18709,11 @@
       <c r="B63" s="37"/>
       <c r="C63" s="38"/>
       <c r="D63" s="2"/>
-      <c r="E63" s="275" t="s">
+      <c r="E63" s="271" t="s">
         <v>8</v>
       </c>
-      <c r="F63" s="275"/>
-      <c r="G63" s="275"/>
+      <c r="F63" s="271"/>
+      <c r="G63" s="271"/>
       <c r="I63" s="2"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -18762,25 +18854,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="279" t="s">
+      <c r="B1" s="275" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="280"/>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="281"/>
+      <c r="C1" s="276"/>
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="276"/>
+      <c r="G1" s="277"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="271" t="s">
+      <c r="B2" s="267" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="267"/>
+      <c r="E2" s="267"/>
+      <c r="F2" s="267"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -20230,12 +20322,12 @@
       <c r="B64" s="37"/>
       <c r="C64" s="38"/>
       <c r="D64" s="2"/>
-      <c r="E64" s="272">
+      <c r="E64" s="268">
         <f>E60-G60</f>
         <v>0</v>
       </c>
-      <c r="F64" s="273"/>
-      <c r="G64" s="274"/>
+      <c r="F64" s="269"/>
+      <c r="G64" s="270"/>
       <c r="I64" s="2"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -20251,11 +20343,11 @@
       <c r="B66" s="37"/>
       <c r="C66" s="38"/>
       <c r="D66" s="2"/>
-      <c r="E66" s="275" t="s">
+      <c r="E66" s="271" t="s">
         <v>8</v>
       </c>
-      <c r="F66" s="275"/>
-      <c r="G66" s="275"/>
+      <c r="F66" s="271"/>
+      <c r="G66" s="271"/>
       <c r="I66" s="2"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -20396,25 +20488,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="279" t="s">
+      <c r="B1" s="275" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="280"/>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="281"/>
+      <c r="C1" s="276"/>
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="276"/>
+      <c r="G1" s="277"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="271" t="s">
+      <c r="B2" s="267" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="267"/>
+      <c r="E2" s="267"/>
+      <c r="F2" s="267"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -21879,12 +21971,12 @@
       <c r="B65" s="37"/>
       <c r="C65" s="38"/>
       <c r="D65" s="198"/>
-      <c r="E65" s="272">
+      <c r="E65" s="268">
         <f>E61-G61</f>
         <v>0</v>
       </c>
-      <c r="F65" s="273"/>
-      <c r="G65" s="274"/>
+      <c r="F65" s="269"/>
+      <c r="G65" s="270"/>
       <c r="I65" s="2"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -21900,11 +21992,11 @@
       <c r="B67" s="37"/>
       <c r="C67" s="38"/>
       <c r="D67" s="198"/>
-      <c r="E67" s="275" t="s">
+      <c r="E67" s="271" t="s">
         <v>8</v>
       </c>
-      <c r="F67" s="275"/>
-      <c r="G67" s="275"/>
+      <c r="F67" s="271"/>
+      <c r="G67" s="271"/>
       <c r="I67" s="2"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -22086,25 +22178,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="279" t="s">
+      <c r="B1" s="275" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="280"/>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="281"/>
+      <c r="C1" s="276"/>
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="276"/>
+      <c r="G1" s="277"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="271" t="s">
+      <c r="B2" s="267" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="267"/>
+      <c r="E2" s="267"/>
+      <c r="F2" s="267"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -23055,12 +23147,12 @@
       <c r="B43" s="37"/>
       <c r="C43" s="38"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="272">
+      <c r="E43" s="268">
         <f>E39-G39</f>
         <v>0</v>
       </c>
-      <c r="F43" s="273"/>
-      <c r="G43" s="274"/>
+      <c r="F43" s="269"/>
+      <c r="G43" s="270"/>
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -23076,11 +23168,11 @@
       <c r="B45" s="37"/>
       <c r="C45" s="38"/>
       <c r="D45" s="2"/>
-      <c r="E45" s="275" t="s">
+      <c r="E45" s="271" t="s">
         <v>8</v>
       </c>
-      <c r="F45" s="275"/>
-      <c r="G45" s="275"/>
+      <c r="F45" s="271"/>
+      <c r="G45" s="271"/>
       <c r="I45" s="2"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -23268,18 +23360,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="218"/>
-      <c r="B1" s="219"/>
-      <c r="C1" s="219"/>
-      <c r="D1" s="219"/>
-      <c r="E1" s="219"/>
-      <c r="F1" s="219"/>
-      <c r="G1" s="219"/>
-      <c r="H1" s="219"/>
-      <c r="I1" s="219"/>
-      <c r="J1" s="219"/>
-      <c r="K1" s="219"/>
-      <c r="L1" s="219"/>
+      <c r="A1" s="216"/>
+      <c r="B1" s="217"/>
+      <c r="C1" s="217"/>
+      <c r="D1" s="217"/>
+      <c r="E1" s="217"/>
+      <c r="F1" s="217"/>
+      <c r="G1" s="217"/>
+      <c r="H1" s="217"/>
+      <c r="I1" s="217"/>
+      <c r="J1" s="217"/>
+      <c r="K1" s="217"/>
+      <c r="L1" s="217"/>
     </row>
     <row r="2" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="155" t="s">
@@ -23297,7 +23389,7 @@
       <c r="J2" s="154"/>
       <c r="K2" s="154"/>
       <c r="L2" s="154"/>
-      <c r="N2" s="220" t="s">
+      <c r="N2" s="218" t="s">
         <v>54</v>
       </c>
       <c r="O2" s="141" t="s">
@@ -23338,7 +23430,7 @@
       <c r="L3" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="N3" s="220" t="s">
+      <c r="N3" s="218" t="s">
         <v>54</v>
       </c>
       <c r="O3" s="141" t="s">
@@ -23384,7 +23476,7 @@
       <c r="M4" s="140" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="220" t="s">
+      <c r="N4" s="218" t="s">
         <v>57</v>
       </c>
       <c r="O4" s="141" t="s">
@@ -23427,7 +23519,7 @@
         <f>L4+K5</f>
         <v>142189</v>
       </c>
-      <c r="N5" s="220" t="s">
+      <c r="N5" s="218" t="s">
         <v>57</v>
       </c>
       <c r="O5" s="141" t="s">
@@ -23470,7 +23562,7 @@
         <f>L5+K6</f>
         <v>207018</v>
       </c>
-      <c r="N6" s="220" t="s">
+      <c r="N6" s="218" t="s">
         <v>60</v>
       </c>
       <c r="O6" s="141" t="s">
@@ -23513,7 +23605,7 @@
         <f t="shared" ref="L7:L18" si="1">L6+K7</f>
         <v>247093</v>
       </c>
-      <c r="N7" s="220" t="s">
+      <c r="N7" s="218" t="s">
         <v>62</v>
       </c>
       <c r="O7" s="141" t="s">
@@ -23556,7 +23648,7 @@
         <f t="shared" si="1"/>
         <v>303144</v>
       </c>
-      <c r="N8" s="220" t="s">
+      <c r="N8" s="218" t="s">
         <v>64</v>
       </c>
       <c r="O8" s="141" t="s">
@@ -23599,7 +23691,7 @@
         <f t="shared" si="1"/>
         <v>346594</v>
       </c>
-      <c r="N9" s="220" t="s">
+      <c r="N9" s="218" t="s">
         <v>64</v>
       </c>
       <c r="O9" s="141" t="s">
@@ -23642,7 +23734,7 @@
         <f t="shared" si="1"/>
         <v>398929</v>
       </c>
-      <c r="N10" s="220" t="s">
+      <c r="N10" s="218" t="s">
         <v>67</v>
       </c>
       <c r="O10" s="141" t="s">
@@ -23685,7 +23777,7 @@
         <f t="shared" si="1"/>
         <v>468120</v>
       </c>
-      <c r="N11" s="220" t="s">
+      <c r="N11" s="218" t="s">
         <v>69</v>
       </c>
       <c r="O11" s="141" t="s">
@@ -23728,7 +23820,7 @@
         <f t="shared" si="1"/>
         <v>518275</v>
       </c>
-      <c r="N12" s="220" t="s">
+      <c r="N12" s="218" t="s">
         <v>71</v>
       </c>
       <c r="O12" s="141" t="s">
@@ -23771,7 +23863,7 @@
         <f t="shared" si="1"/>
         <v>573502</v>
       </c>
-      <c r="N13" s="220" t="s">
+      <c r="N13" s="218" t="s">
         <v>71</v>
       </c>
       <c r="O13" s="141" t="s">
@@ -23814,7 +23906,7 @@
         <f t="shared" si="1"/>
         <v>620604</v>
       </c>
-      <c r="N14" s="220" t="s">
+      <c r="N14" s="218" t="s">
         <v>71</v>
       </c>
       <c r="O14" s="141" t="s">
@@ -23857,7 +23949,7 @@
         <f t="shared" si="1"/>
         <v>713738</v>
       </c>
-      <c r="N15" s="220" t="s">
+      <c r="N15" s="218" t="s">
         <v>75</v>
       </c>
       <c r="O15" s="141" t="s">
@@ -23900,7 +23992,7 @@
         <f t="shared" si="1"/>
         <v>736046</v>
       </c>
-      <c r="N16" s="220" t="s">
+      <c r="N16" s="218" t="s">
         <v>75</v>
       </c>
       <c r="O16" s="141" t="s">
@@ -23943,7 +24035,7 @@
         <f t="shared" si="1"/>
         <v>759582</v>
       </c>
-      <c r="N17" s="220" t="s">
+      <c r="N17" s="218" t="s">
         <v>78</v>
       </c>
       <c r="O17" s="141" t="s">
@@ -23980,7 +24072,7 @@
         <f t="shared" si="1"/>
         <v>759582</v>
       </c>
-      <c r="N18" s="220" t="s">
+      <c r="N18" s="218" t="s">
         <v>80</v>
       </c>
       <c r="O18" s="141" t="s">
@@ -24014,7 +24106,7 @@
       <c r="J19" s="147"/>
       <c r="K19" s="148"/>
       <c r="L19" s="148"/>
-      <c r="N19" s="220" t="s">
+      <c r="N19" s="218" t="s">
         <v>80</v>
       </c>
       <c r="O19" s="141" t="s">
@@ -24054,7 +24146,7 @@
       <c r="J20" s="150"/>
       <c r="K20" s="151"/>
       <c r="L20" s="151"/>
-      <c r="N20" s="220" t="s">
+      <c r="N20" s="218" t="s">
         <v>83</v>
       </c>
       <c r="O20" s="141" t="s">
@@ -24086,7 +24178,7 @@
       <c r="J21" s="135"/>
       <c r="K21" s="60"/>
       <c r="L21" s="60"/>
-      <c r="N21" s="220" t="s">
+      <c r="N21" s="218" t="s">
         <v>83</v>
       </c>
       <c r="O21" s="141" t="s">
@@ -24118,7 +24210,7 @@
       <c r="J22" s="135"/>
       <c r="K22" s="60"/>
       <c r="L22" s="60"/>
-      <c r="N22" s="220" t="s">
+      <c r="N22" s="218" t="s">
         <v>83</v>
       </c>
       <c r="O22" s="141" t="s">
@@ -24214,10 +24306,10 @@
       <c r="K39" s="159">
         <v>12116.39</v>
       </c>
-      <c r="M39" s="219"/>
-      <c r="N39" s="219"/>
-      <c r="O39" s="219"/>
-      <c r="P39" s="219"/>
+      <c r="M39" s="217"/>
+      <c r="N39" s="217"/>
+      <c r="O39" s="217"/>
+      <c r="P39" s="217"/>
     </row>
     <row r="40" spans="1:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K40" s="160">
@@ -24779,11 +24871,11 @@
       <c r="L62" s="121"/>
     </row>
     <row r="63" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K63" s="221">
+      <c r="K63" s="219">
         <f>SUM(K39:K62)</f>
         <v>850487.21</v>
       </c>
-      <c r="L63" s="222"/>
+      <c r="L63" s="220"/>
     </row>
     <row r="68" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K68" s="54"/>

</xml_diff>

<commit_message>
cierre  6 sep 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #08  AGOSTO 2022/CREDITOS  4 CARNES   ZAVALETA   AGOSTO     2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #08  AGOSTO 2022/CREDITOS  4 CARNES   ZAVALETA   AGOSTO     2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="12" activeTab="13"/>
+    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="13" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="REMISIONES OCTUBRE  2021     " sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="161">
   <si>
     <t>REMISION</t>
   </si>
@@ -1471,7 +1471,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="305">
+  <cellXfs count="307">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2093,6 +2093,10 @@
     <xf numFmtId="0" fontId="25" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="18" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2626,13 +2630,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>647703</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>152402</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2679,13 +2683,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>561977</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>123829</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>161927</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -9672,8 +9676,8 @@
   </sheetPr>
   <dimension ref="B1:AN78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -11608,10 +11612,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11690,10 +11694,10 @@
       <c r="E4" s="15">
         <v>18423</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
+      <c r="F4" s="305"/>
+      <c r="G4" s="160"/>
       <c r="H4" s="18">
-        <f t="shared" ref="H4:H50" si="0">E4-G4</f>
+        <f t="shared" ref="H4:H26" si="0">E4-G4</f>
         <v>18423</v>
       </c>
       <c r="I4" s="2"/>
@@ -11737,8 +11741,8 @@
       <c r="E6" s="20">
         <v>44375</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="86"/>
       <c r="H6" s="18">
         <f t="shared" si="0"/>
         <v>44375</v>
@@ -11758,8 +11762,8 @@
       <c r="E7" s="20">
         <v>15089</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="86"/>
       <c r="H7" s="18">
         <f t="shared" si="0"/>
         <v>15089</v>
@@ -11779,8 +11783,8 @@
       <c r="E8" s="20">
         <v>12716</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="86"/>
       <c r="H8" s="75">
         <f t="shared" si="0"/>
         <v>12716</v>
@@ -11800,8 +11804,8 @@
       <c r="E9" s="67">
         <v>16538</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="86"/>
       <c r="H9" s="18">
         <f t="shared" si="0"/>
         <v>16538</v>
@@ -11821,8 +11825,8 @@
       <c r="E10" s="20">
         <v>30178</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="86"/>
       <c r="H10" s="18">
         <f t="shared" si="0"/>
         <v>30178</v>
@@ -11867,8 +11871,8 @@
       <c r="E12" s="20">
         <v>23263</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="86"/>
       <c r="H12" s="18">
         <f t="shared" si="0"/>
         <v>23263</v>
@@ -11888,8 +11892,8 @@
       <c r="E13" s="20">
         <v>39575</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="86"/>
       <c r="H13" s="18">
         <f t="shared" si="0"/>
         <v>39575</v>
@@ -11934,8 +11938,8 @@
       <c r="E15" s="20">
         <v>9608</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="86"/>
       <c r="H15" s="18">
         <f t="shared" si="0"/>
         <v>9608</v>
@@ -11966,7 +11970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>44791</v>
       </c>
@@ -11980,14 +11984,14 @@
       <c r="E17" s="20">
         <v>30528</v>
       </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="22"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="86"/>
       <c r="H17" s="18">
         <f t="shared" si="0"/>
         <v>30528</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>44793</v>
       </c>
@@ -12001,14 +12005,14 @@
       <c r="E18" s="20">
         <v>29415</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="86"/>
       <c r="H18" s="18">
         <f t="shared" si="0"/>
         <v>29415</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>44793</v>
       </c>
@@ -12022,14 +12026,14 @@
       <c r="E19" s="20">
         <v>5009</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="22"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="86"/>
       <c r="H19" s="18">
         <f t="shared" si="0"/>
         <v>5009</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>44797</v>
       </c>
@@ -12043,14 +12047,14 @@
       <c r="E20" s="20">
         <v>1364</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="86"/>
       <c r="H20" s="18">
         <f t="shared" si="0"/>
         <v>1364</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>44797</v>
       </c>
@@ -12058,20 +12062,20 @@
         <v>473</v>
       </c>
       <c r="C21" s="24"/>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="20">
-        <v>0</v>
-      </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
+      <c r="E21" s="306">
+        <v>0</v>
+      </c>
+      <c r="F21" s="85"/>
+      <c r="G21" s="86"/>
       <c r="H21" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>44797</v>
       </c>
@@ -12085,660 +12089,315 @@
       <c r="E22" s="20">
         <v>1600</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="86"/>
       <c r="H22" s="18">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>44800</v>
+      </c>
       <c r="B23" s="13">
         <v>475</v>
       </c>
       <c r="C23" s="24"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
+      <c r="D23" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="20">
+        <v>2920</v>
+      </c>
+      <c r="F23" s="85"/>
+      <c r="G23" s="86"/>
       <c r="H23" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
+        <v>2920</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>44800</v>
+      </c>
       <c r="B24" s="13">
         <v>476</v>
       </c>
       <c r="C24" s="24"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="22"/>
+      <c r="D24" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="20">
+        <v>51478</v>
+      </c>
+      <c r="F24" s="85"/>
+      <c r="G24" s="86"/>
       <c r="H24" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13">
-        <v>477</v>
-      </c>
+        <v>51478</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="23"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="24"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
+      <c r="D25" s="204"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="62"/>
       <c r="H25" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13">
-        <v>478</v>
-      </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
+    <row r="26" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="31"/>
+      <c r="B26" s="100"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="197"/>
+      <c r="E26" s="34">
+        <v>0</v>
+      </c>
+      <c r="F26" s="35"/>
+      <c r="G26" s="36"/>
       <c r="H26" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13">
-        <v>479</v>
-      </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="13">
-        <v>480</v>
-      </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="13">
-        <v>481</v>
-      </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13">
-        <v>482</v>
-      </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="75">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="13">
-        <v>483</v>
-      </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="13">
-        <v>484</v>
-      </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="13">
-        <v>485</v>
-      </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="13">
-        <v>486</v>
-      </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="125"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="13">
-        <v>487</v>
-      </c>
-      <c r="C35" s="24"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
-      <c r="B36" s="13">
-        <v>488</v>
-      </c>
-      <c r="C36" s="24"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="13">
-        <v>489</v>
-      </c>
-      <c r="C37" s="24"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
-      <c r="B38" s="13">
-        <v>490</v>
-      </c>
-      <c r="C38" s="24"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="13">
-        <v>491</v>
-      </c>
-      <c r="C39" s="24"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="13">
-        <v>492</v>
-      </c>
-      <c r="C40" s="24"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
-      <c r="B41" s="13">
-        <v>493</v>
-      </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
-      <c r="B42" s="13">
-        <v>494</v>
-      </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
-      <c r="B43" s="13">
-        <v>495</v>
-      </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
-      <c r="B44" s="13">
-        <v>496</v>
-      </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
-      <c r="B45" s="13">
-        <v>497</v>
-      </c>
-      <c r="C45" s="24"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="13">
-        <v>498</v>
-      </c>
-      <c r="C46" s="24"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
-      <c r="B47" s="13">
-        <v>499</v>
-      </c>
-      <c r="C47" s="24"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="13">
-        <v>500</v>
-      </c>
-      <c r="C48" s="24"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="204"/>
-      <c r="E49" s="60"/>
-      <c r="F49" s="61"/>
-      <c r="G49" s="62"/>
-      <c r="H49" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="31"/>
-      <c r="B50" s="100"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="197"/>
-      <c r="E50" s="34">
-        <v>0</v>
-      </c>
-      <c r="F50" s="35"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I50" s="2"/>
-    </row>
-    <row r="51" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="37"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="198"/>
-      <c r="E51" s="39">
-        <f>SUM(E4:E50)</f>
-        <v>283011</v>
-      </c>
-      <c r="F51" s="39"/>
-      <c r="G51" s="39">
-        <f>SUM(G4:G50)</f>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="37"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="198"/>
+      <c r="E27" s="39">
+        <f>SUM(E4:E26)</f>
+        <v>337409</v>
+      </c>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39">
+        <f>SUM(G4:G26)</f>
         <v>5330</v>
       </c>
-      <c r="H51" s="40">
-        <f>SUM(H4:H50)</f>
-        <v>277681</v>
-      </c>
-      <c r="I51" s="2"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="37"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="198"/>
-      <c r="E52" s="41"/>
-      <c r="F52" s="42"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="44"/>
-      <c r="I52" s="2"/>
-    </row>
-    <row r="53" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B53" s="37"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="198"/>
-      <c r="E53" s="45" t="s">
+      <c r="H27" s="40">
+        <f>SUM(H4:H26)</f>
+        <v>332079</v>
+      </c>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="37"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="198"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B29" s="37"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="198"/>
+      <c r="E29" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F53" s="42"/>
-      <c r="G53" s="46" t="s">
+      <c r="F29" s="42"/>
+      <c r="G29" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="H53" s="44"/>
-      <c r="I53" s="2"/>
-    </row>
-    <row r="54" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="37"/>
-      <c r="C54" s="38"/>
-      <c r="D54" s="198"/>
-      <c r="E54" s="45"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="46"/>
-      <c r="H54" s="44"/>
-      <c r="I54" s="2"/>
-    </row>
-    <row r="55" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="37"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="198"/>
-      <c r="E55" s="270">
-        <f>E51-G51</f>
-        <v>277681</v>
-      </c>
-      <c r="F55" s="271"/>
-      <c r="G55" s="272"/>
-      <c r="I55" s="2"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="37"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="198"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="42"/>
-      <c r="G56" s="43"/>
-      <c r="I56" s="2"/>
-    </row>
-    <row r="57" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B57" s="37"/>
-      <c r="C57" s="38"/>
-      <c r="D57" s="198"/>
-      <c r="E57" s="273" t="s">
+      <c r="H29" s="44"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="37"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="198"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="37"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="198"/>
+      <c r="E31" s="270">
+        <f>E27-G27</f>
+        <v>332079</v>
+      </c>
+      <c r="F31" s="271"/>
+      <c r="G31" s="272"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="37"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="198"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="43"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B33" s="37"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="198"/>
+      <c r="E33" s="273" t="s">
         <v>8</v>
       </c>
-      <c r="F57" s="273"/>
-      <c r="G57" s="273"/>
-      <c r="I57" s="2"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="111"/>
-      <c r="B58" s="112"/>
-      <c r="C58" s="113"/>
-      <c r="D58" s="199"/>
-      <c r="E58" s="115"/>
-      <c r="F58" s="116"/>
-      <c r="G58" s="117"/>
-      <c r="I58" s="2"/>
-    </row>
-    <row r="59" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="101"/>
-      <c r="B59" s="102"/>
-      <c r="C59" s="103"/>
-      <c r="D59" s="200"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="51"/>
-      <c r="G59" s="50"/>
-      <c r="H59" s="104"/>
-      <c r="I59" s="2"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="118"/>
-      <c r="B60" s="119"/>
-      <c r="C60" s="120"/>
-      <c r="D60" s="201"/>
-      <c r="E60" s="122"/>
-      <c r="F60" s="123"/>
-      <c r="G60" s="124"/>
-      <c r="H60" s="104"/>
-      <c r="I60" s="2"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="118"/>
-      <c r="B61" s="119"/>
-      <c r="C61" s="120"/>
-      <c r="D61" s="201"/>
-      <c r="E61" s="122"/>
-      <c r="F61" s="123"/>
-      <c r="G61" s="124"/>
-      <c r="H61" s="104"/>
-      <c r="I61" s="2"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="118"/>
-      <c r="B62" s="119"/>
-      <c r="C62" s="120"/>
-      <c r="D62" s="201"/>
-      <c r="E62" s="122"/>
-      <c r="F62" s="123"/>
-      <c r="G62" s="124"/>
-      <c r="H62" s="104"/>
-      <c r="I62" s="2"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="118"/>
-      <c r="B63" s="119"/>
-      <c r="C63" s="120"/>
-      <c r="D63" s="201"/>
-      <c r="E63" s="122"/>
-      <c r="F63" s="123"/>
-      <c r="G63" s="124"/>
-      <c r="H63" s="104"/>
-      <c r="I63" s="2"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="118"/>
-      <c r="B64" s="119"/>
-      <c r="C64" s="120"/>
-      <c r="D64" s="201"/>
-      <c r="E64" s="122"/>
-      <c r="F64" s="123"/>
-      <c r="G64" s="124"/>
-      <c r="H64" s="104"/>
-      <c r="I64" s="2"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="118"/>
-      <c r="B65" s="119"/>
-      <c r="C65" s="120"/>
-      <c r="D65" s="201"/>
-      <c r="E65" s="122"/>
-      <c r="F65" s="123"/>
-      <c r="G65" s="124"/>
-      <c r="H65" s="104"/>
-      <c r="I65" s="2"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="118"/>
-      <c r="B66" s="119"/>
-      <c r="C66" s="120"/>
-      <c r="D66" s="201"/>
-      <c r="E66" s="122"/>
-      <c r="F66" s="123"/>
-      <c r="G66" s="124"/>
-      <c r="H66" s="104"/>
-      <c r="I66" s="2"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="118"/>
-      <c r="B67" s="119"/>
-      <c r="C67" s="120"/>
-      <c r="D67" s="201"/>
-      <c r="E67" s="122"/>
-      <c r="F67" s="123"/>
-      <c r="G67" s="124"/>
-      <c r="H67" s="104"/>
-      <c r="I67" s="2"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="118"/>
-      <c r="B68" s="119"/>
-      <c r="C68" s="120"/>
-      <c r="D68" s="201"/>
-      <c r="E68" s="122"/>
-      <c r="F68" s="123"/>
-      <c r="G68" s="124"/>
-      <c r="H68" s="104"/>
-      <c r="I68" s="2"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="118"/>
-      <c r="B69" s="119"/>
-      <c r="C69" s="120"/>
-      <c r="D69" s="201"/>
-      <c r="E69" s="122"/>
-      <c r="F69" s="123"/>
-      <c r="G69" s="124"/>
-      <c r="H69" s="104"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="105"/>
-      <c r="B70" s="106"/>
-      <c r="C70" s="107"/>
-      <c r="D70" s="202"/>
-      <c r="E70" s="108"/>
-      <c r="F70" s="109"/>
-      <c r="G70" s="110"/>
-      <c r="H70" s="104"/>
+      <c r="F33" s="273"/>
+      <c r="G33" s="273"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="111"/>
+      <c r="B34" s="112"/>
+      <c r="C34" s="113"/>
+      <c r="D34" s="199"/>
+      <c r="E34" s="115"/>
+      <c r="F34" s="116"/>
+      <c r="G34" s="117"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="101"/>
+      <c r="B35" s="102"/>
+      <c r="C35" s="103"/>
+      <c r="D35" s="200"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="104"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="118"/>
+      <c r="B36" s="119"/>
+      <c r="C36" s="120"/>
+      <c r="D36" s="201"/>
+      <c r="E36" s="122"/>
+      <c r="F36" s="123"/>
+      <c r="G36" s="124"/>
+      <c r="H36" s="104"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="118"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="120"/>
+      <c r="D37" s="201"/>
+      <c r="E37" s="122"/>
+      <c r="F37" s="123"/>
+      <c r="G37" s="124"/>
+      <c r="H37" s="104"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="118"/>
+      <c r="B38" s="119"/>
+      <c r="C38" s="120"/>
+      <c r="D38" s="201"/>
+      <c r="E38" s="122"/>
+      <c r="F38" s="123"/>
+      <c r="G38" s="124"/>
+      <c r="H38" s="104"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="118"/>
+      <c r="B39" s="119"/>
+      <c r="C39" s="120"/>
+      <c r="D39" s="201"/>
+      <c r="E39" s="122"/>
+      <c r="F39" s="123"/>
+      <c r="G39" s="124"/>
+      <c r="H39" s="104"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="118"/>
+      <c r="B40" s="119"/>
+      <c r="C40" s="120"/>
+      <c r="D40" s="201"/>
+      <c r="E40" s="122"/>
+      <c r="F40" s="123"/>
+      <c r="G40" s="124"/>
+      <c r="H40" s="104"/>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="118"/>
+      <c r="B41" s="119"/>
+      <c r="C41" s="120"/>
+      <c r="D41" s="201"/>
+      <c r="E41" s="122"/>
+      <c r="F41" s="123"/>
+      <c r="G41" s="124"/>
+      <c r="H41" s="104"/>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="118"/>
+      <c r="B42" s="119"/>
+      <c r="C42" s="120"/>
+      <c r="D42" s="201"/>
+      <c r="E42" s="122"/>
+      <c r="F42" s="123"/>
+      <c r="G42" s="124"/>
+      <c r="H42" s="104"/>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="118"/>
+      <c r="B43" s="119"/>
+      <c r="C43" s="120"/>
+      <c r="D43" s="201"/>
+      <c r="E43" s="122"/>
+      <c r="F43" s="123"/>
+      <c r="G43" s="124"/>
+      <c r="H43" s="104"/>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="118"/>
+      <c r="B44" s="119"/>
+      <c r="C44" s="120"/>
+      <c r="D44" s="201"/>
+      <c r="E44" s="122"/>
+      <c r="F44" s="123"/>
+      <c r="G44" s="124"/>
+      <c r="H44" s="104"/>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="118"/>
+      <c r="B45" s="119"/>
+      <c r="C45" s="120"/>
+      <c r="D45" s="201"/>
+      <c r="E45" s="122"/>
+      <c r="F45" s="123"/>
+      <c r="G45" s="124"/>
+      <c r="H45" s="104"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="105"/>
+      <c r="B46" s="106"/>
+      <c r="C46" s="107"/>
+      <c r="D46" s="202"/>
+      <c r="E46" s="108"/>
+      <c r="F46" s="109"/>
+      <c r="G46" s="110"/>
+      <c r="H46" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E33:G33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>